<commit_message>
Expanded manifesto forewords coverage
</commit_message>
<xml_diff>
--- a/manifesto-forewords/manifestos.xlsx
+++ b/manifesto-forewords/manifestos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\SDS thesis\scraping-political-speeches\manifesto-forewords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B09B88-8D4B-417C-A7B4-B124CDE65A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB059A5-5338-4C46-9DB1-FD7D66CA7D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="3372" windowWidth="17280" windowHeight="8964" xr2:uid="{F6410A5E-2F41-44E7-A64E-C2EE33441A0E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6410A5E-2F41-44E7-A64E-C2EE33441A0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="223">
   <si>
     <t>party</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>foreword</t>
-  </si>
-  <si>
-    <t>Labour</t>
   </si>
   <si>
     <t>Harold Wilson</t>
@@ -92,9 +89,6 @@
 In this campaign document we set out Labour's alternative to mass unemployment. We explain how a Labour government will help to stop the nuclear arms race. We provide a radical programme of action for a full five-year parliament, to save British industry and rebuild the welfare state.</t>
   </si>
   <si>
-    <t>Conservatives</t>
-  </si>
-  <si>
     <t>Margaret Thatcher</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
   </si>
   <si>
     <t>Tony Blair</t>
-  </si>
-  <si>
-    <t>Liberal Democrats</t>
   </si>
   <si>
     <t>UKIP</t>
@@ -536,9 +527,6 @@
   </si>
   <si>
     <t>http://www.maniffesto.com/wp-content/uploads/2019/11/Contract-With-The-People-Brexit-Party-2019-.pdf</t>
-  </si>
-  <si>
-    <t>Brexit Party</t>
   </si>
   <si>
     <t>Eight years ago, I offered new leadership - fresh, idealistic, energetic, but untested. You voted for change and gave me the chance to serve. In our first term we banished the demons of ten per cent interest rates, mass unemployment, wages of £1.50 an hour, and outside toilets in our schools. We put Labour values into action. And we banished Labour demons too: we showed we could run the economy well, cut crime, and stand up for Britain abroad. We proved our competence.
@@ -922,12 +910,700 @@
 The old mainstream parties have made 'manifesto' a dirty word. Everybody knows that a manifesto is little more than a set of vague promises that its authors have no intention of keeping. By contrast, our Contract with the People is a targeted set of deliverable pledges. We are not seeking election as a government. We are seeking to deliver the Brexit that we were promised three and a half years ago.
 With a Clean-Break Brexit, we can start changing Britain for good from day one. There will be no extended transition period', no more years of wrangling with Brussels, no further entanglement with the EU's controlling political institutions. We will be free to start building our future immediately, to change politics and Britain for good. And that's a promise.</t>
   </si>
+  <si>
+    <t>David Steel</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1983/1983-liberal-manifesto.shtml Democrats (libdems.co.uk)</t>
+  </si>
+  <si>
+    <t>The General Election on June 9th 1983 will be seen as a watershed in British politics. It may be recalled as the fateful day when depression became hopelessness and the slide of the post-war years accelerated into the depths of decline. Alternatively it may be remembered as the turning point when the people of this country, at the eleventh hour, decided to turn their backs on dogma and bitterness and chose a new road of partnership and progress.
+It is to offer real hope of a fresh start for Britain that the Alliance between our two parties has been created. What we have done is unique in the history of British parliamentary democracy. Two parties, one with a proud history, and one born only two years ago out of a frustration with the old system of politics, have come together to offer an alternative government pledged to bring the country together again.
+The Conservative and Labour parties between them have made an industrial wasteland out of a country which was once the workshop of the world. Manufacturing output from Britain is back to the level of nearly 20 years ago. Unemployment is still rising and there are now generations of school-leavers who no longer even hope for work. Mrs Thatcher's government stands idly by. hoping that the blind forces of the marketplace will restore the jobs and factories that its indifference has destroyed. The Labour Party's response is massive further nationalisation, a centralised state socialist economy and rigid controls over enterprise. The choice which Tories and Socialists offer at this election is one between neglect and interference. Neither of them understands that it is only by working together in the companies and communities of Britain that we can overcome the economic problems which beset us.
+Meanwhile the very fabric of our common life together deteriorates. The record wave of violence and crime and increased personal stress are all signs of a society at war with itself. Rundown cities and declining rural services alike tell a story of a warped sense of priorities by successive governments. Our social services have become bureaucratic and remote from the people they are supposed to serve. Mrs Thatcher promised 'to bring harmony where there is discord'. Instead her own example of confrontation has inflamed the bitterness so many people feel at what has happened to their own lives and local communities.
+Our Alliance wants to call a halt to confrontation politics. We believe we have set an example by working together as two separate parties within an alliance of principle. Our whole approach is based on co-operation: not just between our parties but between management and workers, between people of different races and above all between government and people. Because we are not the prisoners of ideology we shall listen to the people we represent and ensure that the good sense of the voters is allowed to illuminate the corridors of Westminster and Whitehall. The TUC and CBI, each paying the bills for the party it supports, have been too much listened to and ordinary people have been heard too little.
+We do not believe that all wisdom resides in one party, or even in the two parties of the Alliance. There are men and women of sense and goodwill n both the other parties. But they have opted out and allowed the demands of the old party politics to make the House of Commons the most noisily partisan assembly in the Western World.
+Our concern is for the long-term, not just for tomorrow. We do not want to solve our immediate problems by piling up new crises for future generations. So when we plan for industrial recovery, we are not simply seeking growth for growth's sake. We want an increase in the sort of economic activity which will provide real jobs, which will rebuild our decaying infrastructure, which will conserve energy, and which will re-use and recycle materials rather than wasting them. We want to invest in education and housing since our long-term future depends upon the skill and maturity of the next generation. The lavish promises and the class- war rhetoric of the Conservative and Labour manifestos have no place in our Programme for Government. We offer instead a sober assessment of the first steps back to economic health and social well-being. But the vision which unites us is of a nation of free people working together in harmony, respecting each other's rights and freedom and sharing in each other's success. To achieve these hopes, we must not only change failed policies. We must reform the institutions which produced them.
+When we advocate a fairer voting system we are therefore talking neither about a constitutional abstraction nor the self-interest of a new political force. Of course we want fairness for ourselves, but even more do we demand a change in the interests of the majority, whose wishes are increasingly distorted by the pull of the extremes. This is in the interests of the cohesion of the country, for it is wrong and dangerous that one big party should be a stranger to the areas of prosperity and the other an incomprehending alien in the areas of deprivation. It is also in the interests of a more stable political and economic direction, without which those who work in industry, public or private, or in the community services, will not have the framework within which to plan for the future.
+We believe that Britain needs the fresh start of the Alliance even more in 1983 than it did in the heady days of our birth in 1981. The Labour Party has not become more moderate. The extremists have been taken out of the shop window; they have not been removed from the shop. The policies of nationalisation, attacks on private enterprise, withdrawal from Europe, with its devastating effect upon our exports and investment prospects, and alienation of our international friends and allies, are all enthroned and inviolate. Jobs and national safety would be at risk.
+Mrs Thatcher offers no alternative of hope or of long-term stability. Some of her objectives were good. Britain needed a shake-up: lower inflation, more competitive industry and a prospect of industrial growth to catch back the ground we had lost over the years. But the Government has not succeeded. After a bad start it has got lower inflation, but the prospects even for the end of this year are not good. And the price paid has been appalling. British industry has seen record bankruptcies and liquidations. Unemployment has increased on twice the scale of the world recession.
+Prospects for the future are more important than arguing about the failures of the past. The last four years could be forgiven if we now had a springboard for the future. We do not. At best we have a prospect of bumping along the bottom. On present policies the 80's will be a worse decade for unemployment than the 30's. Nearly a half of those without a job in 1933 got one by 1937. By 1987, if we continue as we are, unemployment will be at least as bad as in 1983. As a reaction, if the old two-party system is allowed to continue, we shall then lurch into the most extreme left-wing Government we have ever known.
+The Alliance can rescue us from this. There is no need for hopelessness. By giving a moderate and well-directed stimulus to the economy, accompanied by a firm and fair incomes policy, we can change the trend and begin to get people back to work. Unlike the Labour Party. we would do it in a way which encouraged private business. We believe in enterprise and profit, and in sharing the fruits of these.
+Beyond that, further success will depend upon the international climate. That is not wholly ours to command. But it does not intimidate us. The world is looking for a lead. Concerted expansion, greater currency stability, a recognition of interdependence between poorer and richer countries are all possible and necessary. We need the vision and sense of enlightened self-interest which produced the Marshall Plan and pulled post-war Europe together.
+It is an opportunity for Britain. We yearn for a world role and are qualified by our history and experience to perform one.
+The Alliance is unashamedly internationalist. We cannot live in a bunker. We are for a British lead in Europe, for multilateral disarmament and for a new drive to increase our own prosperity by co-operating with others to reduce poverty and squalor throughout the world. We offer reconciliation at home and constructive leadership abroad. We are not ashamed to set our sights high.</t>
+  </si>
+  <si>
+    <t>With your support this election could be about something more important than a change of government. It could be a chance to change a failed political system.
+Britain is deadlocked and that deadlock has meant economic and social decline. There can be very few voters, even among the keenest adherents of the Conservative or Labour cause, who really believe that our problems can all be solved just by yet another change of government. Oppositions promise grandiosely to generate 'the white hot heat of technological revolution' or to 'roll back the frontiers of the state'. It takes at least a year or two of government for them to come to terms with reality and discard their doctrinaire programmes. Each time the country is weakened further.
+We have tried confrontation politics for long enough. In 1964, in 1970, in 1974, incoming governments promised that they held the key to Britain's industrial and social problems, if only they could undo the achievements of their predecessors and push their own prescriptions through Parliament. The hopes they raised have all been cruelly disappointed. It is high time to try a different pattern of government, which is based upon the consent and support of the broad majority of the electorate. That alone can now provide the basis for the long term programme of reform which Britain so desperately needs.
+The Liberal Party has taken the first step towards breaking the deadlock during the past Parliament, by proving that co-operation among different parties is possible, practical and good for Britain. Unavoidably in this first experiment in a new style of government, our achievements were relatively limited. Many of the reforms which we wish to see implemented have had to wait.
+But during the 18 months of the Liberal Agreement with the Labour Government the stability and consistency provided by co-operation among parties which represented a clear majority of the electorate, and the requirement that the Labour Government respect the views of that majority, helped to bring down the annual rate of inflation to 8 per cent. The Tories had raised it from 5.9 per cent to 13.2 per cent. Labour raised it further to a peak of 26.9 per cent, now it is rising again. The Lib-Lab Agreement also reduced Interest Rates to 10 per cent (Minimum Lending Rate). The Tories left it at 12.5 per cent under Labour it reached a peak of 15 per cent in October 1976. It is now back up again.
+Industrial confidence began to return during the agreement. The divisive policies promoted by Labour's lunatic left-wing were effectively held in check. On Liberal insistence the law was changed to encourage profit-sharing, to help bridge the gulf of mistrust between the two sides of industry - which has so far led 48 companies to adopt new profit-sharing schemes.
+Sadly, much of what was achieved for Britain during those 18 months has been thrown away since last October, as Labour clung on to office without secure and agreed majority support. If either of the two establishment parties grabs an exclusive hold on office after this election, Britain will slip even deeper into industrial confrontation and economic decay. The truth is, the Labour and Conservatives parties share a vested interest in the preservation of Britain's divided society. The unrepresentative nature of our electoral system protects them from the full effects of public disillusionment. Continuing industrial and social confrontation reinforces their links with the opposing sides of industry. Britain's secretive and centralised structure of government protects them, turn and turn about, from Parliament and the public.
+Many, on both front benches, would rather see Britain's economy drift further behind our continental neighbours, would rather accept another cycle of industrial conflict and popular discontent, than touch the pattern of adversary politics which supports their alternating hold on political power.
+I appeal to you, as a voter concerned with what is best for Britain, to throw your support behind the fresh approach which the Liberal Party represents - and which we have now demonstrated can work for Britain. The effectiveness of whatever government emerges after this election, the whole style of British government, will depend less upon which big/dinosaur Party returns with the largest number of parliamentary seats than upon the size of the Liberal wedge in the House of Commons. A mass Liberal vote throughout the country and many more Liberal seats will call the final whistle on a discredited Tory/Labour game.
+Part Two of this manifesto sets out the Liberal Party's detailed electoral programme. I want here to stress four underlying themes: our commitment to fundamental political and constitutional reform; our proposals for economic and industrial reform; our plans to change and to simplify our overburdened tax system and our concern to bring to bear an environmental perspective across the whole range of government policies.
+Political reform is the starting point. Until we break the two-party stranglehold, until we get away from the adversary class politics which are embedded in our parliamentary structure, we cannot successfully tackle the problems of economic weakness and industrial mistrust, of misspent resources in housing, of uncertain management of the public sector and of mishandled relations with our neighbours abroad. Electoral reform is the key to the lock. A democratic electoral system would deprive the Conservative and Labour parties of their ability to maintain electoral support by frightening wavering voters with the spectre of a single, unacceptable alternative. It would force them to face up to their own internal contradictions: the unstable coalition within a weakened Labour Party between its nationalising left and its conservative centre; the tensions within the Conservative Party between moderate Tories and doctrinaire free-marketeers. A democratic electoral system is needed, too, to generate the popular consent which is essential to support a long-term programme of economic and social reform.
+The reluctant and unsatisfactory compromises which recent governments have offered in response to demands for the reform of Parliament, for an end to official secrecy, above all for devolution and decentralisation, also demonstrate the need for more thorough-going change and the inability of the establishment front benches to meet that need. Privately, many MPs from both the Labour and Conservative parties accept the case for far-reaching changes, but they are unwilling publicly to challenge their own leadership. A powerful wedge of Liberal MPs in the next Parliament could start a chain reaction of political change.
+Economic and industrial reform must accompany and follow from political reform. Hardly surprisingly, the owner party and the union party have resisted the extension of democracy to industry, seeing a transformation of the pattern of industrial relations as a threat to their entrenched interests. Labour's preferred approach would only strengthen the position of trade unions, which are already one of the most conservative forces in our society. They do not want to involve the workforce as a whole. The Conservative alternative of lightly-disguised confrontation is even more dangerous in 1979 than their Selsdon Park proposals were in 1970, and would no doubt lead again after a painful two years in office to another expensive U-turn.
+We Liberals seek instead to alter fundamentally the framework within which economic policy is made, to bring the different sides of industry together to work constructively to increase the well being of Britain - not to battle destructively over each other's share of a dwindling national cake.
+The two-party confrontation has also wrought havoc with our tax system. Successive governments have tacked on new additions to an already unwieldy structure. It is too complex for most taxpayers to understand or to be sure of their rights and obligations. Many changes have been rushed through Parliament without adequate debate or consideration of their implications, at the behest of some vested interest or in the service of some outdated ideology. As a result tax avoidance has become our fastest growing industry. Liberals are concerned to simplify the personal tax system and reduce its burden to create a tax structure which encourages initiative and promotes a wider distribution of wealth, and above all to establish principles for a stable tax system which can command the respect of the electorate as a whole: wealthy, poor and average earners.
+Neither of the two established parties has paid any serious attention to the long-term conservation of Britain's environment and resources. The argument over North Sea oil has been conducted in terms of immediate benefits rather than long term needs. The necessity to grow more of our own food and the conservation of man's natural habitat, including its flora and fauna, have been wrongly regarded as low priorities in politics. The debate over Britain's future dependence on nuclear power has hardly touched Parliament, conducted instead by environmental groups through the limited forum of the Windscale inquiry. Yet conservation and recycling of our limited and often finite resources is a vital issue for Britain's future, and an issue which concerns a growing section of our electorate. We Liberals have used our influence to force Parliament to pay more attention to the ecological perspective.
+But Parliament as at present constructed does not find it easy to focus on questions like this, which do not fall conveniently into the categories established by the conventions of two-Party politics or the Left/Right dog-fight. Here is a key issue for Britain as the new Parliament takes us into the 1980s, too complicated for the current ritual of debate but too important to ignore.
+It may seem paradoxical that Liberals call at once for more stable government and for radical change. Our concern is for long-term change, as opposed to the twists and turns of short-term policies which have characterised British government since the end of the Second World War. Worthwhile reforms for Britain's economy, for its industrial relations, its tax structure, its social services, its political system itself, can only be achieved after thorough examination and open debate - and can only be made to last if they command the respect and acceptance of the majority of the electorate.
+That is why we are prepared to co-operate with other parties, even as we insist on the need for a fundamental break in Britain's political habits. Of course we want in time to see Britain led by a Liberal Government, implementing a coherent radical programme with the support of a clear majority of voters. But meanwhile we are prepared to co-operate with whichever party will go with us some way along the same road. It would, after all, be a profound and radical change for Britain to benefit from stability in economic policy, to gain a new consensus in pay policy and industrial relations, to achieve a wider agreement on the structure of taxation, or to open up a searching debate on the best use of Britain's limited resources.
+It would be a radical change in itself for the next government to have to base its policies upon the support of the representatives of a genuine majority of the electorate. With your support, and the support of millions of voters like you, we can ensure that those changes take place.</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1979/1979-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1987/1987-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1992/1992-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>The Alliance's vision is of a Britain united, a Britain confident, compassionate and competitive. We know that it is possible to unite our country. We know the British people want greater unity. But we also know the task of drawing Britain together again can only be achieved through political, economic and social reform on a scale not contemplated in our country for over forty years.
+At the last election, about a third of the nation's voters didn't even both to turn out.
+It's hard to think of a more damning condemnation of politics in this country.
+But it's not difficult to understand why so many people feel cynical and uninterested.
+Since the last war the Tories and Labour have each had six turns at Government.
+Many honourable men and women on both sides have worked hard for the nation but the system has defeated all but a few.
+Rigid dogmas, the overriding need for party unity, and indiscriminate three-line whips have all helped to create a climate of conflict and rancour.
+Listen to Parliamentary question time and count how many times the Speaker has to call for order. We've had forty years of yah-boo politics and where has it got us?
+We live in a country that is patently unfair to many of its citizens. While politicians brandish statistics at each other on TV chat shows, we can all see with our own eyes what is happening to our schools, hospitals and inner cities.
+We know there is more crime because our own homes have been broken into, our own neighbours have been mugged, our own children have been offered drugs.
+We know that unemployment remains a huge problem because few families haven't been touched by its shadow.
+For many, the situation seems hopeless. Unable to contemplate five more years of uncaring government under Mrs Thatcher, they still do not trust the Labour Party.
+Mr Kinnock tries hard but for how long can he keep the lid on the extremists of the Left?
+They already dominate some of the Town Halls When the election is over, will they emerge again to claim the rewards of their silence?
+Many of these people feel that the Alliance is the answer - but they ask what chance does it have of changing things? The answer is - every chance.
+At the last election, the Alliance won nearly 8 million votes, little less than the Labour Party.
+If just 72 more people in every 700 vote for the Alliance this time, we will be the single largest party in Parliament. If just 5 more people in every 700 support us, we would have over 70 seats and almost certainly hold the balance of power.
+Think of it. Issues would be judged on their merits. We would curb the Tories' divisive policies and stop the destructive antics of the Labour Left.
+Politicians would be forced to listen to each other and work together. The two-party, two-class pantomime would finally be over.
+It's not an impossible dream. It's closer now than at any time in our history. All you have to do to make it happen is to vote Alliance on June 17th.</t>
+  </si>
+  <si>
+    <t>Be warned: this manifesto may not be what you expect.
+This manifesto does not promise good times just around the corner. It does not avoid difficult questions out of fear of unpopularity. It simply tells the truth; the truth about what Liberal Democrats believe has to be done in order for Britain to succeed.
+If you want Britain to stay the same then you probably won't like this manifesto. But if you want real change, if you long for a better future for yourself, your family, your community and your country, then read on.
+Britain has a clear choice at this election. We can stay much as we are, in the same old muddle, with difficult decisions postponed.
+Our failure to adjust to the modern world will then become every more serious. We will lag further behind in creating and sharing wealth. More and more people will lose their jobs and homes. Our environment will go on deteriorating. Our public services, already second rate, will become even worse.
+We shall fail to get the best out of the European Community, because our leaders will continue to be afraid to tell us that shared success in the Community means sharing sovereignty too.
+Our system of politics will continue to foster confrontation and short-term thinking, and exclude ordinary citizens from the business of government.
+This manifesto offers a different choice for Britain.
+Liberal Democrats do not believe that our country's under-performance has to be accepted. Another forty years of failed government is not inevitable. Britain has many advantages: a wealth of natural resources; a long history of engagement with the rest of the world; a mature and inventive people who value tolerance and freedom.
+But Britain will only succeed when its political leaders start treating voters as informed citizens with shared concerns, not as ignorant consumers to be manipulated. Now is the time for change.
+That is why in this manifesto we set out a clear analysis of Britain's problems and our proposals for putting them right. Above all, Liberal Democrats will trust our fellow citizens with the truth.
+So this manifesto is different from others you may read.
+We are not afraid to say what needs to be said.
+We are not afraid to do what needs to be done.
+And we are clear that if we want to make a modern Britain, we must first change Britain.</t>
+  </si>
+  <si>
+    <t>1970-06-18</t>
+  </si>
+  <si>
+    <t>1974-02-28</t>
+  </si>
+  <si>
+    <t>1974-10-10</t>
+  </si>
+  <si>
+    <t>1979-05-03</t>
+  </si>
+  <si>
+    <t>1983-06-09</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>BRX</t>
+  </si>
+  <si>
+    <t>LIB</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>1987-06-11</t>
+  </si>
+  <si>
+    <t>1992-04-09</t>
+  </si>
+  <si>
+    <t>1997-05-01</t>
+  </si>
+  <si>
+    <t>2001-06-07</t>
+  </si>
+  <si>
+    <t>2005-05-05</t>
+  </si>
+  <si>
+    <t>2010-05-06</t>
+  </si>
+  <si>
+    <t>2015-05-07</t>
+  </si>
+  <si>
+    <t>2017-06-08</t>
+  </si>
+  <si>
+    <t>2019-12-12</t>
+  </si>
+  <si>
+    <t>Jeremy Thorpe</t>
+  </si>
+  <si>
+    <t>There must surely be a better way to run a country than the one we have used for the last twenty-five years. No wonder people are fed up with thirteen years of Tory rule and twelve years under Labour.
+What have we achieved? What sort of society have we turned ourselves into materially and culturally?
+The purchasing power of the pound today is only worth about 7/- compared with its value in 1945.
+Wages keep going up but, owing to rising prices, many people are worse off.
+Over 600,000 people are out of work and no one seems to mind. Up to half a million people are without a proper home. In the so-called Welfare State many thousands of disabled people get no help.
+Parliament has become a slanging shop.
+The precious right of free speech is in peril from hooligan anarchists.
+Legitimate protests are regrettably too often the prelude to violence.
+Strikes, official and unofficial, by a few, paralyse whole sectors of industry and make it daily more difficult to pay our way in the world.
+The big labour unions use their power to take the biggest slice of the national wealth they can. The less powerful and the unorganised are left at the tail end of the pay claim queue. Inefficient monopolies pass on their price increases to the consumer.
+The Hospital service is grossly overstrained because junior doctors and nurses are so badly paid.
+We are only just waking up to the dangers of pollution and the damage we have done to the environment and the quality of life.
+Crime increases at a dangerous rate, too often violent, and the forces of law and order are set an impossible and unnecessary task.
+The election system bolsters up "bigness". The Big parties have totally unfair advantages against minorities. But the system is unfair even between the major parties.
+The whole "System" conspires against the individual, the unrepresented and the weak, in favour of the well-organised big battalions, and no one seems to care.
+But unless someone does care and does something about it the "System" will go on and on. It can only be broken by supporting something different and that something is the Liberal Party.
+It may be true that Liberals cannot expect under the present system to jump overnight from a party of thirteen M.P.s and three million supporters to become the government of the day, but we can break the power of the big battalions if we can get a substantial increase in the number of Liberal M.P.s in the next House of Commons and show that enough people care and want to protest at the present political farce.
+Politics is about power. It is about the sort of society we want to build and it must be a better one than we have now. Man has political power when he exercises a vote. A party has political power whether in government or opposition in so far as it influences and changes policy. Minority parties have political power when they influence policy or public opinion or successfully stand up against injustices or change the climate of politics.
+The Liberal Party is the Party of power for the ordinary people. It is the Party for people who care.
+The Liberal Party has political power but it needs more members in Parliament and a massive Liberal vote outside to strengthen and broaden that power and to use it to break the Tory/Labour stranglehold and create a really satisfying and worthwhile society to live in.
+It is an old adage that he who pays the piper calls the tune. Who pays the Tory piper? In 1968/69 £752,086 was contributed to Tory funds by some 470 companies Who pays the Labour piper? In March the TRADE UNIONS paid £350,000 to Labour's election fund. Big business tycoons and trade union bosses have a powerful say in British politics. We believe that millions of ordinary British people do not want our national politics to be dominated to the exclusion of all else by these two giant interests. Someone must speak for those whom big business and the big trade unions overlook. The Liberal election pledge is this: we will stand up to the big battalions on behalf of these people, where justice so demands. In what follows we show some of the ways in which we will do so.</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1970/1970-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>In this election, the paramount objectives of the Liberal Party, overriding all other considerations are to tell the people the truth about our country's situation and to secure a new approach to our problems in which sectional and partisan interests are set aside in favour of the general welfare of all.
+We are faced with an immediate economic and social crisis, the seriousness of which it is impossible for anyone to calculate with assurance and for which no-one can offer easy remedies.
+But the immediate crisis - desperate as it is - is only the culmination of a long process of deterioration in our ability, and the capacity of our political and social institutions, to manage our counntry's affairs efficiently and with tolerable sanity.
+Moreover, the present crisis is but a symptom of a deeper underlying disorder afflicting not only ourselves but the whole of the so-called western world. The era of western affluence side by side with poverty, and largely at the expense, of the other World is at an end.
+The situation is one which requires of all people - and all parties - a fundamental reappraisal of their attitutdes and policies. Without such a reappraisal it is questionable whether our own or any democratic system can or will survive. Here at home, and at this election, no one and no party has a ready made prescription for the cure of our troubles either in the short term or the long run, and anyone who pretends to have such a cure is a quack.
+But two basic requirements can be met. They might be called 'the essential conditions for democratic survival'.
+The first is to recreat in our society and in our political institutions a loyalty to the 'general good', to which all sectional and partisan interests, however inherently worthy, must be subordinate. But all efforts towards such a consensus, towards finding this area of common ground, will be idle and fruitless unless accompanied by a recognition (and this is the second condition for survival) that our present society is grossly unfair in its distribution of privileges and material rewards between capital and labour, between class and class and between one individual and another. Only when it is manifest that the restructuring of our society is in hand and that a fairer society is in sight will the necessary political consensus be attainable.
+People are now bewildered, frightened and often angry. The first business of any Government should be to draw the national together and to chart the course towards a new society based on fairness and tolerance.
+The role of the Liberal Party at this election is to act as a catalyst in bringing this about by securing the largest possible representation of the 'general interest'. And you, the elector, can help us in this task by rejecting the sterile class conflict of two discredited parties and voting in a new era of reconciliation. It will take courage, but the five Liberal by-election victories in the last fifteen months, during which period we have secured more votes than any other party, shows that it can be done.
+Every Liberal vote cast at this election will be a nail in the coffin of the two party system of confrontation and a step towards national unity and reconstruction.</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1974/feb/february-1974-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1974/oct/october-1974-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>This election will make or break Britain. It is already certain that the Government which takes office after the election will face the greatest peace-time crisis we have known since the dark days of 1931.
+The fact that we are committed to two elections in one year highlights the uncertainties and divisions of British politics. Mr. Heath called the first election back in February because his industrial and economic strategy had totally collapsed and he had no alternative. He lost, and relations between the Conservative Party and the Trade Union Movement will take many years to restore.
+Mr. Wilson has called the second election because he is not prepared to accept the disciplines of a minority Government. So long as a minority Government governs on behalf of the whole nation it can command a majority in Parliament. At the last election, the electorate clearly refused to give him a mandate for those divisive parts of his programme such as further nationalisation and clearly in calling for an election he has shown he is not prepared to accept that verdict.
+Liberals are unashamedly committed to breaking the two Party system in which the Party of Management alternates with the Party of Trade Unionism, each committed to the reversal of their predecessors' policies. Both interest groups represent vital elements in our society. Neither should ever be allowed to dominate the thinking of the government of the day. Instant reversal has brought uncertainty over Europe, over pensions, in the future of industry and has undermined confidence and stability.
+As the leader of a national political party it is my duty to warn the nation of the consequences if we fail to overcome this crisis. It is also my duty clearly and firmly to point the way out of our desperate situation.
+The first priority must be to promote a sense of common endeavour and national purpose in government. We must persuade all people to lay aside the differences which divide and weaken us as a nation and to unite in pursuit. of a solution to our difficulties. We must persuade ourselves that the survival of Britain is far more important than the advancement of any single individual or party and that we have far more in common as British citizens than the artificial divisions which society inflicts on us.
+But this unity will not be enough unless we can also isolate and deal with the fundamental defects - economic, political and social - which have led us to the brink of disaster. The next Government will have, without prejudice or precondition, to set itself to reconstruct Britain on a much fairer basis. It will have to attack poverty at source, redistribute wealth and income so that the rewards of endeavour correspond more closely to the value of the effort involved. It will have to remove the class divisions inherent in our society, particularly in our industrial relations and in the way we allocate national resources between rich and poor.
+I do not claim that it can be done overnight but I do say that unless a start is made-and very soon-the new endeavour, which is needed to rescue us, will not be forthcoming.
+Now is the time to decide whether we are to continue the steady decline in our national life, or whether we are going to pull ourselves back from the brink. Only with the necessary political will coupled with the concerted efforts of us all can we rescue ourselves. In asking for your commitment to the Liberal cause at this election. I am inviting you to join 6 million voters who support a party untainted by failure in government and unprejudiced by vested interests The Liberal Party can attract the support of all people drawn from every spectrum of our society who want to see a fair and tolerant society in Britain. With 6 million voters on which to build, and 600 candidates in the field, the opportunities open to us are unlimited.
+The sort of policies which we are putting forward are fair-they are realistic-they are tough. I claim that they represent a programme which can unite Britain and can achieve the success which as a nation we have so long been denied.
+Our greatest asset is that we could become the first post war Government which owed nothing to any sectional group or interest. In the February election, 2 million traditional Liberals were joined by 2 million previous Tory and 2 million previous Labour voters giving us a total of 6 million votes. It only needs to do this again, and we have united the centre in British politics.
+In short, l believe that Liberals can become the catalyst to bind the country together in a new spirit of common endeavour and I ask for your support in this great undertaking.</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>James Callaghan</t>
+  </si>
+  <si>
+    <t>1964</t>
+  </si>
+  <si>
+    <t>1959</t>
+  </si>
+  <si>
+    <t>Hugh Gaitskell</t>
+  </si>
+  <si>
+    <t>1955</t>
+  </si>
+  <si>
+    <t>1951</t>
+  </si>
+  <si>
+    <t>Clement Attlee</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>1945</t>
+  </si>
+  <si>
+    <t>Winston Churchill</t>
+  </si>
+  <si>
+    <t>Anthony Eden</t>
+  </si>
+  <si>
+    <t>Harold Macmillan</t>
+  </si>
+  <si>
+    <t>Alec Douglas-Home</t>
+  </si>
+  <si>
+    <t>Edward Heath</t>
+  </si>
+  <si>
+    <t>Archibald Sinclair</t>
+  </si>
+  <si>
+    <t>Clement Davies</t>
+  </si>
+  <si>
+    <t>Jo Grimond</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1945/1945-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1950/1950-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1951/1951-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1955/1955-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1959/1959-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1964/1964-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1966/1966-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>Victory is assured for us and our allies in the European war. The war in the East goes the same way. The British Labour Party is firmly resolved that Japanese barbarism shall be defeated just as decisively as Nazi aggression and tyranny. The people will have won both struggles. The gallant men and women in the Fighting Services, in the Merchant Navy, Home Guard and Civil Defence, in the factories and in the bombed areas - they deserve and must be assured a happier future than faced so many of them after the last war. Labour regards their welfare as a sacred trust.
+So far as Britain's contribution is concerned, this war will have been won by its people, not by any one man or set of men, though strong and greatly valued leadership has been given to the high resolve of the people in the present struggle. And in this leadership the Labour Ministers have taken their full share of burdens and responsibilities. The record of the Labour Ministers has been one of hard tasks well done since that fateful day in May, 1940, when the initiative of Labour in Parliament brought about the fall of the Chamberlain Government and the formation of the new War Government which has led the country to victory.
+The people made tremendous efforts to win the last war also. But when they had won it they lacked a lively interest in the social and economic problems of peace, and accepted the election promises of the leaders of the anti-Labour parties at their face value. So the "hard-faced men who had done well out of the war" were able to get the kind of peace that suited themselves. The people lost that peace. And when we say "peace" we mean not only the Treaty, but the social and economic policy which followed the fighting.
+In the years that followed, the "hard-faced men" and their political friends kept control of the Government. They controlled the banks, the mines, the big industries, largely the press and the cinema. They controlled the means by which the people got their living. They controlled the ways by which most of the people learned about the world outside. This happened in all the big industrialised countries.
+Great economic blizzards swept the world in those years. The great inter-war slumps were not acts of God or of blind forces. They were the sure and certain result of the concentration of too much economic power in the hands of too few men. These men had only learned how to act in the interest of their own bureaucratically-run private monopolies which may be likened to totalitarian oligarchies within our democratic State. They had and they felt no responsibility to the nation.
+Similar forces are at work today. The interests have not been able to make the same profits out of this war as they did out of the last. The determined propaganda of the Labour Party, helped by other progressive forces, had its effect in "taking the profit out of war". The 100% Excess Profits Tax, the controls over industry and transport, the fair rationing of food and control of prices - without which the Labour Party would not have remained in the Government - these all helped to win the war. With these measures the country has come nearer to making "fair shares" the national rule than ever before in its history.
+But the war in the East is not yet over. There are grand pickings still to be had. A short boom period after the war, when savings, gratuities and post-war credits are there to be spent, can make a profiteer's paradise. But Big Business knows that this will happen only if the people vote into power the party which promises to get rid of the controls and so let the profiteers and racketeers have that freedom for which they are pleading eloquently on every Tory platform and in every Tory newspaper.
+They accuse the Labour Party of wishing to impose controls for the sake of control. That is not true, and they know it. What is true is that the anti-controllers and anti-planners desire to sweep away public controls, simply in order to give the profiteering interests and the privileged rich an entirely free hand to plunder the rest of the nation as shamelessly as they did in the nineteen-twenties.
+Does freedom for the profiteer mean freedom for the ordinary man and woman, whether they be wage-earners or small business or professional men or housewives? Just think back over the depressions of the 20 years between the wars, when there were precious few public controls of any kind and the Big Interests had things all their own way. Never was so much injury done to so many by so few. Freedom is not an abstract thing. To be real it must be won, it must be worked for.
+The Labour Party stands for order as against the chaos which would follow the end of all public control. We stand for order, for positive constructive progress as against the chaos of economic do-as-they-please anarchy.
+The Labour Party makes no baseless promises. The future will not be easy. But this time the peace must be won. The Labour Party offers the nation a plan which will win the Peace for the People.</t>
+  </si>
+  <si>
+    <t>When the Labour Party published Let Us Face the Future in 1945 those five words were more than the title of the Election Manifesto; they were five words which crystallised the minds of our people at that time. By hard work, good sense and self-discipline the people have laid the foundations of a future based on free social democracy. They have helped Parliament and Government to carry into effect all the main proposals in that Manifesto.
+Now in 1950 the country is facing another General Election. We ask our fellow citizens to assert in their free exercise of the franchise that by and large the first majority Labour Government has served the country well. The task now is to carry the nation through to complete recovery. And that will mean continued, mighty efforts from us all. The choice for the electors is between the Labour Party - the party of positive action, of constructive progress, the true party of the nation - and the Conservative Party - the party of outdated ideas, of unemployment, of privilege.</t>
+  </si>
+  <si>
+    <t>Labour - proud of its record, sure in its policies - confidently asks the electors to renew its mandate.
+Four major tasks face our nation: to secure peace; to maintain full employment and increase production; to bring down the cost of living; to build a just society. Only with a Labour Government can the British people achieve these aims.</t>
+  </si>
+  <si>
+    <t>As we in Britain prepare to go to the poll, the Hydrogen Bomb looms over all mankind. What can we do to meet that menace? The existence of this terrible weapon on both sides of the Iron Curtain maintains an uneasy balance under the threat of mutual destruction. But deterrents can at best only give us a breathing space. We are faced with the choice between world co-operation and world annihilation. The time is short.
+The Labour Party approaches the problem in no party spirit. In April, 1954, we moved a motion in the House of Commons asking for immediate high-level talks. This was carried unanimously. Despite our pressure, those talks have not taken place. Labour believes that the first task of a British Government is to end this delay.</t>
+  </si>
+  <si>
+    <t>We welcome this Election; it gives us, at last, the chance to end eight years of Tory rule. In a television chat with President Eisenhower, Mr. Macmillan told us that the old division of Britain into the two nations, the Haves and the Have Nots, has disappeared. Tory prosperity, he suggested, is shared by all. In fact, the contrast between the extremes of wealth and poverty is sharper today than eight years ago. The business man with a tax-free expense account, the speculator with tax-free capital gains, and the retiring company director with a tax-free redundancy payment due to a take-over bid-these people have indeed 'never had it so good'.
+It is not so good for the widowed mother with children, the chronic sick, the 400,000 unemployed, and the millions of old age pensioners who have no adequate superannuation. While many of those at work have been able to maintain and even improve their standard of living by collective bargaining, the sick, the disabled and the old have continually seen the value of state benefits and small savings whittled away by rising prices. Instead of recognising this problem as the greatest social challenge of our time, the Prime Minister blandly denies it exists.</t>
+  </si>
+  <si>
+    <t>The world wants it and would welcome it. The British people want it, deserve it and urgently need it. And now, at last, the general election presents us with the exciting prospect of achieving it. The dying months of a frustrating 1964 can be transformed into the launching platform for the New Britain of the late 1960s and early 1970s.
+A New Britain - mobilising the resources of technology under a national plan; harnessing our national wealth in brains, our genius for scientific invention and medical discovery; reversing the decline of the thirteen wasted years; affording a new opportunity to equal, and if possible surpass, the roaring progress of other western powers while Tory Britain has moved sideways, backwards but seldom forward.
+The country needs fresh and virile leadership. Labour is ready. Poised to swing its plans into instant operation. Impatient to apply the "new thinking" that will end the chaos and sterility. Here is Labour's Manifesto for the 1964 election, restless with positive remedies for the problems the Tories have criminally neglected.
+Here is the case for planning, and the details of how a Labour Cabinet will formulate the national economic plan with both sides of industry operating in partnership with the Government. And here, in this manifesto, is the answer to the Tory gibe that planning could involve a loss of individual liberty. Labour has resolved to humanise the whole administration of the state and to set up the new office of Parliamentary Commissioner with the right and duty to investigate and expose any misuse of government power as it affects the citizen.
+Much of the manifesto deals with the vital social services that affect the personal lives and happiness of us all, the welfare of our families and the immediate future of our children. It announces, unequivocally, Labour's decisions on the nagging problems the Tories stupidly (in some cases callously) brushed aside:
+The imperative need for a revolution in our education system which will ensure the education of all our citizens in the responsibilities of this scientific age;
+The soaring prices in houses, flats and land;
+Social security benefits which have fallen below the minimum levels of human need;
+The burden of prescription charges in the Health Service.
+Labour is concerned, too, with the problems of leisure in the age of automation and here again Labour firmly puts the freedom of the individual first.
+"It is not the job of the Government to tell people how leisure should be used", the manifesto declares. But, in a society where facilities are not provided when they are not profitable and where the trend towards monopoly is growing, it is the job of the Government to ensure that leisure facilities are provided and that a reasonable range of choice is maintained.
+The pages that follow set out the manifesto in full. Please study it.</t>
+  </si>
+  <si>
+    <t>The time has come when the Government must ask the British people to renew and strengthen its mandate. Since we came to power in October, 1964, the nation has had firm government. But without an effective working majority it is difficult - and would become increasingly so - for the Government to continue to exercise influence in the outside world, and to exert its full authority in Whitehall, Westminster and the councils of industry.
+Since the collapse of the Macmillan Government three years ago, the authority of successive governments had been eroded by an atmosphere of fevered electoral uncertainty.
+The remedy lies in the hands of the electors. The time for decision has come.
+The course the Government recommends to the nation is clear. We are asking for a mandate to carry through the radical reconstruction of our national life which we began eighteen months ago. The road of renewal had been mapped in our election manifesto of 1964. Since we took office we have started on the long process of modernising obsolete procedures and institutions, ending the dominance of vested interests, liberating the forces of youth and building a New Britain.
+The task we have started, however, cannot be completed by Government acting alone. Its fulfilment will only be possible if the British people understand what the Government is doing, and give us their active support in finishing the job. It is for this active support, represented by a clear Parliamentary majority, that we now ask.</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1970/1970-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1979/1979-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>The British people took a historic decision in 1964 and 1966. It was not two decisions but one decision.
+On Thursday, 18 June, many more of the same people - together with millions who have never had a chance of voting before - can take this decision a big stage further. For it takes more than six years to modernise and humanise an advanced industrial country and move it on towards a new kind of greatness.</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1974/Oct/1974-oct-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>In February we put before the British people our Manifesto, 'Labour's Way out of the Crisis'.
+It was a programme for getting Britain back to work, for overcoming what was universally acknowledged to be the gravest economic crisis Britain had faced since the war. A programme to be carried out by a Government of all the people working together.
+Labour formed the Government, got Britain back to work and showed our determination to fulfil the programme which we had put before the people. No post war British Government has achieved more in six months.
+But at every turn we have found ourselves faced in Parliament by a majority which could, and did, coalesce to frustrate the policies we had put before the nation. What is still more serious has been the widespread expectation of an inevitable and early General Election, which created uncertainty in industry and the other institutions of our British society.
+Soon the people must decide on the Government to whom they want to entrust the future of themselves and their families for the next five years.
+They will judge each Party on its record in office, when it had the responsibility: on its record in honouring the pledges it had made to the country. On its willingness to undertake measures which would enlist the support and enthusiasm of our people in fighting the economic crisis.
+They will judge on the policies which each Party puts forward, asking themselves which Party can best be trusted to make a reality of those policies.
+They will judge not only on policies and records, but on the calibre and experience of the men and women who will be responsible for carrying out those policies. On their compassion and the understanding of the problems of ordinary families: on their determination to govern for, and with the sanction of, all of the people.
+In February the country rejected, as we had urged, policies of confrontation and conflict and 'fight to a finish' philosophies. We put before the country the policy of the Social Contract.
+We have shown that as a Government we are prepared to take the decisions that are needed to achieve economic and social justice without which this country can never unite.
+The policies we have followed over the past six months, the policies which the next Labour Government will follow, are policies to strengthen the Social Contract.
+It is not simply, or narrowly, an understanding about wages. It is about justice, equality, about concern for and protection of the lower paid, the needy, the pensioner and the handicapped in our society.
+It is about fairness between one man and another, and between men and women. It is about economic justice between individuals and between regions. It is about co-operation and conciliation, not conflict and confrontation.
+But more than that. What we as democratic socialists maintain is that when the going is toughest it is more than ever necessary to base our policies on social justice, to protect the weak, the poor, the disabled, to help those least able to help themselves, and to maintain and improve their living standards.
+Other Parties which do not believe in fair shares deny themselves the right to call for equal sacrifices.
+Injustice is the enemy of national unity.
+The crisis we are facing demands a still greater emphasis on social justice, as well as economic justice, than at any time in this generation.
+That is the inspiration underlying the policies set out in this Manifesto.
+It carries forward the programme we set out in February. It builds on our achievements in fulfilling, in six months, so much of that programme. It sets out in much more detail the policies we then announced, proposals which have now been firmly rooted in our experience in government, and responsibly costed against the resources which as a nation we can afford.
+This Manifesto, which is inspired by the idealism which has created our Movement, is now put before the country on the basis of the realism deriving from experience. It sets out what in our view is the only way to enable Britain to win through the crisis we now all face, and to share together, as one people, the fruits of the success we are determined to achieve.</t>
+  </si>
+  <si>
+    <t>Now, more than ever, we need Labour's traditional values of cooperation, social justice, and fairness. This manifesto restates these Labour principles in an action programme with a strong sense of the future. They appeal to all our people - young and old.
+The world is changing rapidly. New industrial nations are rising to challenge our key industries on which British jobs and living standards depend.
+The Labour Government is taking firm action to equip Britain to adapt to these changes and to seize new opportunities. And we will take great care to protect working people and their families from the hardships of change.
+But although the 1980s will present a tough challenge, this country will have many things in our favour. North Sea oil offers a golden prospect as do our reserves of natural gas and coal. We must use these resources wisely to plan our future to create new wealth, new jobs, and to look after the family, the elderly, and those in need.
+Too much is at stake to let the Conservatives frustrate the hopes of the coming decade by turning back the clock to the policies that they tried in the early seventies and that failed so badly before.
+The Government's industrial strategy is about how to create more wealth and more jobs through a constructive national partnership with unions and management. The Conservatives will not admit that nowadays governments must step in to help create employment, to limit prices rises, to assist industry to modernize itself. They are ready to gamble the people's future on a return to the nineteenth century free market' - despite its pitiless social consequences. They are as dangerously out of their time as a penny farthing on the motorway.
+Together the people and the Labour Government, even without a parliamentary majority, have achieved much these past five years, as the manifesto shows. In an uncertain world suffering the worst economic trouble for 40 years we have pointed the way forward.
+But nobody who cares about Britain can rest satisfied until far, far more has been accomplished. As long as there are men and women struggling with low pay, mothers stretching the household budget to make ends meet, youngsters in search of a job, children learning in out of date classrooms, patients queuing for a hospital bed or families without a decent home - then there is work for a Labour Government.
+Our purpose is to overcome the evils of inequality, poverty, racial bigotry, and make Britain truly one nation.
+For these we need a Labour majority in Parliament. This manifesto sets out our aims for the next five years. Here are five of our priorities.
+We must keep a curb on inflation and prices. Inflation is our enemy because rising prices hit most hardly at the pensioner, the low paid and the housewife, and inflation causes loss of jobs. Labour has brought inflation down from the alarming level caused by the Conservatives' failure to control the supply of money.
+Now we set ourselves the task of bringing inflation down to 5 per cent in three years. It is an ambitious target. We need the assistance of everyone. And everyone will be better off if we succeed.
+We will carry forward the task of putting into practice the new framework to improve industrial relations that we have hammered out with the TUC. The first step has been the creation of a new standing pay commission which will prevent the disruption of services to the public in future.
+Next, each year there will be three-way talks between ministers, management and unions to consider the best way forward for our country's economy. Germany's Social Democratic Government under Willy Brandt and Helmut Schmidt has proved that this is a good way to reach agreement on how to expand output, incomes and living standards.
+I am realistic enough to know that there are bound to be set backs. But experience reinforces what all of us know in our hearts - there is no sound alternative to working together.
+A Conservative free-for-all in pay and prices would mean endless pitched battles that would be fatal to the interests of all of us. The Labour way is the better way.
+We give a high priority to working for a return to full employment. A good job is a basic human right. During the last five years we have responded to the worldwide unemployment crisis by helping more than one million people to take up new jobs or new training.
+Now we will concentrate special attention on more jobs and training for the regions, the young and the long-term unemployed, and give them hope for the future.
+We are deeply concerned to enlarge people's freedom. Our policy will be to tilt the balance of power back to the individual and the neighbourhood, and away from the bureaucrats of town hall, company board room, the health service and Whitehall.
+Industrial democracy - giving working men and women a voice in the decisions which affect their jobs - is an idea whose time has come. Council tenants will have more freedom from bureaucratic control in their own homes. Parents and teachers will have a greater freedom to influence the running of their children's schools. Whitehall will devolve power, in an acceptable form to Scotland. Local services will be handed back to local authorities closer to the people. These are practical ways to set the people free.
+We will use Britain's influence to strengthen world peace and defeat world poverty. Europe has been at peace for over 30 years but ours is still a dangerous world with more armaments than ever before. Labour will keep Britain strong but we will also work hard for disarmament. It cannot be right that 15 million children in poorer countries die before they are five - yet the world spends so much on the means of destruction. There is a compelling moral need to raise the standard of life of all the world's citizens - no matter where they live.
+We are ready and willing to work with our European partners in closer unity. But we must record that in some aspects of its work the Common Market lacks common sense.
+Above all the agricultural policy is wasteful and expensive. In standing squarely against the discredited aspects of the dear-food policy, we are in fact defending the interests of European families just as much as British families. A nonsense is a nonsense in any language.
+The Labour Government will give a strong lead in the decade ahead. But no government can do it all. Our purpose is to deepen the sense of unity and kinship and community feeling that has always marked out our fellow countrymen and women. No nation can succeed by accepting benefits without responsibilities. I ask everybody who shares our ideals and our faith in Britain to join with us in securing the return of a government that dares to turn the dream of a caring society into practical action. And then work with us to complete the building of a Britain offering hope, social justice, and fairness to all.</t>
+  </si>
+  <si>
+    <t>I had hoped to preserve the Coalition Government, comprising all Parties in the State, until the end of the Japanese war, but owing to the unwillingness of the Socialist and Sinclair Liberal Parties to agree to my proposal, a General Election became inevitable, and I have formed a new National Government, consisting of the best men in all Parties who were willing to serve and some who are members of no Party at all.
+It is a strong Government, containing many of those who helped me to carry the burdens of State through the darkest days and on whose counsel and executive ability I have learned to rely.
+We seek the good of the whole nation, not that of one section or one faction. We believe in the living unity of the British people, which transcends class or party differences. It was this living unity which enabled us to stand like a rock against Germany when she over-ran Europe. Upon our power to retain unity, the future of this country and of the whole world largely depends.
+Britain is still at war, and must not turn aside from the vast further efforts still needed to bring Japan to the same end as Germany. Even when all foreign enemies are utterly defeated, that will not be the end of our task. It will be the beginning of our further opportunity - the opportunity which we snatched out of the jaws of disaster in 1940 - to save the world from tyranny and then to play our part in its wise, helpful guidance.
+Having poured out all we have to beat the Germans, holding nothing back, we must now take stock of our resources and plan how the energies of the British people can best be freed for the work that lies ahead.
+This is the time for freeing energies, not stifling them. Britain's greatness has been built on character and daring, not on docility to a State machine. At all costs we must preserve that spirit of independence and that "Right to live by no man's leave underneath the law".</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1945/1945-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1950/1950-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1951/1951-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1955/1955-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1959/1959-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1964/1964-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1966/1966-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>As Leader of the Conservative and Unionist Party I submit this manifesto of our beliefs and policy to the British electors.
+All who cherish the cause of our country at this fateful moment must cast their vote after hard and long thought, and make sure they cast it effectively.
+I commend to your attention with confidence this outline of our resolves and desires should we be called upon to assume the responsibilities of Government.</t>
+  </si>
+  <si>
+    <t>We are confronted with a critical Election which may well be the turning point in the fortunes and even the life of Britain. We cannot go on with this evenly balanced Party strife and hold our own in the world, or even earn our living. The prime need is for a stable government with several years before it, during which time national interests must be faithfully held far above party feuds or tactics. We need a new Government not biased by privilege or interest or cramped by doctrinal prejudices or inflamed by the passions of class warfare. Such a Government only the Conservative and Unionist Party can to-day provide.
+There must be no illusions about our difficulties and dangers. It is better to face them squarely as we did in 1940. The Conservative Party, who since victory have had no responsibility for the events which have led us to where we are now, offers no bribes to the electors. We will do our best to serve them and to make things better all round, but we do not blind ourselves to the difficulties that have to be overcome, or the time that will be required to bring us back to our rightful position in the world, and to revive the vigour of our national life and impulse.
+We all seek and pray for peace. A mighty union of nations tread that path together, but we all know that peace can only come through their united strength and faithful brotherhood.
+Contrast our position to-day with what it was six years ago. Then all our foes had yielded. We all had a right to believe and hope that the fear of war would not afflict our generation nor our children. We were respected, honoured and admired throughout the world. We were a united people at home, and it was only by being united that we had survived the deadly perils through which we had come and had kept the flag of freedom flying through the fateful year when we were alone. There, at any rate, is a great foundation and inspiration. Everyone knows how the aftermath of war brings extraordinary difficulties. With national unity we could have overcome them. But what has happened since those days?
+The attempt to impose a doctrinaire Socialism upon an Island which has grown great and famous by free enterprise has inflicted serious injury upon our strength and prosperity. Nationalisation has proved itself a failure which has resulted in heavy losses to the taxpayer or the consumer, or both. It has not given general satisfaction to the wage-earners in the nationalised industries. It has impaired the relations of the Trade Unions with their members. In more than one nationalised industry the wage-earners are ill-content with the change from the private employers, with whom they could negotiate on equal terms through the Trade Unions, to the all-powerful and remote officials in Whitehall.
+Our finances have been brought into grave disorder. No British Government in peace time has ever had the power or spent the money in the vast extent and reckless manner of our present rulers. Apart from the two thousand millions they have borrowed or obtained from the United States and the Dominions, they have spent more than 10 million pounds a day, or 22 thousand millions in their six years. No community living in a world of competing nations can possibly afford such frantic extravagances. Devaluation was the offspring of wild, profuse expenditure, and the evils which we suffer to-day are the inevitable progeny of that wanton way of living.
+A Conservative Government will cut out all unnecessary Government expenditure, simplify the administrative machine, and prune waste and extravagance in every department.
+The greatest national misfortune which we now endure is the ever falling value of our money, or, to put it in other words, the ever-increasing cost, measured in work and skill, of everything we buy. British taxation is higher than in any country outside the Communist world. It is higher by eight hundred millions a year than it was in the height of the war. We have a population of fifty millions depending on imports of food and raw materials which we have to win by our exertions, ingenuity, and craftsmanship. Since Devaluation it takes nearly twelve hours of work with hands or brains to buy across the dollar exchange what we could have got before for eight hours. We have now to give from one-quarter to one-third more of our life's strength, skill and output of every kind and quality to get the same intake as we did before Devaluation two years ago. We pay more for what we buy from abroad. we get less for what we sell. That is what Socialist Devaluation has meant. This costly expedient has not prevented a new financial crisis.
+We are a hard working people. We are second to none in ability or enterprise so far as we are allowed to use these gifts. We now have the only Socialist Government in the Empire and Commonwealth. Of all the countries in the world Britain is the one least capable of bearing the Socialist system.
+The Nation now has the chance of rebuilding its life at home and of strengthening its position abroad. We must free ourselves from our impediments. Of all impediments the class war is the worst. At the time when a growing measure of national unity is more than ever necessary, the Socialist Party hope to gain another lease of power by fomenting class hatred and appealing to moods of greed and envy.
+Within the limits of a statement of this kind, it is only possible to deal with some of the main questions now before us. We wish to be judged by deeds and their results and not by words and their applause. We seek to proclaim a theme, rather than write a prospectus. Many years ago I used the phrase, "Bring the rearguard in." This meant basic standards of life and labour, the duty of the strong to help the weak, and of the successful to establish tolerable conditions for the less fortunate. That policy is adopted by all Parties to-day. But now we have the new Socialist doctrine. It is no longer, "Bring the rearguard in," but "Keep the vanguard back." There is no means by which this Island can support its present population except by allowing its native genius to flourish and fructify. We cannot possibly keep ourselves alive without the individual effort, invention, contrivance, thrift and good housekeeping of our people.
+In 1945 I said:
+"What we desire is freedom; what we need is abundance. Freedom and abundance - these must be our aims. The production of new wealth is far more beneficial than class and Party fights about the liquidation of old wealth. We must try to share blessings and not miseries. The production of new wealth must precede common wealth, otherwise there will only be common poverty.
+It is because these simple truths have been denied and our people duped by idle hopes and false doctrine that the value of our money has fallen so grievously and the confidence of the world in Britain has been impaired. Confidence and currency are interdependent and restoring confidence by sound finance is one of the ways in which the value of our money may be sustained and the rising cost of living checked.
+The Conservative aim is to increase our national output. Here is the surest way to keep our people fully employed, to halt the rising cost of living, and to preserve our social services. Hard work, good management, thrift - all must receive their due incentive and reward.
+In the wider world outside this Island we put first the safety, progress and cohesion of the British Empire and Commonwealth of Nations. We must all stand together and help each other with all our strength both in Defence and Trade. To foster commerce within the Empire we shall maintain Imperial Preference. In our home market the Empire producer will have a place second only to the home producer.
+Next, there is the unity of the English-speaking peoples who together number hundreds of millions. They have only to act in harmony to preserve their own freedom and the general peace.
+On these solid foundations we should all continue to labour for a United Europe, including in the course of time those unhappy countries still behind the Iron Curtain.
+These are the three pillars of the United Nations Organisation which, if Soviet Russia becomes the fourth, would open to all the toiling millions of the world an era of moral and material advance undreamed of hitherto among men. There was a time in our hour of victory when this object seemed to be within our reach. Even now, in spite of the clouds and confusion into which we have since fallen, we must not abandon the supreme hope and design.
+For all these purposes we support the Rearmament programme on which the Socialist Government have embarked. We believe however that far better value could be got for the immense manpower and sums of money which are involved. Special sacrifices are required from us all for the sake of our survival as free democratic communities and the prevention of war.
+Our theme is that in normal times there should be the freest competition and that good wages and profits fairly earned under the law are a public gain both to the Nation and to all in industry-management and wage-earner alike. But the vast Rearmament policy of spending five thousand millions in three years on Defence inevitably distorts the ordinary working of supply and demand, therefore justice requires special arrangements for the emergency. We shall set our face against the fortuitous rise in company profits because of the abnormal process of Rearmament. We shall accordingly impose a form of Excess Profits Tax to operate only during this exceptional period.
+At the same time a revision of the existing system of taxation on commercial and industrial profits is required. Relief will be given in cases where profits are ploughed back and used for the renewal of plant and equipment.
+We believe in the necessity for reducing to the minimum possible all restrictive practices on both sides of industry, and we shall rely on a greatly strengthened Monopolies Commission to seek, and enable Parliament to correct, any operations in restraint of trade, including of course in the nationalised industries.
+I will now mention some other practical steps we shall take.
+We shall stop all further nationalisation.
+The Iron and Steel Act will be repealed and the Steel industry allowed to resume its achievements of the war and post-war years. To supervise prices and development we shall revive, if necessary with added powers, the former Iron and Steel Board representing the State, the management, labour, and consumers.
+Publicly-owned rail and road transport will be reorganised into regional groups of workable size. Private road hauliers will be given the chance to return to business, and private lorries will no longer be crippled by the twenty-five mile limit.
+Coal will remain nationalised. There will be more decentralisation snd stimulation of local initiative and loyalties, but wage negotiations will remain on a national basis.
+All industries remaining nationalised will come within the purview of the Monopolies' Commission and there will also be strict Parliamentary review of their activities.
+We seek to create an industrial system that is not only efficient but human. The Conservative Workers' Charter for Industry will be brought into being as early as possible, and extended to agriculture wherever practicable. The scheme will be worked out with trade unions and employers, and then laid before Parliament.
+There you have a clear plan of action in this field.
+Housing is the first of the social services. It is also one of the keys to increased productivity. Work, family life, health and education are all undermined by overcrowded homes. Therefore a Conservative and Unionist Government will give housing a priority second only to national defence. Our target remains 300,000 houses a year. There should be no reduction in the number of houses and flats built to let but more freedom must be given to the private builder. In a property-owning democracy, the more people who own their homes the better.
+In Education and in Health some of the most crying needs are not being met. For the money now being spent we will provide better services and so fulfil the high hopes we all held when we planned the improvements during the war.
+The whole system of town planning and development charges needs drastic overhaul.
+We shall review the position of pensioners, including war pensioners, and see that the hardest needs are met first. The care and comfort of the elderly is a sacred trust. Some of them prefer to remain at work and there must be encouragement for them to do so.
+To obtain more food practical knowledge and business experience must be released to comb the world for greater supplies.
+We shall maintain our system of guaranteed agricultural prices and markets and protect British horticulture from foreign dumpers. We have untilled acres and much marginal land. Farmers and merchants should work together to improve distribution in the interests of the public.
+Subject to the needs of Rearmament, the utmost will be done to provide better housing, water supplies, and drainage, electricity and transport in rural areas.
+The fishing industry will be protected from unrestricted foreign dumping. Every effort will be made by international agreement to prevent over-fishing.
+Food subsidies cannot be radically changed in present circumstances, but later we hope to simplify the system and by increases in family allowances, taxation changes and other methods, to ensure that public money is spent on those who need help and not, as at present, upon all classes indiscriminately.
+Apart from proposals to help Britain to stand on her own feet by increasing productivity, we must guard the British way of life, hallowed by centuries of tradition. We have fought tyrants at home and abroad to win and preserve the institutions of constitutional Monarchy and Parliamentary government. From Britain across the generations our message has gone forth to all parts of the globe. However well-meaning many of the present Socialist leaders may be, there is no doubt that in its complete development a Socialist State, monopolising production, distribution and exchange, would be fatal to individual freedom. We look on the Government as the servant and not as the masters of the people. Multiplying orders and rules should be reduced, and the whole system kept under more rigorous Parliamentary scrutiny. We shall call an all-Party conference to consider proposals for the reform of the House of Lords.
+We shall restore the University constituencies, which have been disfranchised contrary to the agreement reached by all three Parties during the war.
+The United Kingdom cannot he kept in a Whitehall straitjacket. The Unionist policy for Scotland, including the practical steps proposed for effective Scottish control of Scottish affairs, will he vigorously pressed forward.
+There will he a Cabinet Minister charged with the care of Welsh affairs,
+We shall seek to restore to Local Government the confidence and responsibility it has lost under Socialism.
+All these and other issues of the day can only he stated briefly in our Party Manifesto. A much fuller account will he given of them in Britain Strong and Free which will he published in a few days.
+I close with a simple declaration of our faith. The Conservative and Unionist Party stands not for any section of the people but for all. In this spirit, we will do our utmost to grapple with the increasing difficulties into which our country has been plunged.</t>
+  </si>
+  <si>
+    <t>I took the decision to recommend a dissolution of Parliament and the holding of a General Election after much thought, and for reasons which seem to me of supreme national importance.
+One of the greatest figures ever to be Prime Minister of Britain has put aside his burden. I have been called upon to take his place and to lead the Conservative and Unionist Party. It will be my purpose to give effect, in terms of the modem world, to the faith we hold and the principles we defend.
+In the year 1955 - in this age of peril and promise - what needs to be done can be carried through only with the trust and goodwill of the people of this country.
+This Parliament is already in its fourth year, and it is inevitable that, with a change of Prime Minister, there should be expectation of a General Election. I believe that it is better to face this issue now. Uncertainty at home and abroad as to the political future must he bad for our influence in world affairs and bad for our trade.
+Moreover, as is made clear in the pages which follow, we have far-reaching plans for the future of our country. They will take years rather than months to realise, and I need the support of the country to make them possible.
+As you know, much of my political life has been concerned with foreign affairs. Twice in a lifetime my generation has seen its world shaken, and almost destroyed, by a world war. Our civilisation could not hope to survive a third. It has been my work to do all I can to prevent such a catastrophe, and this will remain my firm resolve for the whole time I serve you.
+But to secure peace we have to do more than lust want it or just hope for it We must be firm and resolute. Weakness can lead only to war or to subjugation without a struggle. Because of this we and our allies have to be militarily strong. We have to accept the burden this entails. However costly, it is a price worth paying to avoid a war. We must make it certain that any would-be breaker of the peace knows beyond all doubt that aggression will be met, and that at once, by overwhelming retribution. If it is known that we have both the power and the will to deliver such retribution, we can hope that the danger of war will recede and that we can build a lasting peace.
+For this reason I have no doubt that we are right to make the hydrogen bomb and it is a source of strength to the country that the Opposition should support us in that step. Mr. Attlee, whose Government made the atomic bomb, has agreed that we must possess this newer and still more powerful deterrent In the face of its destructive power, any group of men would have to be not only bad, but mad, to unleash a war This fact may be the greatest force for peace.
+But our policy needs more than a deterrent. It must have a more positive side. We must seek to remove the distrust which today poisons the atmosphere between East and West.
+We have built the unity of the West, and our country has played a leading part in this. We are now ready for wider discussion. We will spare no effort to bring about meetings with the leaders of the Soviet Union and try to agree around the table proposals which will make a fresh advance towards disarmament and security for all peoples. I shall never despair of finding by agreement solutions which will rid the world of fear.
+At home we need a new authority if we are to develop the full sweep of our plans, which offer enormous opportunities.
+Within the lifetime of the Parliament which is about to be elected the first stage of our programme to produce electricity from nuclear power will be completed. What this means in material progress in Britain, how we plan to effect a steady and accelerating increase in the living standards of every section of our people, is set out in this document These projects will inevitably take time but they can soon begin to revolutionise our national life.
+During the last three and a half years the Conservative Government has achieved many of the aims proclaimed in 1951. We have seen solvency succeed the threat of national bankruptcy. We have seen both employment and earnings reach new high levels. We have seen new houses and new schools and new factories built and building, and soon we shall see new hospitals too. We have seen the social services extended and improved.
+Now the time has come for a new effort and fresh advances. To realise them we need a mandate measured not in months but in years. Here are some of the demands we shall have to meet
+We must fight with vigour the war on the slums and the war against ill-health and disease. We must equip our rising generation with an education to fit them for the requirements of this new age and to enable them to make the best use of their talents. We must produce more and produce it more efficiently. We must capture new markets overseas. We must save to invest in the future - at home and in the Commonwealth and Empire.
+To be successful we need a great national effort in which the fullest use is made of our finest asset - the character of our people. For that character to find its true expression we have to deepen our sense of national unity.
+How can this be achieved? One way would be to try to impose it from the top. The Conservative way is to encourage the growth of unity and fellowship in a free and neighbourly society in which the people of every calling work naturally together. I believe that this can be brought about if we develop in this country what I have many times described as a property-owning democracy.
+Such ownership can be expressed in the home, in savings or in forms of partnership in industry. It can take many shapes; but the essential theme is clear. We are against increased ownership of power and property by the State. We seek ever wider ownership of power and property by the people. We aim at a community of free men and women working together for the common good.</t>
+  </si>
+  <si>
+    <t>As Leader of the Conservative and Unionist Party I submit this Manifesto to the judgment of my fellow countrymen and women.
+This constructive programme-indeed its very title-will show you that we do not intend to rest in the next five years upon the achievements of the past. We must both de fend and develop the great gains that we have made. Our policy can be simply stated:
+Prosperity and Peace.
+I do not remember any period in my lifetime when the economy has been so sound and the prosperity of our people at home so widely spread; but we must also do what we can to extend a generous helping hand to the Commonwealth family and others overseas.
+As for peace, it is of course the supreme purpose of all policy. I have lived through two wars and all my efforts are directed to prevent a third. Events of the last few months give me hope that we may be moving into a more constructive period. Vital international negotiations lie ahead and I ask you to continue to entrust them to a Conservative Government.</t>
+  </si>
+  <si>
+    <t>As Leader of the Conservative and Unionist Party, I submit this Manifesto to my fellow countrymen and women.
+Its object is to declare the principles for which Conservatives stand and to show how we propose to translate them into action. Part of it is a record of achievement, and that is deliberate. For work well done carries conviction that our policies for the future will succeed. Our philosophy is to use what is good from the past to create a future which is better.
+But these pages are not an introduction to an easy, sheltered life. No country has an inherited right to wealth or influence. Prosperity has to be worked for. The future will be assured only if our people recognise the simple economic rules which must be kept by a country dependent on earning its living in a competitive world. This manifesto points the way.
+Throughout, you will find a constant theme. It is the creation of a social and economic climate in which men and women can develop their personalities and talents to their country's benefit as well as their own. Conservatives believe that a centralised system of direction cramps the style of the British people. Only by trusting the individual with freedom and responsibility shall we gain the vitality to keep our country great.
+Such greatness is not measured in terms of prosperity alone. What counts is the purpose to which we put prosperity. The Conservative purpose is clear from our record and from our programme. It is to raise the quality of our society and its influence for good in the world. We are using the growth of wealth to expand opportunities for the young, to provide more generously for the old and the sick and the handicapped, to aid developing countries still battling against widespread poverty, and to maintain the strength on which national security and our work for peace depend.
+In a world as dangerous as that in which we live it can make no sense whatever for Britain unilaterally to discard her strength. We therefore reject the idea of giving up our nuclear arm. We adopt instead a balanced policy of strength and conciliation: strength to be used to stop wars before they start; conciliation to reach areas of agreement with the Soviet Union and the Communist world which will replace tension and potential conflict. The Nuclear Test Ban Treaty was one such achievement. We mean to work for more until the danger of war is eliminated. The way will be rough but we will persevere. I ask you to conclude that we should retain British power and influence so that they may be used for such high purpose.
+In short, I trust that the values for which Conservatives stand and the policies which we intend to follow commend themselves to the imagination and the common sense of the British people.</t>
+  </si>
+  <si>
+    <t>I present to the people of Britain a manifesto which is also a blueprint It is a blueprint not for a year but for a full Parliament. I am deter mined to promise nothing that we cannot achieve. I know that we shall inherit from the Labour Government a weak economic position, and I intend to give first priority to the management of our economy, to the strengthening of Britain's competitive position in world markets and to the repayment of the heavy burden of debt which they have incurred.
+Equally I am determined to break away from the growing constraint of Socialism and the dreariness which stems from it: from the pattern of inflation and stagnant production which has been created.
+I want to see our social services recognise the overriding claims of those in most need. I want to see choice become once more part of the pattern of life of the individual. I want to see our country with confidence in itself and in the future taking its place in the European Economic Community.
+These are the things we must achieve. This manifesto points the way. I ask now for your confidence so that we can put it into effect I call not for words - but for action.</t>
+  </si>
+  <si>
+    <t>This Manifesto sets out the policies of the Conservative Party for a better Britain. It provides a programme for a Parliament How fast we can go will depend on how difficult a situation we find when we take office.
+But good government is not lust a matter of the right policies. It also depends on the way the government is run. This is something which I have thought about deeply. Indeed, it has been one of my main interests since I entered the House of Commons in 1950.
+During the last six years we have suffered not only from bad policies, but from a cheap and trivial style of government Decisions have been dictated simply by the desire to catch tomorrow's headlines. The short-term gain has counted for everything; the long-term objective has gone out of the window. Every device has been used to gain immediate publicity, and government by gimmick has become the order of the day. Decisions lightly entered into have been as lightly abandoned.
+It is not surprising that under this system several senior Labour Ministers have at different times left the Government in disgust at the way it is run. It is not surprising that when ever I have travelled abroad in recent years friends of Britain have told me of their sadness at the way in which our reputation has shrunk. It is not surprising that young people in this country looking at politics for the first time should be suspicious and cynical.
+I am determined therefore that a Conservative Government shall introduce a new style of government: that we shall re-establish our sound and honest British traditions in this field.
+I want to see a fresh approach to the taking of decisions. The Government should seek the best advice and listen carefully to it. It should not rush into decisions, it should use up-to-date techniques for assessing the situation, it should be deliberate and thorough. And in coming to its decisions it must always recognise that its responsibility is to the people, and all the people, of this country.
+What is more, its decision should be aimed at the long term. The easy answer and the quick trick may pay immediate dividends in terms of publicity, but in the end it is the national interest which suffers. We have seen that too often in the recent past.
+Finally, once a decision is made, once a policy is established, the Prime Minister and his colleagues should have the courage to stick to it Nothing has done Britain more harm in the world than the endless backing and filling which we have seen in recent years. Whether it be our defence commitments, or our financial policies, or the reform of industrial relations, the story has been the same. At the first sign of difficulty the Labour Government has sounded the retreat, covering its withdrawal with a smokescreen of unlikely excuses. But courage and intellectual honesty are essential qualities in politics, and in the interest of our country it is high time that we saw them again.
+So it will not be enough for a Conservative Government to make a fresh start with new policies. We must create a new way of running our national affairs. This means sweeping away the trivialities and the gimmicks which now dominate the political scene. It means dealing honestly and openly with the House of Commons, with the press and with the public.
+The decisions which a Government has to take affect the livelihood and perhaps the lives of millions of our fellow citizens. No-one has any business to take part in public life unless he is prepared to take such decisions with the seriousness which they deserve.
+This is my strongest personal conviction, and I shall not be content until it is the guiding principle of the government of this country.</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1970/1970-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1979/1979-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>Today we face great dangers both from within our own country and from outside. The problems are formidable, but there is no reason why they should overwhelm us.
+The assets of the British people are great. Not simply our technical skills and our natural resources, but also, more important than these, the strength and stability of our institutions and the determination of our people in moments of crisis to ensure that good sense and moderation prevail.
+If we are to make the best use of those assets it is essential that the affairs of this country are in the hands of a strong government, able to take firm measures in defence of the national interest.
+This means a Conservative Government with a renewed mandate from the people and with a full five years in which to guide the nation safely through the difficult period that lies ahead.
+That is why we need a General Election now.
+Once the General Election is behind us then we must put aside our differences and join in a common determination to establish and maintain a secure, civilised fair society.</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1974/Feb/february-1974-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>The dangers now facing Britain are greater than any we have seen since the last war. These dangers are both economic and political.
+Over recent months prices have been rising at an annual rate of over 20 per cent, and on present policies they will rise as much next year. This means that in two years the pound will be worth only 55p. Unemployment is rising rapidly, and the deficit in our balance of payments this year will be £4,000 million. By the end of the 1970s, on present forecasts, we are likely to owe £15,000 million for oil alone.
+At the same time the rule of law is threatened, and there are conflicts within the nation.
+If we do not solve our economic problems, our political difficulties will be made worse. And if we do not tackle our political problems, our economic problems will be insoluble.
+Our main aim therefore is to safeguard the existence of our free society.
+For inflation at its present pace threatens not only the standard of living of everybody in the country, but also the survival of our free and democratic institutions. No major democracy has ever survived such a catastrophic rise in the cost of living. We cannot be sure that we would be the exception.
+In any case inflation and rising prices tear society apart. They destroy the confidence of people in one another and the future; they distort the existing relationships within our country; they poison the social environment; they wipe out people's savings; they imperil our economic system; they lead in the end to high unemployment and to widespread, if not national, bankruptcy; and they bring particular hardship and misery to the most vulnerable people in the land.
+And that is not all. Another consequence of inflation is that financial manipulations often provide much greater scope for gain than solid hard work. This in itself breeds disillusionment and frustration. Lack of confidence in the currency leads to lessening respect for the law: hence sectional groups are starting to take the law into their own hands and to pursue their ends with a ruthless disregard for the interests of others.
+Finally, inflation weakens international confidence in sterling and intensifies the balance of payments crisis. In a few years time North Sea oil should give us an advantage over many of our competitors. But if we rely too much on borrowing from abroad to finance our payments deficit, our gains from North Sea oil will be mortgaged for many years ahead, and our hopes for prosperity based upon that oil will be dashed.
+Inflation is therefore a moral and political evil as well as a social and economic evil. Everything else is secondary to the battle against inflation and to helping those who have been wounded in it.
+There is no quick or simple way of defeating inflation. We do not claim to have any easy solution. Indeed no government can beat inflation by itself.
+The only way the battle can be won is by the Government and the people of this country uniting on a national policy. In the interest of national unity we will not re-introduce the Industrial Relations Act. Equally, no government should pursue a policy of wholesale nationalisation for party ends nor seek to further the interests of only a section or a class of the population. And certainly our economic condition is far too grave for our country to be subjected to a divisive and dogmatic attack upon the private enterprise sector of our economy.
+Inflation has dogged Britain since the war because as a country we have too often paid ourselves more than we earn. Lately this chronic inflation has been made acute by the explosion in the world price of food and raw materials.
+We need to bring back confidence in our currency; we need to stop paying ourselves more than we produce; and we need to produce more than we have produced in the past.
+To restore confidence in our currency we propose a comprehensive price stabilisation programme. This will use every tolerable means available to fight inflation. We will rigorously control public spending and the money supply and there must be restraint in prices and incomes.
+Because of the economic crisis there is no room for any early improvement in living standards. But our aim is to protect people's real income as far as it is possible to do so - by increasing pensions and other long4erm benefits every six months, by developing new forms of savings protected against inflation, and by pay arrangements which take account of rises in the cost of living.
+This is a far better way of protecting the interests of people at work than the excessive increases in some wage settlements over the last few months. These merely feed inflation and lead eventually to heavy unemployment. We believe that our attempt to protect the real value of wages, combined with the responsible self-interest of trade unions, should make a voluntary policy on pay and prices effective. But no government could honestly say that it will never be necessary to use the law in the national interest to support an effective policy for fighting inflation. In the absence of a viable prices and incomes policy any government would have to take harsher financial and economic measures than would otherwise be needed.
+Restraint and restriction are only palliatives. The best way of solving Britain's economic problems is by increasing our productivity and expanding British agriculture. It is only by producing more wealth that we can significantly help those who need help: the poor, the sick and the old. There is enormous scope for improving productivity, and our taxation and industrial policies will be directed towards this objective.
+Yet only part of our troubles are economic, and inflation is not the only threat to our free way of life. Modern industrial society is fragile. It is vulnerable to the terrorist and the anarchist. But at present an even greater danger is the short-sighted selfishness of some powerful groups. The great technological advances of this century have closely integrated our economy and the whole organisation of national life. This integration has brought immense material advantages, but by laying society open to disruption it has brought weakness as well. The whole is at the mercy of a part to an extent unimagined even a few years ago.
+Nevertheless no part of the nation can exist by itself. Disruption may bring temporary advantage to a few, but all are hurt in the end. The nation is diminished and impoverished by it.
+Trade unions are an important estate of the realm. We shall co-operate closely with them, and we hope that our proposals for industrial partnership will lead to close and effective co-operation both with employees and management. But we shall not be dominated by the trade unions. They are not the government of the country.
+We believe that the survival of a mixed economy is vital to national prosperity. If all economic power were in the hands of politicians and civil servants, if all economic and industrial decisions were taken in Whitehall, Britain would become a dictatorship. An all-powerful government is the end of freedom.
+A mixed economy ensures the diffusion of power. That is the only way we can prevent the abuse of power. Hence, the destruction of the mixed economy would entail the destruction of our democratic liberties, and the end of our parliamentary democracy.
+Obviously the struggle against inflation and the gravity of Britain's economic predicament prevent us from doing immediately all the things we should like to do. Like everyone else, governments must practise restraint.
+In the present economic emergency it would be irresponsible for any government to pretend that there can be general increases in public spending in real terms. This means having to postpone many of the things we would like to do straightaway. Only as we overcome our economic difficulties will it be possible to carry through the proposals in the second part of this Manifesto which involve expenditure. These proposals therefore are all subject to this important qualification.
+But we will act now in three areas which have been particularly hard hit by inflation and which in one way or another affect the basic livelihood of every family in the country - pensions, housing and food production. Our plans for these, which are set out later, will cost money; and in order to prevent inflationary consequences, it may be necessary to make cuts in public spending or increases in taxation. But as Britain's economic position improves, our general objective will be to reduce the burden of taxation.
+Our policies will lead to a united nation. We shall uphold the law and the authority of Parliament. It is in Parliament, not in the streets, that national policies must be worked out and disputes resolved.
+Our nation still possesses great moral reserves. Our patriotism, our knowledge that what unites us is far more significant than what divides us, our pride in our way of life and in our institutions, our sense of history, our idealism, our wish to make our country better and to improve the lot of our fellow citizens - all these feelings and beliefs remain strong in Britain. But they can only be properly summoned to the service of our nation by a government that commands the confidence of the country because it puts the country first.
+The Conservative Party, free from dogma and free from dependence upon any single interest, is broadly based throughout the nation. It is our objective to win a clear majority in the House of Commons in this election. But we will use that majority above all to unite the nation. We will not govern in a narrow partisan spirit. After the election we will consult and confer with the leaders of other parties and with the leaders of the great interests in the nation, in order to secure for the government's policies the consent and support of all men and women of good will. We will invite people from outside the ranks of our party to join with us in overcoming Britain's difficulties. The nation's crisis should transcend party differences.
+In any event, as a national Party we will pursue a national policy in the interests of the nation as a whole. We will lead a national effort. In normal times the party struggle is the safeguard of freedom. But the times are far from normal. In a crisis like this, it is the national interest which must prevail. We will ensure that it does.</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1974/Oct/october-1974-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>For me, the heart of politics is not political theory, it is people and how they want to live their lives.
+No one who has lived in this country during the last five years can fail to be aware of how the balance of our society has been increasingly tilted in favour of the State at the expense of individual freedom.
+This election may be the last chance we have to reverse that process, to restore the balance of power in favour of the people. It is therefore the most crucial election since the war.
+Together with the threat to freedom there has been a feeling of helplessness, that we are a once great nation that has somehow fallen behind and that it is too late now to turn things round.
+I don't accept that. 1 believe we not only can, we must. This manifesto points the way.
+It contains no magic formula or lavish promises. It is not a recipe for an easy or a perfect life. But it sets out a broad framework for the recovery of our country, based not on dogma, but On reason, on common sense, above all on the liberty of the people under the law.
+The things we have in common as a nation far outnumber those that set us apart.
+It is in that spirit that I commend to you this manifesto.</t>
+  </si>
+  <si>
+    <t>The Liberal Party, having for five years formed part of the All-Party Government, which has victoriously guided Britain through the dangers of the European war, now appeals with confidence to the new electorate.
+The Liberal Party has no responsibility for forcing an early election and, realising that the existing register is imperfect and will disfranchise many thousands of voters, was prepared to continue the Coalition until a new register was ready in October, and had expressed willingness to discuss its continuation until the end of the Japanese war.
+Nevertheless, now that the decision has been taken, we welcome the opportunity of submitting our programme to the Nation.</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1945/1945-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1950/1950-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1951/1951-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1955/1955-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1959/1959-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1964/1964-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdemmanifesto.com/1966/1966-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>"I will find a way or make one . . ." - Hannibal on crossing the Alps
+The Liberal Party offers the electorate the opportunity of returning a Liberal Government to office. We believe that our Party is more likely to unite the nation than either the Conservatives or the Socialists - locked as they are in what is really a class struggle.
+Britain has been brought close to bankruptcy by the effects of two wars, continued world disunity, and aid to friends abroad. The generous help we have received from our Commonwealth partners and the United States has helped us immeasurably, but will not long continue. We can only effect our recovery through our own efforts.</t>
+  </si>
+  <si>
+    <t>Great Britain is facing a new crisis - one of the biggest in her history. The people have not yet grasped how vast are the problems we have to solve very soon indeed.
+There is still no sure peace between nations. Hanging over the whole world is the fear that some governments are planning aggression. There is still war in Korea, and the dispute in Persia is an immediate danger. We have begun a gigantic programme of rearmament, which will affect the living standards of all of us. At the same time, the Dollar Gap has again opened and that, together with shortage of all foreign currencies, brings the ugly threat that we may not be able to buy the raw materials we must have to keep up the employment of our people. On top of all this is the fact which comes home to every housewife every day: the cost of living keeps going up.
+One thing is certain, no matter what the result of the Election. The country will need not only courage but unity. The nation cannot afford another parliament based on open class division, bitter party strife, and the remorseless friction of two great party machines.</t>
+  </si>
+  <si>
+    <t>Just under four years ago the Liberal Manifesto opened with the statement that this country was "facing a new crisis and one of the biggest in our history".
+It would be ungenerous not to admit that since the last General Election we have gone some way to arrest the decay which set in with the second post-war Labour Government; the crisis was confronted but has not been resolved. There are still great problems fraught with danger which cause much concern.
+There are some who are so encouraged by the better face of our affairs as to think that halcyon days have come; there are some who feel that it does not greatly matter which Party steers because the winds have abated and the sea is calm; there are some who believe that we have now reached such stability and such assurance of continued prosperity that socialism and other forms of extremism can be counted out; there are some who can persuade themselves against all the evidence that the Conservative and Socialist Parties are liberalised. These ideas are delusions. The Liberal Party stands as a security against the fate that would befall a people whose future depended upon the outcome of a struggle between two class parties seeking power to be used in the service of their own particular clients. The independent mind, the small man and the consumer are neglected by both the great Parties.
+War, devastating and possibly final, is a continuing threat. The fear of war enforces the use on a colossal scale of manpower and materials on purposes of defence. The prosperity of Britain hangs in the balance Continued inflation endangers all the social progress of the last ten years, checks further progress and may defeat our hopes of making full employment in a free society our normal economic condition. To face and overcome external and internal dangers Liberal policies remain essential, and Liberal Members of Parliament alone can effectively advocate them.</t>
+  </si>
+  <si>
+    <t>People Count. . . and because more and more people are realizing that Liberals believe that People count there has been the recent remarkable increase in public support for the Liberal Party. At this Election we hope to consolidate and improve that position as a first stage to the eventual formation of a Liberal Government which will be able to create a Liberal society in this country.
+That is our ultimate aim and we appeal to all progressively minded people to start by working and voting for Liberal candidates at this vital Election.
+At the General Election the votes do not choose a Government, they choose a Parliament. The first task is for everyone to vote for a Member of Parliament and that Member should represent you and your neighbours.
+You will get a Tory or Socialist Government after this Election, but the kind of Tory or Socialist Government you get will depend on the strength of Liberalism in the House of Commons and the strength of the Liberal vote in the country.
+The House of Commons should be a strong influence on the Government. That is what it is for. Lately it has been far too much under the thumb of the Party machines and we must have more Liberals to save us from Tory or Labour reactionaries.
+If the House of Commons is to be truly representative we must breathe new life into it to make it what you and I want. This has not been happening. First, most of the issues today are not between Conservatives and Socialists but between Liberals and the Government, whether it be Conservative or Socialist.
+For instance, the question of how industry should be run is largely one of providing encouragement for efficient management, giving a greater stake in it, and a greater sense of security to the worker and recognizing the important part which the Trade Unions must play, not against management but in close co-operation with it. We all depend on the industries of this country to produce a higher standard of living.
+Liberals believe that they should not only be efficient but provide a friendly and secure atmosphere in which everyone involved can have a sense of useful purpose in serving the community. The only people who continually hammer away at this are the Liberals.
+The need to bring the Social Services up to date and to sweep away out of date restrictions on the individual is a Liberal task.
+In Foreign Affairs, are we to put ourselves at the head of a great movement for greater Western Unity as Liberals want - a unity which is vital if the summit talks are to succeed in establishing a genuine peace? This is a Liberal issue.
+On Defence, the issue for years has been "Does Britain need to make its own A-Bombs." On this Tories and Labour have been united in saying 'yes'. Only recently (and possibly too late) has Labour begun to see that if every country makes its own bombs the risk of war is increased. Liberals for years have been saying that the H-bomb ought to be held in trust for all the free peoples and we should all make a contribution to its production.
+Again in Africa, the issue is a fundamental Liberal one about how you treat human beings, in which the irresponsible desire for domination of black by white or white by black must be eradicated in favour of a system in which all races mix freely with full respect for one another.
+The Conservative and Labour Parties are not united internally on many of the important issues such as Defence and financial policy. We have seen resignations from the Government we know the fierce arguments which go on behind closed doors in Socialist Committees.
+These arguments should not be hidden from the light of day. They should take place in the House of Commons and in the open Council Chamber, but the last thing either the Conservative or Labour Parties want is to air their disagreements in public.
+We must have more Liberals in Parliament and Local Government for the sake of honest, above board politics. We must have Liberals to raise these Liberal issues. The Conservative Party is clearly identified in the minds of the electors with employers and big business, and they cannot deal objectively or fairly with the problems continually arising between employer and employee. The Labour Party is in the hands of the Trade Union Leaders.
+The return of a Socialist Government inevitably means that management is put on the defensive, for it does not know what is going to hit it next The return of a Conservative Government means that the Trade Unions feel justified in going on to the offensive.
+The whole nation is the loser from this crazy line up of power politics, and those who lose most in the struggle are those who live on fixed incomes, such as old age pensioners and a host of others who are solicited at Election time but are forgotten after the result is declared.
+A Liberal vote is a protest against the British political system being divided up between two powerful Party machines, one largely financed by the employers and the other by the Trade Unions.
+There is a vital task to be done in building up a Progressive alternative Party. The Labour Party have failed to appeal to youth; they have lost their enthusiasm: and so long as they remain tied to nationalisation (which is part of their constitution) and financed by the vested interests of the Trade Union establishment, they will never broaden their appeal sufficiently to embrace all the people who want a progressive party in this country.
+England is a democracy and that means there is a Government and an Opposition, and one takes the place of the other from time to time. After all, even Tories do not presumably envisage a Tory Government for ever, there must be an alternative and it should be Liberal, not Socialist.
+As a result of the failure of the Labour Party to free itself from sectional interests or keep up its momentum, there seems at the moment to be every likelihood of another Tory Government. If it is not to slip under the influence of its reactionary wing we must demonstrate that there is a strong non-socialist block of opinion in the country which will not tolerate oppression in Africa, another Cyprus, or complacency over inflation, Government expenditure, and the set-up in the nationalised industries.
+A big Liberal vote would show that there are people who share Labour's concern about poverty but who are opposed to nationalisation. This would make it harder for Labour leaders to carry through the nationalisation of steel and other industries.
+There are millions of Liberals in this country. There are also millions of young people and uncommitted voters who simply do not see themselves mirrored in the image of Tory bigwigs or Labour bosses. There are all the consumers, small business owners, professional men and technicians, craftsmen and farmers, fishermen, shopkeepers and pensioners who have no interest in the Capital v Labour struggle and are greatly harmed by it. Now is their chance to make themselves felt in the New Liberal Party.
+Below you can read some of the chief points in our policy but the immediate task is to build a non-Socialist Opposition whose arteries are not too hard to stand the flow of real blood of enthusiasm about the real issues of our time.</t>
+  </si>
+  <si>
+    <t>The Liberal Party offers the electorate a radical, non-Socialist alternative. In the long run, our objective is to form a government. In the short run, we seek sufficient support to send back a force of Liberal M.P.s which will hold a decisive position in the next Parliament.
+Many thinking people in Britain dissociate themselves from politics today. A strong Liberal Party is essential to bring them into public life.
+In the past five years we have brought new blood into local government by increasing the number of Liberal councillors from 500 to over 1,800. We have pioneered great issues of policy like the Common Market, regionalism and the need for national policies on redundancy and monopolies.
+Liberal by-election successes forced the Prime Minister to sack seven Ministers and make the first hesitant Tory gestures towards modernization. We ask for your vote at this general election to bring about a more substantial and dramatic change in British politics.
+A decisive Liberal influence is needed, in particular, to carry out three major aims. Modern technology provides the means of achieving a new age of abundance which could provide everyone with a richer life and great new opportunities. Since the war this country has lagged behind and failed to seize these opportunities. The vested interests in the Conservative and Labour parties have blocked the way. The Liberal Party seeks a decisive position in the next Parliament to make sure that change and growth are stimulated.
+Our second aim is to ensure that individual people benefit from the new industrial revolution. The age of automation could be an age when the individual is trampled on and power is dangerously concentrated in the hands of big business and the state. Change must be humanised so that the new wealth within our reach is used to give the individual a richer life and protect the weak. Class consciousness in the factory, on the housing estate, or in politics, must give way to a new spirit of partnership.
+The third Liberal objective is to apply the idea of partnership in international affairs. In the nuclear age mankind cannot afford narrow nationalism. The economic benefits of modern science can only be achieved if there is a lavish flow of ideas, people and goods, amongst the nations. The giant risks of the nuclear age and the explosive problem of world poverty cannot be mastered until the nations act together. A strong force of Liberal M.P.s will ensure that Britain plays a new and greater part as a pioneer of the new international order that mankind so badly needs.</t>
+  </si>
+  <si>
+    <t>Eighteen months ago many people had high hopes that a change of Government from Conservative to Labour would bring about a real change in the country's fortunes. They had watched the country drift from one economic crisis to another and seen how Britain's rate of expansion and industrial growth had continued to fall behind that of other countries.
+Now events have shown that, for all their talk about modernisation, Labour too cannot find the answer to our problems. However admirable their intentions. they, like the Conservatives, have been unable to implement workable solutions.
+There are very simple reasons for this. Both parties have their roots firmly in one section of the community or another. The Conservatives, both ideologically and financially, are still tied to the interests of capital. Equally Labour are tied to the interests of the Unions, often to the detriment of both.
+Is it surprising that their actions are seldom acceptable or effective for the country as a whole?
+Today, more than ever, the unique position of the Liberal Party enables us to bring new thinking and a fresh, objective approach to Britain's economic and social problems and to put forward solutions that work. We can do this precisely because we have no vested interest in protecting one group or another. We are not a class party'. We draw our support from all groups and classes and we are free to reconcile conflicting interests for the benefit of the whole community. We are the party of all individuals, no matter what their background.
+Already the three million votes polled at the last election in support of Liberal attitudes and Liberal policies have acted as a powerful brake and a positive influence on the policies of the Labour Government. Indeed the Liberal Party has provided the only effective opposition in curbing the wasteful excesses of Socialism and compelling Labour to give priority to at least some of the things that matter.
+Steel nationalisation was shelved as a result of Liberal pressure and saved the country millions of pounds. Without that pressure it could still happen.
+Land nationalisation was checked in response to Liberal pressure. The nationalisation of small plots of building land in private ownership has been dropped.
+Pensions and rates. Although Labour's plans do not go far enough Liberal pressure has forced the Government to put these issues before further nationalisation plans.
+The Neglected Regions. For years Liberals have been calling for action to revitalise the depressed areas of Britain. Even the tentative moves now being made by Labour would not have been made but for Liberal pressure.
+The Highland Development Board. A clear example of a Liberal proposal being implemented by Labour in response to pressure from the Highland Liberal MPs.
+A Really Positive Vote. The effectiveness of Liberal pressure to date is only the beginning. An increased number of Liberal MPs and an increased Liberal vote in each constituency will bring about still more positive action in Parliament. And there is plenty to be done.
+The most vital need is for a fresh and realistic approach to economic planning, defence and the machinery of government, because only then will the wealth be created that can bring about a real improvement in living standards, housing, education and the social services for all the people of Britain.
+The policies outlined show the positive action that is needed. Consider them carefully and decide for yourself.
+Three million people voted Liberal last time for what they knew was right. The 10 Liberal MP's have done the work of 30 times that many. Those votes have really counted. A higher vote. More MPs. The same drive. And a Liberal Government will be near.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,6 +1615,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -965,10 +1647,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1284,15 +1968,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D6C4B3-4694-4D7C-8241-D0EA9A7209FC}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="62.21875" style="1" customWidth="1"/>
   </cols>
@@ -1301,14 +1986,14 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1316,746 +2001,1376 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1974</v>
+        <v>132</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>167</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1983</v>
+        <v>129</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>159</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1983</v>
+        <v>131</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>210</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1987</v>
+        <v>132</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>1987</v>
+        <v>129</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>1992</v>
+        <v>131</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>165</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>211</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>1992</v>
+        <v>132</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>1992</v>
+        <v>129</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>190</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>1997</v>
+        <v>131</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>212</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>1997</v>
+        <v>132</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>1997</v>
+        <v>129</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>160</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>1997</v>
+        <v>131</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>213</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>2001</v>
+        <v>132</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>171</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>2001</v>
+        <v>129</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>2001</v>
+        <v>131</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>214</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>2001</v>
+        <v>132</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>35</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>2005</v>
+        <v>129</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>162</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>94</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <v>2005</v>
+        <v>131</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>215</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <v>2005</v>
+        <v>132</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>53</v>
+        <v>173</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>96</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21">
-        <v>2005</v>
+        <v>129</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>163</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>194</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>97</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>2005</v>
+        <v>131</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>216</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>98</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" t="s">
         <v>4</v>
       </c>
-      <c r="B23">
-        <v>2010</v>
-      </c>
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>57</v>
+        <v>181</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>2010</v>
+        <v>129</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25">
-        <v>2010</v>
+        <v>131</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26">
-        <v>2010</v>
+        <v>132</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>102</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27">
-        <v>2010</v>
+        <v>129</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>103</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>2015</v>
+        <v>131</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29">
-        <v>2015</v>
+        <v>132</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>65</v>
+        <v>184</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>105</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30">
-        <v>2015</v>
+        <v>129</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>64</v>
+        <v>207</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31">
-        <v>2015</v>
+        <v>131</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>2015</v>
+        <v>132</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33">
-        <v>2017</v>
+        <v>129</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34">
-        <v>2017</v>
+        <v>131</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35">
-        <v>2017</v>
+        <v>132</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36">
-        <v>2017</v>
+        <v>129</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37">
-        <v>2017</v>
+        <v>131</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38">
-        <v>2019</v>
+        <v>132</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39">
-        <v>2019</v>
+        <v>129</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>115</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40">
-        <v>2019</v>
+        <v>131</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41">
-        <v>2019</v>
+        <v>132</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B42">
-        <v>2019</v>
-      </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>118</v>
+      <c r="E68" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>131</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" t="s">
+        <v>79</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" t="s">
+        <v>63</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D7371718-58B6-44A1-B12B-1BCAA4964B42}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{29613CAF-2038-4D33-999A-49CC0C5EBEA1}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{82003BC9-261C-498E-A7A0-5A316A101FA0}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{86BA4AB3-91DE-4965-8A52-5C7915BF2288}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{5BF064B8-4788-444B-852E-B0F85BF9F61F}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{CAD11900-4F62-49AA-897C-CBDADF5AE6BB}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{7815F4BA-E0C6-4D59-93A4-6C3C546AE73B}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{6A8BFAE7-F4C3-4962-BACD-18EC0517CE75}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{E62BFF6B-2EA8-4D63-92E4-9C439375677F}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{D68A4F37-6F6F-49A2-9DB1-7F9CFEB0E36E}"/>
-    <hyperlink ref="D13" r:id="rId11" xr:uid="{F80DFD9A-574E-4CB4-A487-9B96169AD3DD}"/>
-    <hyperlink ref="D14" r:id="rId12" xr:uid="{DBB52C04-7E52-4463-94BC-455822B92727}"/>
-    <hyperlink ref="D15" r:id="rId13" xr:uid="{9C390DB6-3210-49EC-B23E-0539EB002217}"/>
-    <hyperlink ref="D16" r:id="rId14" xr:uid="{D4F6D3AD-651D-4864-B3AF-EDABDDF98652}"/>
-    <hyperlink ref="D17" r:id="rId15" xr:uid="{501D7B83-5D4B-4647-A5A7-6FC823F7EE00}"/>
-    <hyperlink ref="D18" r:id="rId16" xr:uid="{2C05A670-2A5A-469B-BF8E-E5667A1D24DF}"/>
-    <hyperlink ref="D20" r:id="rId17" xr:uid="{9A4FB7A9-6B5E-4D25-BEE5-D6B1DCBE8646}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{DA8B88A4-3CA8-44D2-A01A-C085094FD401}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{8C7F8365-5BCF-47D2-BA54-012A4111D58F}"/>
-    <hyperlink ref="D25" r:id="rId20" xr:uid="{66A90D95-889E-4EEC-A486-278CE83ABCD1}"/>
-    <hyperlink ref="D24" r:id="rId21" xr:uid="{B7DBD44E-CB6B-42EE-96BC-D4676A8C8D5F}"/>
-    <hyperlink ref="D28" r:id="rId22" xr:uid="{75B1BB56-2757-415D-94A2-816A8DFBBBD6}"/>
-    <hyperlink ref="D30" r:id="rId23" xr:uid="{79AA7B72-6791-4FA5-AAB8-0EFFAD1FA2CA}"/>
-    <hyperlink ref="D29" r:id="rId24" xr:uid="{A03EDA82-3A2E-4B03-89D3-C3D5CE2D7582}"/>
-    <hyperlink ref="D31" r:id="rId25" xr:uid="{4BC1A719-F7FF-426D-8C51-6F4708899C76}"/>
-    <hyperlink ref="D32" r:id="rId26" xr:uid="{9E76004A-CC93-42C9-B93A-CFB844B12859}"/>
-    <hyperlink ref="D33" r:id="rId27" xr:uid="{D7F16FB4-1888-4303-B2D3-BFD3FF131743}"/>
-    <hyperlink ref="D35" r:id="rId28" xr:uid="{B38BCD6E-D43B-407E-BDA6-8082CD44215B}"/>
-    <hyperlink ref="D34" r:id="rId29" xr:uid="{C9A71007-38B7-4B17-88DC-CFBD806BFB6E}"/>
-    <hyperlink ref="D36" r:id="rId30" xr:uid="{592C30BE-BA5D-493F-BFC0-118C3EAA15A6}"/>
-    <hyperlink ref="D37" r:id="rId31" xr:uid="{AE34F1D4-1906-479F-A55B-827199F1ADDA}"/>
-    <hyperlink ref="D38" r:id="rId32" xr:uid="{49CE0AD2-5EB2-44CE-A43F-26E05E7CE28A}"/>
-    <hyperlink ref="D39" r:id="rId33" xr:uid="{75640ADC-21AA-4D0C-8639-AA4E5B345998}"/>
-    <hyperlink ref="D40" r:id="rId34" xr:uid="{137F227D-7821-4183-B122-92EF8BAC7DFE}"/>
-    <hyperlink ref="D41" r:id="rId35" xr:uid="{05E1DA35-0899-474D-8533-6CF1F1556381}"/>
-    <hyperlink ref="D11" r:id="rId36" xr:uid="{36843EB4-D203-4905-9CBA-08E0CF7E7DFB}"/>
-    <hyperlink ref="D22" r:id="rId37" xr:uid="{E54BFA64-F35A-402E-AE35-D2D6E81485EA}"/>
-    <hyperlink ref="D21" r:id="rId38" xr:uid="{A2E9EFAD-FEB5-4964-97B5-A05A27DAD294}"/>
-    <hyperlink ref="D26" r:id="rId39" xr:uid="{2076C4C5-164A-43EA-8EDC-FBE2AE2287A1}"/>
-    <hyperlink ref="D27" r:id="rId40" xr:uid="{BADCAE52-CBAA-4307-B7B2-7C3961A92C9D}"/>
-    <hyperlink ref="D42" r:id="rId41" xr:uid="{5448D857-AD73-4762-9F4B-B55411AAD96F}"/>
+    <hyperlink ref="D26" r:id="rId1" xr:uid="{D7371718-58B6-44A1-B12B-1BCAA4964B42}"/>
+    <hyperlink ref="D35" r:id="rId2" xr:uid="{29613CAF-2038-4D33-999A-49CC0C5EBEA1}"/>
+    <hyperlink ref="D36" r:id="rId3" xr:uid="{82003BC9-261C-498E-A7A0-5A316A101FA0}"/>
+    <hyperlink ref="D38" r:id="rId4" xr:uid="{86BA4AB3-91DE-4965-8A52-5C7915BF2288}"/>
+    <hyperlink ref="D39" r:id="rId5" xr:uid="{5BF064B8-4788-444B-852E-B0F85BF9F61F}"/>
+    <hyperlink ref="D41" r:id="rId6" xr:uid="{CAD11900-4F62-49AA-897C-CBDADF5AE6BB}"/>
+    <hyperlink ref="D42" r:id="rId7" xr:uid="{7815F4BA-E0C6-4D59-93A4-6C3C546AE73B}"/>
+    <hyperlink ref="D44" r:id="rId8" xr:uid="{6A8BFAE7-F4C3-4962-BACD-18EC0517CE75}"/>
+    <hyperlink ref="D45" r:id="rId9" xr:uid="{E62BFF6B-2EA8-4D63-92E4-9C439375677F}"/>
+    <hyperlink ref="D47" r:id="rId10" xr:uid="{D68A4F37-6F6F-49A2-9DB1-7F9CFEB0E36E}"/>
+    <hyperlink ref="D48" r:id="rId11" xr:uid="{F80DFD9A-574E-4CB4-A487-9B96169AD3DD}"/>
+    <hyperlink ref="D49" r:id="rId12" xr:uid="{DBB52C04-7E52-4463-94BC-455822B92727}"/>
+    <hyperlink ref="D50" r:id="rId13" xr:uid="{9C390DB6-3210-49EC-B23E-0539EB002217}"/>
+    <hyperlink ref="D51" r:id="rId14" xr:uid="{D4F6D3AD-651D-4864-B3AF-EDABDDF98652}"/>
+    <hyperlink ref="D52" r:id="rId15" xr:uid="{501D7B83-5D4B-4647-A5A7-6FC823F7EE00}"/>
+    <hyperlink ref="D53" r:id="rId16" xr:uid="{2C05A670-2A5A-469B-BF8E-E5667A1D24DF}"/>
+    <hyperlink ref="D55" r:id="rId17" xr:uid="{9A4FB7A9-6B5E-4D25-BEE5-D6B1DCBE8646}"/>
+    <hyperlink ref="D54" r:id="rId18" xr:uid="{DA8B88A4-3CA8-44D2-A01A-C085094FD401}"/>
+    <hyperlink ref="D58" r:id="rId19" xr:uid="{8C7F8365-5BCF-47D2-BA54-012A4111D58F}"/>
+    <hyperlink ref="D60" r:id="rId20" xr:uid="{66A90D95-889E-4EEC-A486-278CE83ABCD1}"/>
+    <hyperlink ref="D59" r:id="rId21" xr:uid="{B7DBD44E-CB6B-42EE-96BC-D4676A8C8D5F}"/>
+    <hyperlink ref="D63" r:id="rId22" xr:uid="{75B1BB56-2757-415D-94A2-816A8DFBBBD6}"/>
+    <hyperlink ref="D65" r:id="rId23" xr:uid="{79AA7B72-6791-4FA5-AAB8-0EFFAD1FA2CA}"/>
+    <hyperlink ref="D64" r:id="rId24" xr:uid="{A03EDA82-3A2E-4B03-89D3-C3D5CE2D7582}"/>
+    <hyperlink ref="D66" r:id="rId25" xr:uid="{4BC1A719-F7FF-426D-8C51-6F4708899C76}"/>
+    <hyperlink ref="D67" r:id="rId26" xr:uid="{9E76004A-CC93-42C9-B93A-CFB844B12859}"/>
+    <hyperlink ref="D68" r:id="rId27" xr:uid="{D7F16FB4-1888-4303-B2D3-BFD3FF131743}"/>
+    <hyperlink ref="D70" r:id="rId28" xr:uid="{B38BCD6E-D43B-407E-BDA6-8082CD44215B}"/>
+    <hyperlink ref="D69" r:id="rId29" xr:uid="{C9A71007-38B7-4B17-88DC-CFBD806BFB6E}"/>
+    <hyperlink ref="D71" r:id="rId30" xr:uid="{592C30BE-BA5D-493F-BFC0-118C3EAA15A6}"/>
+    <hyperlink ref="D72" r:id="rId31" xr:uid="{AE34F1D4-1906-479F-A55B-827199F1ADDA}"/>
+    <hyperlink ref="D73" r:id="rId32" xr:uid="{49CE0AD2-5EB2-44CE-A43F-26E05E7CE28A}"/>
+    <hyperlink ref="D74" r:id="rId33" xr:uid="{75640ADC-21AA-4D0C-8639-AA4E5B345998}"/>
+    <hyperlink ref="D75" r:id="rId34" xr:uid="{137F227D-7821-4183-B122-92EF8BAC7DFE}"/>
+    <hyperlink ref="D76" r:id="rId35" xr:uid="{05E1DA35-0899-474D-8533-6CF1F1556381}"/>
+    <hyperlink ref="D46" r:id="rId36" xr:uid="{36843EB4-D203-4905-9CBA-08E0CF7E7DFB}"/>
+    <hyperlink ref="D57" r:id="rId37" xr:uid="{E54BFA64-F35A-402E-AE35-D2D6E81485EA}"/>
+    <hyperlink ref="D56" r:id="rId38" xr:uid="{A2E9EFAD-FEB5-4964-97B5-A05A27DAD294}"/>
+    <hyperlink ref="D61" r:id="rId39" xr:uid="{2076C4C5-164A-43EA-8EDC-FBE2AE2287A1}"/>
+    <hyperlink ref="D62" r:id="rId40" xr:uid="{BADCAE52-CBAA-4307-B7B2-7C3961A92C9D}"/>
+    <hyperlink ref="D77" r:id="rId41" xr:uid="{5448D857-AD73-4762-9F4B-B55411AAD96F}"/>
+    <hyperlink ref="D37" r:id="rId42" xr:uid="{858B6E84-29F7-429E-AE95-25B7AD93E5C0}"/>
+    <hyperlink ref="D34" r:id="rId43" xr:uid="{FD3E3B4C-29F6-4D8B-A1AF-D186679148B8}"/>
+    <hyperlink ref="D40" r:id="rId44" xr:uid="{089089D2-B642-4566-B78E-B4DD9735D31B}"/>
+    <hyperlink ref="D43" r:id="rId45" xr:uid="{024C1334-D7CE-4286-AA92-8288553A807E}"/>
+    <hyperlink ref="D25" r:id="rId46" xr:uid="{ED613AAC-A737-402A-A7AE-86BC0DF101E0}"/>
+    <hyperlink ref="D28" r:id="rId47" xr:uid="{B3DC5D65-F951-4D80-AFA7-F84B7CB7EB7D}"/>
+    <hyperlink ref="D31" r:id="rId48" xr:uid="{DB9CBA10-86A7-4664-9FBA-51B23AA846DD}"/>
+    <hyperlink ref="D2" r:id="rId49" xr:uid="{9FDBF89D-D0E0-435A-843C-9E4F8088BEDE}"/>
+    <hyperlink ref="D5" r:id="rId50" xr:uid="{1B825FEC-378E-4719-BB83-5C5EC859A9F0}"/>
+    <hyperlink ref="D8" r:id="rId51" xr:uid="{E96C1A10-B9D2-4BE2-BB30-AFED637D77A5}"/>
+    <hyperlink ref="D11" r:id="rId52" xr:uid="{CAFB0F4A-C9D9-4887-9328-D8B7AA42086F}"/>
+    <hyperlink ref="D14" r:id="rId53" xr:uid="{59264C40-5848-4257-861C-5EB690848749}"/>
+    <hyperlink ref="D17" r:id="rId54" xr:uid="{DE13670C-FACA-4694-AA2A-3FB3FA7EC2BD}"/>
+    <hyperlink ref="D20" r:id="rId55" xr:uid="{22D87374-DFA4-4CC3-B4CB-A37089FACC43}"/>
+    <hyperlink ref="D23" r:id="rId56" xr:uid="{44EF5743-9AF1-447B-A028-563DA71EB2EE}"/>
+    <hyperlink ref="D29" r:id="rId57" xr:uid="{4E6365BD-CB9F-4764-A3A4-4C077B22D98A}"/>
+    <hyperlink ref="D32" r:id="rId58" xr:uid="{B6BC084B-93B7-4D62-97C2-2A7302161267}"/>
+    <hyperlink ref="D3" r:id="rId59" xr:uid="{735A807E-A069-47B2-ACBD-88A8382DC7C0}"/>
+    <hyperlink ref="D6" r:id="rId60" xr:uid="{2F8727A1-BB8A-4818-9903-593953DAC4D7}"/>
+    <hyperlink ref="D9" r:id="rId61" xr:uid="{F83C40E1-D412-443D-8F1E-8B2E58973B42}"/>
+    <hyperlink ref="D12" r:id="rId62" xr:uid="{32D171CB-2A22-4AF6-9304-2BE62606820C}"/>
+    <hyperlink ref="D15" r:id="rId63" xr:uid="{EC562266-9033-4350-912C-2964574CC1AD}"/>
+    <hyperlink ref="D18" r:id="rId64" xr:uid="{709542EC-4CE9-4A7C-AF90-735102CFAC68}"/>
+    <hyperlink ref="D21" r:id="rId65" xr:uid="{10F4B09A-7449-4289-B264-B7F399EAA683}"/>
+    <hyperlink ref="D24" r:id="rId66" xr:uid="{B9D519DC-A441-4DC3-BE20-95799F858DAC}"/>
+    <hyperlink ref="D27" r:id="rId67" xr:uid="{FB5B66B5-8CE2-4A1A-9EFA-090190206CE6}"/>
+    <hyperlink ref="D30" r:id="rId68" xr:uid="{990C6BDB-84F6-4ED5-91E0-C6BDCE50EC19}"/>
+    <hyperlink ref="D33" r:id="rId69" xr:uid="{EB13DC78-CD4E-40D9-AF42-F03708587C2C}"/>
+    <hyperlink ref="D4" r:id="rId70" xr:uid="{B78B4CF4-2838-4592-A00A-884D53D76D35}"/>
+    <hyperlink ref="D7" r:id="rId71" xr:uid="{08355141-B1B5-43F1-8BE2-411A86D96BEF}"/>
+    <hyperlink ref="D10" r:id="rId72" xr:uid="{8FCF0E72-4E67-425E-8DB0-B65A50895DC8}"/>
+    <hyperlink ref="D13" r:id="rId73" xr:uid="{72F650FC-8EB0-48AB-A40F-C03F4A5B8A8D}"/>
+    <hyperlink ref="D16" r:id="rId74" xr:uid="{4A3F7F64-64BD-4AEF-9A5D-385A80847A7F}"/>
+    <hyperlink ref="D19" r:id="rId75" xr:uid="{76D08BD9-6ACB-465C-95C8-AC7BC74FA433}"/>
+    <hyperlink ref="D22" r:id="rId76" xr:uid="{B2F277A7-CC8B-42DE-9BAB-B973904EB620}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId77"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Manifestos extended back to 1900!
Now including 1910s Liberal manifestos (with temperance movement and rural policies); 1920s radical Labour manifestos; 1930s Labour and Conservative manifestos during the national government coalition era - exciting!
</commit_message>
<xml_diff>
--- a/manifesto-forewords/manifestos.xlsx
+++ b/manifesto-forewords/manifestos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\SDS thesis\scraping-political-speeches\manifesto-forewords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB059A5-5338-4C46-9DB1-FD7D66CA7D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BF8609-2D73-480F-9A84-3BAD15D775A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6410A5E-2F41-44E7-A64E-C2EE33441A0E}"/>
+    <workbookView xWindow="7185" yWindow="765" windowWidth="21600" windowHeight="11235" xr2:uid="{F6410A5E-2F41-44E7-A64E-C2EE33441A0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="307">
   <si>
     <t>party</t>
   </si>
@@ -1597,6 +1597,850 @@
 The most vital need is for a fresh and realistic approach to economic planning, defence and the machinery of government, because only then will the wealth be created that can bring about a real improvement in living standards, housing, education and the social services for all the people of Britain.
 The policies outlined show the positive action that is needed. Consider them carefully and decide for yourself.
 Three million people voted Liberal last time for what they knew was right. The 10 Liberal MP's have done the work of 30 times that many. Those votes have really counted. A higher vote. More MPs. The same drive. And a Liberal Government will be near.</t>
+  </si>
+  <si>
+    <t>1900</t>
+  </si>
+  <si>
+    <t>Henry Campbell-Bannerman</t>
+  </si>
+  <si>
+    <t>H.H. Asquith</t>
+  </si>
+  <si>
+    <t>1906</t>
+  </si>
+  <si>
+    <t>1910 Jan</t>
+  </si>
+  <si>
+    <t>1910 Dec</t>
+  </si>
+  <si>
+    <t>1918</t>
+  </si>
+  <si>
+    <t>1922</t>
+  </si>
+  <si>
+    <t>1923</t>
+  </si>
+  <si>
+    <t>1924</t>
+  </si>
+  <si>
+    <t>1929</t>
+  </si>
+  <si>
+    <t>1931</t>
+  </si>
+  <si>
+    <t>1935</t>
+  </si>
+  <si>
+    <t>David Lloyd George</t>
+  </si>
+  <si>
+    <t>Herbert Samuel</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1900/1900-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1918/1918-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1922/1922-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1923/1923-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1924/1924-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1929/1929-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1931/1931-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1935/1935-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>Yielding to pressure from the less scrupulous of his colleagues and supporters, Lord Salisbury has recommended the Queen to dissolve Parliament as and from today. When Lord Beaconsfield was blamed for not taking a General Election in 1878 on the conclusion of the Berlin Conference, he declared that:
+'A Minister with a large majority in the House of Commons has no business to dissolve merely with the object of gaining an advantage at the polls due to transitory circumstances. It is said I have lost a golden opportunity. I am not so sure of it. The English people do not like breaches of Constitutional practice.'
+It would seem that Her Majesty's present advisers are less scrupulous than Lord Beaconsfield, and a 'Khaki' Election in the month of October is accordingly ordered.
+The Nation will not soon forget the dark days of less than a year ago following the miscalculation of a Government that had risked a war without first counting the cost. The matter of conducting the negotiations had, at least, not made for a peaceful solution. For years this Government, without remonstrance, had allowed the Transvaal to arm itself to the teeth, and yet continued to underestimate its military strength. Diasters in the field fell like thunderclaps upon our country and overwhelmed it with shame, apprehension, and distress. Out of this state of humiliation it has been lifted, not by the statesmanship and administration of the Government, but by the genius of Lord Roberts and the bravery and endurance of officers and men; while the whole people, without distinction of Party, calmly, patiently, stubbornly facing their adversity, have cheerfully yielded up those they love best to hardship and to death in the service and for the honour of a common country.
+And now this Government are scheming that in the achievements of a great General and a brave army their own negligence, miscalculation, and the manifold misdoing shall be forgiven and forgotten. They are seeking to prostitute the sacrificies of a whole people to the interests of one political Party. By a Dissolution on a stale Register and a point-blank refusal of such special legislation as would put the new Register in force - sharp practice unprecedented since the great Reform Bill - they deliberately disfranchise half a million of electors, and their appeal to the nationl for a verdict of acquittal and confidence is so far a delusion and a sham. Liberal, whatever their differences of opinion, must unite in indignant protest against such an obvious and discreditable electioneering trick, and call upon their fellow-citizens not to be blinded to the vast and varied interests at stake by the dust of a false and partial issue. Not Lord Roberts and his soldiers, but Lord Salisbury and his colleagues ask for the Nation's confidence, and that in all departments, for the next six years.
+What have they done to deserve it? Have they other credentials than the mis-management of negotiations and of war?
+Abroad, where it was prophesied for them by one of themselves that the advent of this Heaven-sent Government would shed an unwonted felling of calm and security over Europe, their career has been marked by a continuous series of wars and rumours of war. In theories and complications with which they have been called upon to deal, they have shown neither clear purpose nor resourceful diplomacy, not any true sense of the greatness and dignity of the country whose destinies and traditions have been committed to their keeping. In the Near East, thanks to the feebleness and ineffectiveness with which the voice of this country was heard in the Councils of Europe, we have seen the Armenian Christians slaughtered and unavenged, Greece humiliated, the Sultan triumphant, and Crete only delivered from his sway by a happy accident, of which admirals were able to take advantage where Statesmen had failed. In India the wanton breach of the country's pledged word and the abandonment of the wise policy of their predecessors kindled the whole frontier into a flame. In Siam, Tunis, and Madagascar British interests were gratuitously sacrificed by a series of what were called 'graceful concessions'.
+Finally, in the Far East the Government subjected the country to a succession of humiliation. They entered into a futile and unnecessary contest with Russia, on which they were at every point worsted. They neglected golden opportunities which might have been seized with effect, and finally were forced to console themselves and the country with Wei-hai-Wei, the possession of which has imposed an additional burden to our already over-taxed military resources, and is a source of naval weakness rather than strength. And in this, as in all other matters, the Government so unskilfully represented the interests and presented the case of this country, that the nations of Europe now stand towards us in an attitude of hostility and suspicion.
+At home, the lavish and grandiloquent promises with which the confidence of the country was wooed have issued in a singularly bare and exiguous performance. The great social programme has evaporated into air. The scheme for Old Age Pensions, which was so simple that anyone could understand it,' and which 'any Liberal Unionist agent' was prepared to explain, has disappeared in a vanishing vista of Committees of Inquiry. The great question of Temperance Reform, which bulked so largely in election addresses, has also been shelved. In the early days of the Government it was pushed aside, the profits of the Brewers being preferred to the prayers of the Bishops, and of late, when revived by the highly significant Report of his own licensing Commission, it was dismissed by the Prime Minister with cheap jibes about 'free indulgence.' The scheme of Employers' liability which was to compensate 'every man for every accident', 'as a matter of right and certainty, without the risk of litigation,' has partial in its incidence, and has proved the most litigious Act of modern times.
+There is one section of their policy to which the Government have devoted themselves with zeal and persistence - that of administering doles from the public exchequer to the classes on whose support they rely. That policy appears to have been pursued with all the more gratification because it involved the emphasis and extension of the principle of Sectarianism in Education, and preserved the so-called 'Voluntary' Schools from that public control which should always follow the grant of public money. In doles of this sort of Agricultural Landowners, to Clerical Tithepayers and to Denominational Schools, the whole of the magnificent revenue derived from Sir William Harcourt's great financial reforms has been uselessly and mischievously dribbled away; during years of peace and increasing income there has been no substantial remission of taxation; while, to complete the picture of the Government's financial recklessness, the Sinking Fund, the reserve of the country against the time of war, was wantonly raided, in the teeth of his own financial principles, by the Chancellor of the Exchequer.
+Is it likely that the nation will forget this record of the Government's unskilful handling of its interests abroad, and the vicious principles of its legislation at home? Shall we not all unite in condemnation of a Ministry which, for the five years of its existence, has kept the Empire in a ferment, has squandered its resources, and in legislation and administration has shown neither the will nor the power to pursue or to initiate a policy of progress and reform?
+The miliary conquest of the Orange Free State and the Transvaal is said to be over, and those territories have been formally annexed to the dominions of the British Crown. But to annex a territory is one thing, to settle it is another. There remains before this country a task of delicacy and difficulty which throw mere operations of war into the shade. It is a task which calls for tenacious purpose, discriminating judgement, broad and liberal sympathies. It consists in the reconciliation of a humbled but brave people to the conditions of a new flag, and in the reconstruction of free institutions within the bounds of an Empire for meny who before owed no direct allegiance save to themselves. Is such a task to be left to a Party with Tory ideals and Tory traditions, and a Government with the personnel and the record of the present administration? Is it reasonable to expect that those who so little understood the task before them at the beginning of the war, will be able to cope with the far heavier and more complicated problems presented by its sequel? These are the questions connected with South Africa which the electorate of these islands have now the opportunity and the responsibility of determining.
+There are, moreover, far-reaching questions affecting the relations between the Colonies and the Mother Country to which new attention has been directed by the attitude and action of the Colonies in this war. These are questions which ought not to be left for solution to the Tory Party, whose record in these matters in times past has never been happy, and has sometimes been disastrous.
+But we do not forget that questions of Foreign Policy and the Government of our Empire across the seas are by no means only matters for Liberals to ponder. Nor does our duty end with opposition to the class legislation with the Government has forced upon us. It is sometimes said by cynics that the work of the Liberal Party is done, but he who thinks this must be blind indeed to the grim and menancing group of subjects which has been called 'the Conditions of the People Question.' So long as the Housing Problems both of the Town and of the Rural Districts remain unsolved; so long as our Land Laws are unreformed; so long as the evils of intemperance continue unchecked; so long as complete Religious Equality is denied; so long as the doors of Parliament are open only to the wealthy; so long as some men have many votes while many have none; so long as the Peers may arbitrarily overrule the Commons - so long must there remain work with the Liberal Party alone can do.
+To secure that the government of the Empire shall be conducted upon liberal principles, to maintain a firm but non-provocative policy abroad, to forward social pgogress at home, and to provide strong business-like administration in all the great Departments of the State, is as much the duty of Liberals today as it ever was, and it is to strenuous endeavour to secure that liberals shall have the power to perform these duties that we call upon our Federated Associations to devote themselves. Every seat won from the Tories is a gain to the cause of the people.</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1910/jan/january-1910-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>I ask for a renewal of the confidence with which on six previous occasions you have honoured me. Never during the long connection between us, as constituency and member, have issues so grave been submitted to you for your decision.
+Four years ago the country gave an emphatic verdict in favour of the maintenance of Free Trade. Since then we have passed through times both of enlarging and of slackening industry, and our fiscal system has stood the test of both. During the alst 12 months a further strain has been cast upon it. A large addition has to be found to the provision for National Defence - an addition due to the paramount necessity of keeping our Navy equal to all the demands that may be made upon it, and superior to all the dangers to which, from any quarter, our Empire may be exposed. At the same time, the grant of old age pensions, and the prospect of further and fuller developments of a policy of social reform, involved the State in liabilities, actual and contingent, which could only be satisfied by a substantial increase of taxation. The Budget was freely and exhaustively discussed in the House of Commons, and in the end it received the approval of an overwhelming majority of the representatives of the people.
+The supporters of what is called Tariff Reform saw in the passing of such a Budget into law the 'death warrant' of their schemes. They accordingly mustered and set in motion the formidable interests and influences which they can command, either as followers or as allies; with the result that the House of Lords, in defiance of the counsels of the wisest and coolest heads in the Tory party, rejected the whole provision which the Commons had made for the finance of the year.
+This is a proceeding without precedent in our history, a wanton breach of the settled practice of the Constitution, and an assumption on the part of the non-representative House of a power to control taxation, which has been repudiated in the past by Tory as emphatically as by Liberal statesmen.
+In a sentence, the House of Lords, has violated the Constitution in order to save from a mortal blow the cause of Tariff Reform.
+If you care either for Free Trade, which has made our country prosperous, or for Popular Government, which has made it free, now is the time to assert your devotion; for in this contest the fortunes of both are at stake.
+There is before you a larger issue still. The claim of the House of Lords to control finance is novel, and a mere usurpation. But the experience of the Parliament which has today been dissolved shows that the possession of an unlimited veto by a partisan people, however clearly expressed, is always liable to be rendered inoperative. Given a Tory majority in the House of Commons, the House of Lords interposes no check upon legislative innovations of the most violent and unexpected kind, as we saw in the case of the Education Act of 1902 and the Licensing Act of 1904. On the other hand, a Liberal majority in the House of Commons, as has been demonstrated during the last four years, is, under existing conditions, impotent to place on the Statute-book the very measures which it was sent to Westminster to carry in to law.
+It is absurd to speak of this system as though it secured to us any of the advantages of a Second Chamber, in the sense in which that term is understood and practically interpreted in every other democratic country.
+The limitation of the veto is the first and most urgent step to be taken; for it is the condition precedent to the attainment of the great legislative reforms which our party has at heart, and which I laid before my fellow Liberals in a recent speech at the Albert Hall.
+I appeal to you, in this momentous crisis, with confidence, for the support which during twenty-four years you have never withdrawn from me.</t>
+  </si>
+  <si>
+    <t>http://www.libdems.co.uk/manifestos/1910/dec/december-1910-liberal-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>I ask you to renew the unbroken relationship between us, as Constituency and Member, which has now entered upon its twenty-fifth year.
+During the whole of this long connection there has been complete confidence both on the one side and the other, and neither you nor I have every wavered in our allegiance to the great ideals and purposes of which the Liberal Party is the champion and trustee.
+I am, therefore, not under the necessity, which would be binding on a new-comer, of making to you any general profession of political faith. As lately as January in the present year, I expounded to you in detail, and you approved by a decisive majority at the poll, the present aims of liberal policy.
+The appeal which is now being made to you and to the country at large may almost be said to be narrowed to a single issue. But upon its determination, in one sense or the other, hangs the whole future of Democratic Government.
+Are the people, through their freely chosen representatives, to have control, not only over finance and administrative Policy, but over the making of their law? Or are we do continue in the one-sided system under which a Tory majority, however small in size and casual in creation, has a free run of the Statute Book, while from Liberal legislation, however clear may be the message of the polls, the forms of the Constitution persistently withhold a fair and even chance?
+You will not, I am sure, be misled in the judgement you are called upon to pronounce by the belated and delusive composition which the House of Lords is, at the last moment, being advised to offer to its critics. The schemes which are now being put forward, in the hope of disguising the real issue, would result, if they were carried into law, in the creation of a Second Chamber predominantly Conservative in character, practically inoperative while there is a Tory majority in the House of Commons, completely independent of the prerogatives of the Crown, and capable of interposing an even more formidable veto than the prsent House of Lords upon the prompt and effective translation into law of the declared will of the nation.
+I ask you to repeat, with still greater emphasis, the approval which only eleven months ago you gave to the proposals of His Majesty's Government.</t>
+  </si>
+  <si>
+    <t>It was in the summer of 1886 that I was first elected member for East Fife. Our boundaries have now been enlarged, and I appeal to the new constituency to grant me a renewal of the confidence which I have enjoyed for an unbroken term of more than thirty-two years. The Parliament in which has just been dissolved has been one of the most remarkable in our history. It carried through a series of great political and social changes, and in its later years had sanctioned and sustained to the end with patriotic unity our national part in the Great War. During most of those stirring events it was my privilege to be First Minister of the Crown. It was while I held that office that our Empire entered the war; that our vast voluntary armies, largely through the genius and energy of Lord Kitchener, were raised and organised; that Italy became associated with us as an Ally; that the Military Service Act was passed into law; that the enemy's cruisers and merchant ships were driven from the seas and his ports blocked; and that by rigorous taxation, as well as the use of our unrivalled credit, we were enabled not only to bear our own burden, but substantially to lighten that of our fellow combatants. Throughout the war, whether in or out of office, I have supported every measure for its efficient and successful prosecution. Hostilities have now been brought to a glorious end, and it is impossible to overstate the decisive importance of the part played in the struggle by our own Navy, our Army , our Air Force, and our Mercantile Marine. We can also look forward with confidence to the complete attainment of the common purpose which I set forth on behalf of the Allies at the beginning of the war, and to the bringing into being of a League of nations, which will, we hope, secure the peace of the world and the reign of international justice and humanity.
+With peace we must set our own hous in order. We must be on our guard to make secure what has already been won. There must be no tampering with the essentials of Free Trade. Self-government for Ireland must be promptly translated from what it is already - a statutory right - into a working reality. Temporary restraints necessary in war upon personal liberty and the free expression of opinion must be removed without delay. The ties which unite us to our fellow-subjects in the great Dominions have been strengthened by our comradeship in the efforts and sacrifices of the war. Peace will bring with it a call and a stimulus to the inter-Imperial development of our common counsel, without any impairment of complete local autonomy. To India we owe an early redemption of the pledges which with the assent of all parties, have been given by the Imperial Government.
+In the field of creative reform at home, social and industrial - our first duty is owed to those who have won us the victory and to the dependants of the fallen. In the priorities of reconstruction they have the first claim, and every facility should be given them not only for reinstatement, and for protection against want and unemployment, but for such training and equipment as will open out for them fresh avenues and new careers. The war has cleared away a mass of obstructive prejudices and conventions, and with peace will come a realisable prospect of a new and better ordered society. Some of the earliest and most practical steps to be taken in regard to land, housing, health, temperance, the future conditions of industry, were recently indicated by me at Manchester. I summed up their general purpose in the following words:-
+'In every chapter of reconstruction I should be prepared to adopt for myself, and to recommend to my friends, as an appropriate watchword the formula of a national minimum. In concrete terms, I understand that to mean that we ought not to be content until every British citizen - man, woman, and child - has in possession or within reach a standard of existence - physical, intellectual, moral, social - which makes life worth living, and not only does not block, but opens the road to its best and highest possibilities.'
+But I am not bound (as none of us should be) to any cut-and-dried programme. I will give wholehearted support, reserving in regard to particular measures complete freedom of judgement and action to any policy from any quarter, Liberal, Unionist, or Labour, which proceeds on these lines, and is animated by this spirit. The best security for the successful prosecution of such a policy is that, in accordance with our traditions, it should be subject to full scrutiny in the free atmosphere of a representative House of Commons. For that purpose it is essential that every elector should claim and should exercise unfettered liberty of choice.</t>
+  </si>
+  <si>
+    <t>The complete collapse of the coalition Government at length gives the Electors an opportunity of pronouncing their verdict upon its performances, and of deciding where to put their trust in the future. For four years the alliance between Mr Lloyd George and the Conservative Party has dominated the affairs of the nation. This combination has now broken up in general confusion and discredit, leaving behind it an unexampled record of extravagance and failure. It must be remembered that both wings of the Coalition are responsible for its misdeeds, and neither can escape its share of public condemnation.
+The circumstances of the Coupon Election were so abnormal that it was easy to be misled by the specious appeal then put forward jointly by Mr Lloyd George and Mr Bonar Law. But the events which have since happened consitute a complete justification of the warning which Liberal leaders then gave that the continuance of Coalition meant the abandonment of principle and the substitution of autocratic for Parliamentary Government.
+It is now universally agreed that what the last House of Commons and the country needed was an opposition strong enough in numbers not only to express, but to make effective its criticisms both of expenditure and of policy.
+Mr Lloyd George and his colleagues have spent as they pleased; their Peace Treaties are impossible of fulfilment; they have shown themselves equally incapable of securing good understandings abroad and of pursuing consistent policy at home. No confidence could be placed in their declarations whether in the industrial or the international sphere.
+The nation demands a complete change - conviction instead of compromise, economy instead of extravagance and waste.
+Now that economy - the supreme need of the nation - has become a popular watch-word, its value is everywhere proclaimed. But the Electors will not be satisfied with the belated and coerced repentance of those who have been responsible for wasteful expenditure in the past.
+The one Party in the State which has consistently fought waste, challenged estimates, moved reductions and stood for economy is the Independent Liberal Party.
+It did so when economy was unpopular, and when the leaders of the late Coalition denied and ridiculed the possibility of retrenchment. The country will judge those who formed and supported the Caolition, not by what they now say, but by what they, when in power, then did.
+The Liberal Party rejoices that there is now general assent to the Irish settlement on the lines of Dominion Home Rule, but it must not be forgotten that for a year the Coalition was engaged in a futile attempt to reduce Ireland to submission by the exercise of undisciplined force. It was the Independent Liberals both in and out of Parliament who aroused the conscience of the country to the criminal folly of such methods, and consistently pressed the policy of conciliation which was too tardily adopted.
+When the late Government led the country into disastrous and costly adventures in Russian and Mesopotamia it was again Independent Liberalism which denounced the recklessness of these enterprises.
+By the terms of the compact which brought it into being the Coalition was bound to make a breach in our Free Trade system. At every stage in the series of irritating and ill-conceived measures which have hampered our industrial recovery during the last four years, it has been Indepenent Liberalism that has fought the battle against Protection and Government interference. What is needed in the new Parliament is the full and effective expression of the Liberal spirit.
+Liberalism is not Socialism. Liberalism repudiates the doctrine of warfare against private enterprise.
+Peace and disarmament made secure through the League of Nations
+The prompt revision and settlement of Reparation and Inter-Allied Debts.
+Drastic Economy in public expenditure and the abandonment of the policy of military adventures abroad.
+Fulfilment by the community of its responsibility for securing the workers against the hardships of unemployment, co-operation between Capital and labour, and honest and fair treatment of organised labour as the only basis of industrial peace.
+Unqualified Free Trade with the immediate repeal of the Safeguarding of Industries Act and similar protective measures.
+The defence of such essential social services as Education, Housing, and Public Health.
+Political and legal equality for women and men.
+A comprehensive reform of the existing Land System, including the Taxation and Rating of Land Values.
+The democratic reform of our Licensing System.
+Re-adjustment of our electoral system by the introduction of Proportional Representation.
+Liberals stand for the nation
+It would be easy to follow the example of others and attempt to purchase electoral support by displaying a long series of glittering promises. But the country has too much reason to know the difference between promise and performance, and the simple truth is that great and necessary schemes of social reform, involving large outlay of public money, cannot be realised unless and until real Peace has been established by a foreign policy based upon and conceived in the spirit of the League of nations and National Finance is placed upon sure foundations by a course of rigorous economy. By these means, and by these means alone, can prosperity be promoted, employment assured, and taxes lightened.
+The essence of the Liberal spirit is that it sets the well-being of the community as a whole above the interests of any particular section of class. It is this spirit which distinguishes Liberalism from any other political party which is now appealing for electoral support. The moment has come to restore Liberalism to its rightful place in the councils of the Nation.</t>
+  </si>
+  <si>
+    <t>The Government, elected twelve months agon on a programme of five years of tranquility, has suddenly decided to plunge the country into the turmoil of a General Election, on the allegation - unproved and unproveable - that Tariffs are a cure for unemployment. The Prime Minister has deliberately chosen the earliest possible date for the Polls in order to avoid informing the House of Commons, and through the House of Commons the country, as to the reasons and the scope of his proposals. Tory Ministers profess that they are driven to this precipitate action by a sudden inspiration concening unemployment, and hope to stampede the country by reviving the musty war-cry that Tariff Reform means work for all.
+There is one explanation and one only, for the course which the Government have pursued. It is that in a single year their conduct of foreign policy in great matters essential to our livelihood has signally and disastrously failed. By their own declarations, repeatedly made, the first condition of our recovery is the restoration, not merely of the home market, but of world trade. By their own declarations in Despatches, addressed to our Allies, the growing collapse produced by French policy in Germany, and the reaction of that policy upon trade and credit, throughout Europe, are the main cause of the distress in which our trade is plunged. For at least a century past, no greater economic, political or moral question has confronted Europe than the French and Belgian occupation of the heart of Germany industry in the Ruhr. In no great European question, for at least a century past, has it ever been doubtful where Britain stood. Yet for a whole year neither our Allies, nor Neutral Powers, nor our late enemies, have known whether in this crucial issue Britain had a voice or mind or conscience of her own.
+In January the Government refused to associate the country with the occupation of the Ruhr; but for months they half condoned it and waited on results. Only when its falure was becoming manifesto did they declare their view, held apparently since January, that the invasion was a breach of the Treaty of Versailles. In December of last year the American Secretary of State, Mr Hughes, offered American co-operation in an impartial investigation of Germany's capacity to make reparation for damage done in the war. The British Government took no steps for nine whole months to urge acceptance of this offer upon our Allies. In June Germany put forward proposals, largely on Lord Curzon's prompting, for meeting the Allies' demands. The British Government declared, quity properly, that these proposals called for reply. Five months have passed, and no reply has ever been made. British policy was one of the chief rallying powers in Europe after the Napoleonic wars. For the past year its blindness, indecision and impotence have been such that it has ceased to exercise any guiding influence upon European affairs.
+In Eastern policy the tale has been the same. It was not enough that we should abandon all for which we fought against Turkey in the war. By the shameless Treaty of Lausanne we have also surrendered all the securities for British commerce in Turkey which we enjoyed before the war. By the policy which we have followed British trade in Turkey is practically at an end. Our weakness has been noted elsewhere, and a similar fate now threatens our hold on valuable markets in the Far East.
+By moral indecision, by divided counsels, and by diplomatic incompetence, the Government have failed in Europe and Asia alike, to make one single effective effort to assert our rights, to restore our trade, or to bring back peace and order to a distracted world.
+Every serious observer of contemporary affairs knows that Liberal criticism of this policy during the Parliament now dissolved was abundantly justified. Our warnings were left unheeded, and the inaction of the Government has been a potent contributory cause of unemployment at home.
+Liberal policy stands for the prompt settlement of Reparations, with due consideration for the position of inter-allied debts, and for an earnest endeavour to co-operate with the great American Commonwealth in bringing peace to the world. Liberals hold that the economic restoration of Europe is the necessary condition of the revival of our industries and the establishment of peace. They would welcome the reopening of full relations with Russia.
+The whole force of the Liberal Party will be thrown into the support of the League of Nations. Our foreign policy should aim at making full use of the League, and enlarging its scope and power, until all nationsl are included within it, and at substituting international co-operation for the perpetuation of national enmities and the piling up of the means of destruction.
+But the return to noraml economic conditions must take time, and in the interval unemployed men and women cannot be left to await better times with no prospect but unemployment benefit and Poor Law relief. The schemes of the Government are totally inadequate.
+Trade restrictions cannot cure unemployment, Post-war conditions do not justify such restrictions; they merely render it more disastrous. High prices and scarcity can only lower the standard of living, reduce the purchasing power of the country, and thereby curtail production. An examination of the figures shows that the suggested tariff cannot possibly assist those trades in which unemployment is most rife. The last thing which taxation on imports can achieve is to provide more work for those engaged in manufacture for export.
+Mr Baldwin asks for a blank cheque, and if he is wrong the country must take the risk. He offers no evidence. He formulates no scheme. In the face of declarations made last year by prominent Tariff Reformers like Mr Bonar Law and Mr Austen Chamberlain, that after-war conditions make proposals for Tariff Reform inopportune and injurious, he asks for power to tax an undefined number of commodities, without any disclosure of the scale or range of the duties, or the industries to be disturbed.
+The Liberal Party is equally convinced that the remedies recommended for unemployment by the Labour Party - Socialism and the Capital Levy - would prove disastrous. What is needed is not the destruction of enterprise but its encouragement; not the frightening away of Capital but its fruitful use.
+The Liberal Party is not content with criticising the proposals of others. The country has made enormous sacrifices to restore the national credit. A bold and courageous use should be made of that credit on enterprises that would permanently improve and develop the home country and the Empire; such as internal transport by road the water, afforestation, the supply of cheap power secured by the co-ordinated used of our resources of coal and water, reclamation and drainage of land, the development of Imperial resources especially in our Crown Colonies, railway building in the Dominions and India, the facilitation of overseas settlement under the British flag, cheapening the means of transport in order to develop inter-imperial trade, and a freer use of the provisions of the Trade Facilities Act.
+The Liberal Party proposes thoroughly to remodel the Insurance Acts with a view to providing benefits sufficient to allow a reasonable subsistence to a man and his family without aid from Poor Law Relief. The Poor Law Authorities should not have to bear a burden which ought to be regarded, not as a local, but as a national charge.
+The Liberal Party will take all possible steps to promote the co-operation of employers and employed. The worker should be secured a proper status and a fair share in the produce of the industry in which he is engaged. Liberal industrial policy is based upon the principles of partnership between Labour and Capital, security of livelihood for the worker, and public advantage before private profit.
+Women electors should be among the first to recognise and resist the Protectionist attack on the standard of life of the porrest homes in the country. Of all sections of the community they are in the closest and most intimate contact with prices, and no one will suffer more from Tariffs than the Chancellor of the Exchequer of the home. Liberals aim at securing political, legal, and economic equality between men and women. Mothers and Father should have equal rights and responsibilities in the guardianship of their children.
+The thrift disqualification attached to Old Age Pensions should be immediately removed. Liberal policy concentrates upon lifting from the homes of the poor those burdens and anxieties of the old, the sick, and the widow with young children, which the community has the power and duty to relieve.
+The needs of British Agriculture require special consideration. Import duties on what the farmer buys can only further injure his position. British Agriculture requires a free hand, stability of prices, greater capital resources, security of tenure, adequate means for preventing the exaction of unfair and uneconomic rents, and improved transport. Credit facilities for the farmer, and co-operative marketing on a large scale with Government assistance, which has so successfully helped American agriculture over a great crisis, can also be applied in our own country. Opportunity should be given for the cultivator to become the owner of his own land on reasonable terms by a system of land purchase. A free man on his own land, whether as farmer or smallholder, has always proved the most successful and energetic of producers. Small holdings and allotments should be developed and encouraged.
+The agricultural Labourer is engaged in a skilled industry of cardinal importance to the nation, and ought to be adequately remunerated. The State must recognise that the conditions of his work make it vital to secure that his standard of life should be raised, his housing vastly improved, and the amenities of rural life enlarged. Every opportunity should be given to him and his children to improve their position on the land which he has cultivated for so long.
+Unemployment is also caused by over-taxation and wasteful administration. There is urgent need and abundant scope for retrenchment in the expenditure of the taxpayer's money in some departments of public service. The Liberal Party draws a sharp distinction between the use of the National revenue for purposes which add to the wealth and comfort of the people as a whole and the waste of public money in directions which are unproductive or destructive. Liberals will be no parties to the starvation of, or to false economies in, Education. They believe that no better investment of National Wealth can anywhere be found than in developing the faculties and intelligence of the youth of the country.
+For the same reason, Liberal Policy centres upon the promotion of all those things which build up the home - housing, temperance, child-welfare and other social services.
+The rapid and adequate provision of Housing Accommodation is an urgent public duty. It should be treated, not as a local, but as a national problem; and until the present shortage has been overtaken, there should be no decontrol of rents.
+The excessive consumption of alcoholic drink is one of the main causes of unemployment, disease, and poverty; and the right of the citizens of a locality to decide for themselves the drink facilities in their own area should no longer be withheld.
+Reforms in local government and rating are long overdue. For some years the Poor Law system has been ripe for legislative revision. The overlapping of Insurance, Old Age Pensions, and Poor Law Relief requires immediate action. The present rating system discourages improvement and penalises those who create industries or provide houses; it must be so altered that as great a part of the burden of rates as is practicable is transferred to those who benefit most by the efforts of the community, namely, the owners of the site value.
+The dweller in the town, like the dweller on the land, should be entitled, if he so demands and his terms are fair, to become the owner of his factory, shop or home. Lease-hold enfranchisement has long been an object of Liberal policy. It is time that it became the law of the land.
+Mr Baldwin's sudden plunge has thrown his own supporters into confusion and has firmly united the Liberal Forces. The country has now the opportunity of overthrowing a Government whose record is one of unrelieved futility, and of calling for an alternative administration, which will pursue Peace and Reconciliation abroad, Social and Industrial improvement at home, and which is definitely committed to the defence of Free Trade as the best basis upon which to rebuild the life of the Nation.</t>
+  </si>
+  <si>
+    <t>The country has been plunged into a General Election for the third time in two years. This election has been forced on us by the Labour Prime Minister and his Government for two reasons.
+First, they were not prepared to face an impartial enquiry into the circumstances which led to the withdrawal of a prosecution against a Communist writer for inciting to mutiny in the Navy and Army. Next, they wished to evade Parliamentary discussion of a reckless propsal to guarantee, at the risk of the British taxpayer, a loan to the Communist Government of Russia.
+The Liberal Party in Parliament, whilst they have rejected crude schemes of 'Nationalisation' promoted by the Labour Party, have assisted the Government in every move made by it towards sound social reform, and they regret that the efforts of the Ministry in that direction have been so halting, ineffective and unimaginative.
+They have pressed the Government week by week to fulfil its pledges to provide work for the unemployed by schemes of National Development, in order that we might be adequately equipped to meet the competition of our trade rivals. They have urged that the credit of the nation should be used in permanently improving and developing the Home County and the Empire, such as Power Supply, Afforestation, Reclamation and Drainage of Land, Overseas Settlement under the British flag and development of the Empire's resources. The Government has taken no definite or effective action in these matters.
+They have pressed the Government repeatedly to fulfil their election promises to the Ex-Service men, the War fighters in the Civil Service, the ex-ranker Officers and others; again without result.
+The Liberal Party are in full sympathy with all efforts for mutual disarmament and for the promotion of international peace. But they have been unable to prevent the Government increasing Military Estimates by twelve million over the expenditure of last year, or starting a naval race in the building of new cruisers.
+The Liberal Party is in favour of re-establishing economic and commercial relations with the Russian people. But at a time when every nerve should be strained to re-establish British credit and equip British industry for the recovery of foreign trade, the Labour Ministry has undertaken to recommend Parliament to ratify a Treaty which contemplates that the British taxpaer should guarantee a loan to a Government whose principles deny the obligations which civilised nations regard as binding between borrower and lender. This was done shortly after the Prime Minister had declared in the House of Commons that only credulous people would believe that he would countenance such a procedure.
+In 'Labour's Appeal to the Nation', the manifesto on which the Labour Party fought the last Election, the confident assertion was made that the Labour Party alone had a positive remedy for unemployment. The country has waited in vain for this remedy to be produced, let alone applied. Unemployment is more serious now than when the Government came into power. At that time the number of unemployed persons was 1,153,600. The most recent Return, that of September 29th this year, shows that the number of unemployed has swollen to 1,198,800, and it is still increasing. The Government's policy on this vital question has been one of drift and indecision. Nothing new and effective has been done, and their profuse electoral promises remain to this day unredeemed.
+It has long been obvious that the solution of the Housing Problem depends mainly on a sufficiency of skilled building labour being made available. Mr Wheatley's Housing Act professed to deal, specifically with this part of the problem. But no effective measures have been taken to train young apprentices, or otherwise to increase the number of building craftsmen. Instead of its being possible to say that under the Wheatley Act progress in house building has been made, the fact is that fewer houses are now being begun than when the Government came into office. The Liberal policy on housing is to insist that the reserve of unemployed labour should be utilised to build houses for the people.
+Liberalism, in pursuance of its historic role of giving equal opportunities to all classes, and of creating the fundamental conditions of economic and political freedom, has a special responsibility for promoting and carrying through great policies of land reform.
+The long-standing neglect of agriculture in Great Britain must be redressed. Real improvement cannot be achieved either by fantastic schemes for setting officials to control all imported and home-grown food, or be impracticable and mischievous measures for taxing imported food. It can be achieved only be securing to land workers the fruits of their energy and enterprise through a complete alternation in the system of land tenure. That system must be modified in accordance with modern necessities. The Liberal land policy contemplates a land tenure which would combine the advantages of ownership and of tenancy without the disadvantages of either. On the basis of this reform can be built a coherent scheme of agricultural credit with the assistance of the State, of businesslike marketing of produce, of co-ordinating transport services, of draining and reclaiming land for productive uses.
+The Liberal policy is to liberate farmers from the restrictions of an out-of-date land system; to liberate agricultural labourers from poverty and lack of opportunity; and to make the best use of all the land of the country in the interest of the whole community.
+A large section of our town dwellers have neither room to live nor room to work, nor room to play. Many of the evils of town lief are the result of allowing private owners of land to hold up growing towns by withholding land from use, and selling it yard by yard at exorbitant prices. The Liberal land policy for the towns is to enable towns to assert their rights, to undo the results of past neglect, and to create the conditions necessary for the health of town workers and the efficiency of industry. Land Values, created by the activity and expenditure of the community, must be made to contribute to the expenses of maintaining the conveniences, utilities, and amenities of the town. The degradation and disgrace of our slums must be wiped out, and facilities for all classes of the population to get access to the fresh air and open spaces provided. The leasehold system, which allows landowners to take for themselves the fruits of traders' enterprise, must be reformed. Occupiers of dwelling houses held on lease must be given the right to purchase their freehold at a price which will not confiscate the investment made in building or buying their homes. Occupiers of shops and business prmises on short leases must be enabled to obtain from a Land Court compulsory orders for the renewal of their leases on fair terms. In order to control effectively their future development, towns must be given powers to acquire at fair prices all land likely to be required in the future for housing, open spaces, and other purposes connected with the health and welfare of their population. The radical cure of slums by building new Industrial Towns, planned from the beginning for healthy living, comfort, amenity and efficient industry, must be taken in hand, and there as elsewhere all increments in value created by the community secured by it.
+The hindrances to national prosperity imposed by our present system of land tenure particularly obstruct the development of the great industry of coal mining. Largely owing to the land system our coal resources are wastefully used and wrongly applied. Nothing is more urgent in the national interest than to bring permanent peace to our coal fields, and so to use our coal as to make it a far greater source of wealth and power.
+The coal problem is intimately linked up with the power problem, since power is coming more and more to mean electrical power, in generating and distributing which we are falling far behind our leading competitors. The Liberal policy is to make coal what it ought to be and is in many other countries - a great national asset - by empowering the State to acquire all mineral rights, and to provide State assistance and direction in the building of super-power stations. By a levy on the purchase price at which mining royalties are taken over by the State, funds will be provided for rebuilding and bettering the mining villages, many of which are a disgrace to the country and a standing menace to the peace and efficiency of the industry.
+The Liberal Party has worked out a ten years' programme of educational advance. If it comes into power it will wipe out the arrears of educational reform which have accumulated in unprogressive areas; it will get rid of the worst buildings, and will reduce the size of the classes in Elementary Schools. It will effect much-needed reform in Rural Education and improve the qualification of teachers. With special concern for young workers in and out of work, and for more Secondary Schools, it will press for large additional provision for pupils over 14 years of age with maintenance allowance in suitable cases. It will extend provision for University Education, and, as regards Technical, Evening and Adult Education, it will seek to collaborate with employers and employed in making a determined effort to increase the efficiency of all schools which prepare the youth of the nation for their vocation in life and fit them for their responsibilities as future citizens. It recognises that the fulfilment of these aims demands such conditions of service and such payment of teachers as shall secure a constant and increasing supply of properly qualified men and women, and believers that satisfactory conditions as regards remuneration can best be secred by national agreement.
+The Liberal Party hold unshakeably by its policy of Free Trade. The country gave its verdict a year ago on the policy of Protection, and it may safely be trusted in the present election to give an equally decisive verdict on the Labour Party's policy of Controls and Shackles.
+The alarming increase in recent years of industrial disputes, unless arrested, will inevitably destroy our supremacy in the markets of the world.
+The Liberal remedy is the co-operation of all engaged in industry - investor, manager, workman - and the fair distribution of its profits amongst all engaged in it. It is by co-operation and goodwill, and not be Socialism, that prosperity can be restored to British Trade and better wages and security of employment obtained for British Workmen.
+A further extension and a complete co-ordination of the Insurance Acts, which were initiated by the Liberal Party before the War, is now a matter of urgent national necessity. The Liberal policy is that the various schemes of social and economic insurance which are now in operation should be so amended and consolidated as to make certain that the benefits provided shall afford a man and his family a reasonable subsistence, without the necessity for applying for relief from the Porr Law. Old Age Pensions must be freed from the disqualifications attaching to thrift. Pensions for widows and allowances for orphans during their schools life must be provided. Breadwinners breaking down in health before the age of 70 must be assured of support outside the Poor Law. All this must be carried out by a comprehensive policy of contributory insurance, maintaining self-respect and giving to all citizens security against destitution.
+One of the gravest social problems of the day is that of the excessive consumption of alcoholic liquor. It ought to be dealt with, in the light of experiments made at home and abroad, on bold and democratic lines. Here, too, the record of the Government is utterly disappointing. Its attitude to temperance legislation is illustrated by the rejection through Labour votes of the temperance proposals put forward by Welsh Liberal members. This shows how little faith can be placed in the professions which the Labour Party made while in Opposition, but are either unable or unwilling to fulfil when in power.
+The existing machinery for expressing in Parliament the will of the people is delusive and misleading. It is apt to give a decisive majority in Parliament to a pronounced minority of votes in the country. In the last three elections it worked out unequally and unfairly. It is imperative that effective steps should be taken to secure a real correspondence between Parliamentary representation and electoral strength.
+In placing Labour in power, Liberalism followed constitutional usage. In voting against the Government, Liberalism has consulted the deepest interests of the country's security, credit and good government. The people have now a choice to make between three parties. They have an opportunity of putting in power a Liberal Government which will pursue the path of Peace, Social Reform and National Development, avoiding, on the one hand, unthinking resistance to progress, and, on the other hand, unbalanced experiments and impracticable schemes which will destroy the whole social and economic system upon which the prosperity of this country has been built.</t>
+  </si>
+  <si>
+    <t>The General Election now in progress will have an important and in some respects a decisive influence on the well-being of this great country. The by-elections of the last two years have made it abundantly clear that the nation has lost confidence in the present Government. Its complete failure to grapple with the serious emergency in our trade and the consequent abnormal unemployment has created a general sense of disappointment in all classes of the community. Even Conservatives do not conceal their disillusionment with the Government they succeeded in placing in power five year ago. Whatever the result of this election may be, it is clear that the supporters of the Government will be in an emphatic minority in the next Parliament.
+The issue, therefore, for the electors is whether they will entrust the destinies of the country to the Liberal Party, which can show a long record of great and enduring service to the nation, and which can command today amongst its leaders a number of able and experienced men, who in some of the highest offices of the State served their country well, or to the Socialist Party, which, apart altogether from being inexperienced, is committed to proposals which would be disastrous to the trade, commerce, and industry of the land. Reports come in from every part of this island which indicate a sensational revival of the trust in Liberalism and a general desire to see the affairs of the nation once more placed in the hands of a Liberal Administration.
+For the twelfth time I solicit the suffrage of my fellow-electors of Caernarvon Boroughs. Having represented them in the House of Commons continuously since 1890, I need enter upon no elaborate explanation of my political opinions. On all such matters as the urgent importance of restoring agriculture to its proper position in the economy as the urgent importance of restoring agriculture to its proper position in the economy of the nation, the vital need for ampler facilities for education, the temperance question, housing, and the complex problem of giving security, leasehold enfranchisement, opportunities, and independence to the poorer and less fortunate sections of the community, the importance of Empire development, and certainly not lease the fair treatment for all questions specially affecting Wales, her language, and her people, my views are well known to you. In this election I only want to stress what seems to me to be major issues which call for urgent treatment.
+The greatest world issue before the country today is peace. Everybody wants peace and talks peace, but the acid test of whether covenants, treaties and pacts of peace mean anything, and whether the Government has confidence in the League of nations, in the Kellogg Pact, in the Washington Treaties they will cut their vast and swollen armaments to the police level. If they continue to spend money on armaments and organise conscript nations in arms, it is becuase they really reust not in peaceful methods, but in war. We are spending £112,000,000 a year on armaments and little more than £100,000 a year on the League of Nations.
+My first object, if elected to the new Parliament, will be to urge that immediate steps be taken to give a practical response to the offer, made by President Hoover in his inaugural address, to co-operate with other nationsl to bring about that large and simultaneous reduction of armaments which is the only sure protection against war, and the only sure foundation for peace. A conference of nations to discuss measures that will lead to drastic reduction in these increasing armaments should be immediately summoned.
+The central domestic issue which confronts us is unemployment. There can be no national health, no widespread prosperity, there can be no national happiness and contentment so long as more than a million of our fellow-countrymen are unable to find work and earn wages by their work. The nation ought, and will rally to whatever party can give grounds for believing that it can get rid of this running sore from the body-politic.
+The Liberal Party has not simply made election promises. As a result of the only thorough and consistent study which has been given to our national problems during the last few years by some of the ablest economic experts, aided by experienced business men, it has produced a sound, safe, practical programme for every elector to judge for him or her self.
+Last February the Prime Minister stated in the House of Commons that 'in the view of the Government the object which we desire can best be attained by perseverance in our policy', by perseverance, that is to say, in a policy which has resulted in unemployment being substantially the same as it was when they came into office in 1924. The Labour Party policy was recently announced by Mr Ramsay MacDonald at the Albert Hall. If they are returned to power they will appoint another committee.
+The Liberal policy is a practical policy. In the first place it seeks to restore the prosperity of our industries by breaking down the barriers to international trade, by promoting harmonious relations between employer and employed, by encouraging in every way greater efficiency in industry, and by restoring the Trades Facilities Act, which gave the support of the national credit to industrial enterprise of a substantial and valuable kind and which could not be initiated or carried out without special assistance. Before the Act was abandoned by the present Government, enterprises of the aggregate value of £74,000,000 were put through at an infinitesimal cost to the Treasury.
+In the second place, it pledges itself to find immediate employment for those now out of work on works of national utility and development, many of these works, like electricity, telephones, housing, roads, and railways, being long overdue. It is surely better, instead of wasting our substance by spending £70,000,000 a year on 'doles' for which there is no return, to lay out this enormous expenditure in providing work on plans which will leave the nation richer and more efficient for its tasks. The details of these plans are set forth in the liberal pamphlet 'We Can Conquer Unemployment', and need not be repeated here.
+I shall continue my life-long opposition to the policy of raising prices at home and impeding foreign trade by Protection, Freer trade for all nations is the only road to national, Imperial, and international prosperity.
+The Liberal programme deals with the immediate and ultimate needs of the nation. Its watchwords are the restoration of prosperity to our industries; the conquest of unemployment; the cutting down of unproductive expenditure; temperance reform; the completion of proper housing for the people; slum clearance; revitalisation of agriculture; the emancipation of the leaseholder from harse and unjust conditions that confiscate his capital and toil; a great expansion of education; vigorous national development of the resources of the country; Imperial unity; the devolution of purely national questions within the nation to the nationalities concerned; freer trade; international peace by the substitution of arbitration for force, and all-round reduction of armaments.
+It is on this programme that I confidently seek re-election.</t>
+  </si>
+  <si>
+    <t>The country is faced by an economic crisis of great gravity. Not only has Britain been driven off the Gold Standard, but almost every other nation is reeling under the strain of an unparalleled depression.
+Nothing save the highest statesmanship can steer the world back to normal conditions and prevent disasters of the greatest magnitude.
+The Liberal Party held that the Government and Parliament should devote themselves to the vast and urgent tasks that faced them, without a General Election at this time. But the Prime Minister has decided to appeal to the country for a mandate to carry through whatever measures may be found to be needed to deal with the emergency, and the electorate is now called upon to give its judgement.
+In these circumstances, the Liberal Ministers have felt it their duty to co-operate with the Prime Minister in maintaining a strong and stable Government composed of men of all parties.
+The situation today is not less critical than it was when the National Government was formed. Despite the fact that the Budget has been balanced, the nation has gone off the Gold Standard, and the effects of this on national and international credit, and on the cost of our food and raw materials, have yet to be fully felt.
+The vital need of today is to avoid any inflation of the pound, which would mean a rapid fall in the purchasing power of money, the loss of savings, large and small, and a general lowering of the standard of life of the whole community.
+Common action by the countries of the world is urgently required to stabilise currency, to deal with the international debts and reparations, and to make a powerful effort to secure a lowering of the tariff barriers to trade which are without doubt one of the principal causes of the universal depression and unprecedented unemployment.
+At home it is imperative both to keep the Budget balanced and to secure a favourable balance of trade, by whatever methods, whether related to currency, to the expansion of exports or the restriction of imports, which might be found to be necessary and effective for that purpose. At the same time, energetic action should be taken to promote industrial and agricultural development, with a view to increasing the production of foodstuffs at home and the export of manufactured goods abroad.
+The Liberal Party goes to the polls as the vigorous advocate of those Liberal aims and ideals which have rendered the highest service to the country and to the Empire. We are strongly of opinion that no issues of controversy between the parties supporting the Government should have been introduced at this election.
+Having regard, however, to pronouncements that have been made, we feel bound to declare our view that whatever emergency measures might be found to be necessary to deal with the immediate situation, freedom of trade is the only permanent basis for our economic prosperity and for the welfare of the Empire and of the world. Protection has not saved those countries which have adopted it from more acute unemployment than ourselves.
+Taxation on the staple foods of the people has always been opposed by the Liberal Party and would lay fresh burdens on those least able to bear them.
+The abandonment by Great Britain of her free trade policy would aggravate the divisions between nations and would check the growing realisation throughout the world of the disasters towards which they have been leading mandkind.
+It is profoundly to be regretted that the financial difficulties of this time have put a check upon measures of social reform and of national development, and have demanded severe sacrifices from the whole nation.
+Liberalism, which for generations has played a leading part in the effort to raise the standards of life of the people, and which still stands as the principal bulwark between the country and a disastrous conflict between classes, deeply deplores these events.
+but it sees in the maintenance of sound finance, which is the condition of the restoration of industry and commerce, the indispensable steps to the lessening of unemployment and to the resumption of social progress.
+Despite the professions in the recent declaration of the Labour Party that it would wish to balance the Budget and to prevent inflation, the programme of expenditure to which that party has now committed itself must defeat both those aims and lead to financial disaster.
+The conditions of the present Election are one more proof of the imperative need of a reform in the electoral system if the real wishes of the voters are to be truly expressed at the polls.
+To safeguard international peace, to maintain and increase the strength of the League of Nations, and to promote the success of the forthcoming Disarmament Conference are among the price purposes to which the nations should address themselves. The development of responsible government in India through the Round Table Conference is also of the highest importance.
+It is an independent party, standing with undiminished conviction for those causes of individual and national liberty and social progress with which liberalism has always been identified, forming a barrier against both reaction on the one hand and rash and injurious changes on the other, but co-operating now with the Prime Minister in dealing with the crisis which is upon us, that the Liberal Party appeals to the nation.
+It asks that the electorate shall use its power to ensure that liberal ideas shall have a powerful expression and an effective influence both in the Government and in the coming Parliament.</t>
+  </si>
+  <si>
+    <t>A General Election is being held at a moment of acute international crisis. After long delay the Government have lately been taking definite action at Geneva. All parties support the action. An election is therefore unnecessary.
+Upon the success or failure of the League of nations in its effort to penalise aggression must depend our own future policy, in foreign affairs and as to armaments. If the League succeeds we shall take one course; if it failes, another. The issue is now in the balance. Until we know we cannot judge. This is precisely the moment when the nation ought not to be asked to give a mandate on these matters for the next five years.
+Our aim is to maintain the peace of the world and preserve our own security. Armaments, on however vast a scale, will not bring security or stop war. The national defences must be kept efficient and large enough for the needs of the times, but a colossal, panic expenditure upon arms is not the road to peace. It is the duty of the House of Commons to examine, upon their merits and with the utmost care, all demands for increased expenditure, especially upon armaments, and to insist upon the strictest control of their manufacture and sale, and the elimination of the motive of private profit. It is the duty of the voters to elect a House of Commons that will do this. Through strengthening the League of nations, and through international disarmament, and there alone, the true path to security lies.
+Liberals are convinced that a change in the policy adopted in this country during the last four years is essential if the poverty and distress so widely prevailing are to be ended, and if the peril of war which overhands the world is to be removed. The continued un-employment of 2,000,000; the unrelieved misery - of the depressed areas; the low wages of the miners, of the farm workers, and of many others; the immensely reduced figures of our export trade compared with a few years ago; the plight of our shipping industry - all point to a wrong policy. And the unrest in the world is due chiefly to the hard struggle of some of the great Powers to keep their peoples in proper comfort. All this comes from the diastrous reduction in the volume of world trade. And that is due to the restrictions imposed by Governments. The present Government in Great Britain has been among the most active in increasing these restrictions. While rendering li-service to greater freedom of trade, and entering into some agreements with other countries for trifling reductions here and there, its actions on the whole have immensely increased the obstacles with hamper world commerce. The Ottawa Agreements - now repudiated by the Canadian people - were among the most disastrous. It is urgently necessary that there should be a change, if our unemployed workers are to be brought back into employment, and if the sources of world unrest, threatening war, are to be removed. To rid commerce of the hindrances that come from tariffs, quotas, subsidies, and unstable currencies is the first step to a restored prosperity and a more tranquil world. The Liberal Party alone has continously urged the vital importance of this issue. It alone can be trusted to press it forward to a solution.
+Liberals stand for a vigorous sustained policy of national development. They have long advocated the employment of idle capital and idle labour upon a great number of enterprises, which are urgently needed - for the housing of the people, the expansion of industry and agriculture, and the better equipment of our country. The present Government has stubbornly rejected that policy.
+The Liberal Party condemns the Means Test regulations. It considers that to treat the 'household' as a unit is wrong. The Government has dissolved Parliament without issuing the revised regulations promised eight months ago, and so has refused to submit them to the judgement of the electorate. It ought not to be given a free hand to settle this matter as it chooses in the next Parliament.
+The Liberal Party has laid before the country a wide and detailed programme, dealing with the organisation of industry and the status of the worker; with the ownership and use of land, the securing for the public benefit of the land values created by the public, the development of agriculture, the reforms that are essential in the coal industry; with the raising of the school age and a great expansion in our educational system; with the inclusion of other classes in National Insurance; with housing, temperance, the extension of leisure, and greater facilities for its use.
+The Liberal Party stands, as ever, for personal and political liberty. It has fought against the many encroachments upon freedom which have been made in recent years. It opposes the withdrawal from Parliament of proper control over unemployment assistance, and will not cease to resist the constant attempts to transfer powers from representative bodies to irresponsible boards. It will always strenuously defend democratic institutions against the attacks of Fascists or Communists or others in other parties who set small store by liberty. In order to raise the authority of the House of Commons it would reform our defective and unjust electoral system, and through proportional representation, enable the true desires of the people to be expressed in Parliament.
+It would give the same rights to women as to men throughout the political and social system.
+Liberals do not recognise the present Administration as a 'National Government'. A truly National Government is one that is supported by all parties and approved by the nation in general. No party supports the present Government except the Conservative. In the by-elections only one elector in three votes for it. Liberals see in the sudden dissolution of Parliament at this moment as an attempt to use the international situation as a means of securing another lease of power for the Conservative Party.
+We appeal to the nation to ensure in the next House of Commons an effective representation of Liberal opinion. We think it of vital importance that the existing Conservative Government, for such in effect it is, should not be left in a position of uncontrolled authority. And it is no less essential in the national interest that, when it leaves office, the only alternative should not be a Socialist Party pledged to a reckless scheme of wholesale nationalisation. We present to the electors in the Liberal policy here outlined, and we claim for it the active support of all who endorse its general aims and approve its specific proposals.</t>
+  </si>
+  <si>
+    <t>Keir Hardie</t>
+  </si>
+  <si>
+    <t>George Barnes</t>
+  </si>
+  <si>
+    <t>Arthur Henderson</t>
+  </si>
+  <si>
+    <t>William Adamson</t>
+  </si>
+  <si>
+    <t>Ramsay Macdonald</t>
+  </si>
+  <si>
+    <t>http://labourmanifesto.com/1906/1906-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://labourmanifesto.com/1918/1918-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>This election is to decide whether or not Labour is to be fairly represented in Parliament.
+The House of Commons is supposed to be the people's House, and yet the people are not there.
+Landlords, employers, lawyers, brewers, and financiers are there in force. Why not Labour?
+The Trade Unions ask the same liberty as capital enjoys. They are refused.
+The aged poor are neglected.
+The slums remain; overcrowding continues, whilst the land goes to waste.
+Shopkeepers and traders are overburdened with rates and taxation, whilst the increasing land values, which should relieve the ratepayers, go to people who have not earned them.
+Wars are fought to make the rich richer, and underfed schoolchildren are still neglected.
+Chinese Labour is defended because it enriches the mine owners.
+The unemployed ask for work, the Government gave them a worthless Act, and now, when you are beginning to understand the causes of your poverty, the red herring of Protection is drawn across your path.
+Protection, as experience shows, is no remedy for poverty and unemployment. It serves to keep you from dealing with the land, housing, old age, and other social problems!
+You have it in your power to see that Parliament carries out your wishes. The Labour Representation-Executive appeals to you in the name of a million Trade Unionists to forget all the political differences which have kept you apart in the past, and vote for [candidate name].</t>
+  </si>
+  <si>
+    <t>The Labour Party has left the Coalition, and is appealing to the men and women of the country with a programme that is a challenge to reaction.
+Victory has been achieved, and Labour claims no mean share in its achievement. Not only have the workers supplied the vast majority of our soldiers and sailors, and sustained the burden of war at home; the democratic diplomacy which found expression in the War Aims of Labour has been one of the most powerful factors in winning the war, and must be the most powerful factor in the rebuilding of the world. The Peace which Labour demands is a Peace of International Co-operation. It declares absolutely against secret diplomacy and any form of economic war, and demands, as an essential part of the Peace Treaty, an International Labour Charter incorporated in the very structure of the League of Free Peoples.
+Labour welcomes the extension of liberty and democracy in Europe. It has warned the Coalition that opposition towards the young democracies of the Continent, and especially that intervention on the side of European reaction, will be disastrous. Labour demands the immediate withdrawal of the Allied forces from Russia. In the interest of world-democracy it stands for the immediate restoration of the Workers International.
+The principles which Labour acclaims as Allied war aims it will apply to our own subject peoples. Freedom for Ireland and India it claims as democratic rights, and it will extend to all subject peoples the right of self-determination within the British Commonwealth of Free Nations. Labour's appeal to the people is not a sectional appeal, unless an appeal which excludes only militarists, profiteers, and place-hunters be regarded as sectional. It includes all who are determined that the fruits of victory shall not be wasted in the interests of riches or reaction. Especially does Labour appeal to two sections of the community - to the soldiers and sailors who have fought the nation's battles abroad, and to the men and women workers at home.
+The returning soldier or sailor will find himself once more a worker. His cause is one with that of the workers at home. Civil and industrial liberties have been largely suspended during the war; and soldier and worker want their liberties back now. The Labour Party stands for the destruction of all war-time measures in restraint of civil or industrial liberty, the repeal of the Defence of the Realm Act, the complete abolition of Conscription, and the release of all political prisoners. It stands for free citizenship, a Free Parliament, for Free Speech, and against the domination of the Press by sinister political influences.
+The Labour Party means to introduce large schemes of land reorganisation, and it is fully aware that this can only be done in the teeth of the most powerful vested interests. land nationalisation is a vital necessity; the land is the people's and must be developed so as to afford a high standard of life to a growing rural population not be subsidies or tariffs, but by scientific methods, and the freeing of the soil from landlordism and reaction.
+Labour demands a substantial and permanent improvement in the housing of the whole people. At least a million new houses must be built at once at the State's expense, and let at fair rents, and these houses must be fit for men and women to live in. Labour will press for a really comprehensive Public Health Act co-ordinating all health authorities, based on prevention rather than cure, and free from servile or inquisitorial features. It will also press for real public education, free and open to all, with maintenance scholarships without distinction of class, and for justice to the teachers, upon whom education finally depends.
+Labour will resist every attempt to place burdens upon the porr by indirect taxation. Labour is firm against tariffs and for Free Trade. The way to deal with unfair competition of imports made under sweated conditions is not by tariffs, but by international labour legislation, which will make sweating impossible. In paying the War Debt, Labour will place the burden on the broadest backs by a special tax capital. Those who have made fortunes out of the war must pay for the war; and Labour will insist upon heavily graduated direct taxation with a raising of the exemption limit. That is what Labour means by the Conscription of Wealth.
+In industry, Labour demands the immediate nationalisation and democratic control of vital public services, such as mines, railways, shipping, armaments, and electric power; the fullest recognition and utmost extension of trade unionism, both in private employment and in the public services. It works for an altogether higher status for labour, which will mean also better pay and conditions. The national minimum is a first step, and with this must go the abolition of the menace of unemployment, the recognition of the universal right to work or maintenance, the legal limitation of hours of labour, and the drastic amendment of the Acts dealing with factory conditions, safety, and workmen's compensation.
+Labour has always stood for equal rights for both sexes, when other parties were ignoring or persecuting women. In politics, the Labour Party stands for complete adult suffrage, in industry for equal pay and the organisation of men and women workers in one trade union movement. To the woman worker and to the wife of the working man or the soldier, Labour can make a confident appeal. Better pay and pensions for the workman or soldier mean better conditions for his wife and family. There must be no sex party: the Labour Party is the Women's Party. Woman is the Chancellor of the Exchequer of the home. Labour stands with the Co-operative Movement in its insistence on reasonable food prices and fair distribution, and in its resistance to unfair taxation. The Labour Party will do all it can to aid co-operators in their struggle for a democratic food organisation and against unfair discrimination. Labour and Co-operation are a single movement, and in the coming battle with reaction they must fight side by side.
+Labour's programme is comprehensive and constructive. It is designed to build a new world, and to build it by constitutional means. It is a programme of national and international justice, founded on permanent democratic principles. Even in an election as sinister as this, in which a large part of the nation's youth is arbitrarily disfranchised by the Government, Labour confidently appeals to the country to support its programme of social justice and economic freedom.</t>
+  </si>
+  <si>
+    <t>http://labour-party.org.uk/manifestos/1910/jan/1910-jan-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>A general election has been forced upon the country by the action of the House of Lords rejecting the Budget. The great question you are to decide is whether the Peers or the people are to rule this country.
+Each Session since the last general election important Bills, upon which the House of Commons had spent much time, have been mutiliated or destroyed by the House of Lords, an irresponsible body which represents nothing but its own class interests. Not content with this, they now claim the right to decide what taxes shall be paid, upon whom they shall be levied, and for what purpose they shall be spent. They also claim to dictate the date at which Parliament shall be dissolved. The time has come to put an end to their power to override the will of the Commons.
+The country has allowed landowners to pocket millions of pounds every year in the share of unearned increment, and yet they object to pay a small tax upon what, in justice, should belong to the State. They wish at all costs to preserve their power to plunder the people.
+The Labour party welcomes this opportunity to prove that the feudal age is past and that the people are no longer willing to live on the sufferance of the Lords.
+The issues you have to decide are simple. Our present system of land ownership has devastated our countryside, has imposed heavy burdens upon our industries, has cramped the development of our towns, and has crippled capital and impoverished labour.
+At this crisis the Labour party mertis your support. It comes with great achievements and with a determination to do much more.
+In 1906 it pledged itself to restore to trade unions the same liberty as capital enjoyed during trade disputes.
+THAT PLEDGE HAS BEEN FULFILLED
+It pledged itself to insist upon old-age pension.
+THAT PLEDGE HAS BEEN FULFILLED
+It pledged itself to help drastic housing reform.
+THAT PLEDGE HAS BEEN FULFILLED
+It pledged itself to work for the relief of the burdens on persons of small or moderate means by the taxation of unearned incomes and land values.
+THAT PLEDGE HAS BEEN FULFILLED
+It pledged itself to pay special attention to the unemployed, and to compel any and every Government to contribute to the solution of this problem.
+THAT PLEDGE HAS BEEN FULFILLED
+The experience of the last four years has demonstrated the value of the Labour Party acting on independent lines. There still remain many problems to be solved.
+The right to work has still to be won, but is now well within the range of practical politics.
+The Poor Law must be broken up and pauperism abolished.
+Old-age pensions must be extended and increased on their present non-contributory basis.
+Restrictions upon the franchise, including the sex bar, must be swept away.
+The working and middle classes are still overburdened with rates and taxes. All these problems will demand the attention of an active, determined, and independent party, drawn from the people and in touch with the people. The Labour Party, therefore, appeals to you to renew your confidence in it, to add to its ranks, and increase its power. Vote for the Labour candidates. The land for the people. The wealth for the wealth producers. Down with privilege. Up with the people.</t>
+  </si>
+  <si>
+    <t>http://www.labour-party.org.uk/manifestos/1910/dec/1910-dec-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>You are again being asked to return a majority pledged to remove the House of Lords as a block in the working of our Constitution. Do it, and do it emphatically.
+But you ought not to allow this to cover up the questions in which you are specially interested.
+The iniquitous Osborne Judgement, which deprives organised Labour of the power to protect itself by political action, either locally or nationally, must be reversed.
+Do you think that you protect yourselves if the doors of the House of Commons are closed to You?
+The Osbourne Judgement is only the latest example of Judge-made Law, from which you have already suffered so much.
+You should also support payment of Members which, with the reversal of the Osborne Judgement, is now the Charter of the Trade Unionist.
+The New Parliament, will be called upon to deal with the right to work; sickness insurance, land reform; adult suffrage; Poor Law reform; factory inspection; medical treatment for school children.
+None of these subjects can be properly considered unless there is a strong and independent Party of Labour sitting in the House of Lords.
+Let all petty differences go to the four winds. Now is the time to unite. The poverty of one is the poverty of all. Let those who suffer join to remove their suffering. It can be removed in no other way.
+The Labour Party appeals to you to stand by yourselves and vote for the Labour candidates.</t>
+  </si>
+  <si>
+    <t>http://www.labour-party.org.uk/manifestos/1923/1923-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.labour-party.org.uk/manifestos/1924/1924-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.labour-party.org.uk/manifestos/1929/1929-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.labour-party.org.uk/manifestos/1931/1931-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.labour-party.org.uk/manifestos/1935/1935-labour-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>After a year of barren effort, the Conservative Government has admitted its inability to cope with the problem of Unemployment, and is seeking to cover up its failure by putting the nation to the trouble and expense of an election on the Tariff issue.
+The Labour Party challenges the Tariff policy and the whole conception of economic relations underlying it. Tariffs are not a remedy for Unemployment. They are an impediment to the free interchange of goods and services upon which civilised society rests. They foster a spirit of profiteering, materialism and selfishness, poison the life of nations, lead to corruption in politics, promote trusts and monopolies, and impoverish the people. They perpetuate inequalities in the distrubution of the world's wealth won by the labour of hands and brain. These inequalities the Labour Party means to remove.
+Unemployment is a recurrent feature of the existing economic system, common to every industrialised country, irrespective of whether it has Protection or Free Trade. The Labour Party alone has a positive remedy for it. We denounce as wholly inadequate and belated the programme of winter work produced by the Government, which offers the prospect of employment for only a fraction of the unemployed in a few industries; and in particular provides no relief for women and young persons.
+The Labour Party has urged the immediate adoption of national schemes of productive work, with adequate maintenance for those who cannot obtain employment to earn a livelihood for themselves and their families. The flow of young workers from the schools must be regulated to relieve the pressure on the labour market, and full educational training, with maintenance, must be provided for the young people who are now exposed to the perils and temptations of the streets.
+The Labour Programme of National Work includes the establishment of a National System of Electrical Power Supply, the development of Transport by road, rail and canal, and the improvement of national resources by Land Drainage, Reclamation, Afforestation, Town Planning and Housing Schemes. These not only provide a remedy for the present distress, but are also investments for the future.
+Agriculture, as the largest and most essential of the nation's industries, calls for special measures to restore its prosperity and to give the land workers a living wage. The Labour Policy is one that will develop Agriculture and raise the standard of rural life by establishing machinery for regulating wages with an assured minimum, providing Credit and State Insurance facilities for Farmers and Small-holders, promoting and assisting Co-operative Methods in Production and Distribution, so as to help stabilise prices, and make the fullest use of the results of research.
+The Labour Party proposes to restore to the people their lost rights in the Land, including Minerals, and to that end will work for re-equipping the Land Valuation Department, securing to the community the economic rent of land, and facilitating the acquisition of land for public use.
+Labour's vision of an ordered world embraces the nations now torn with enmity and strife. It stands, therefore, for a policy of International Co-operation through a strengthened and enlarged League of Nations; the settlement of disputes by conciliation and judicial arbitration; the immediate calling by the British Government of an International Conference (including Germany on terms of equality) to deal with the Revision of the Versailles Treaty, especially Reparations and Debts; and the resumption of free economic and diplomatic relations with Russia. This will pave the way for Disarmament, the only security for the nations.
+Labour condemsn the failure of the Government to take steps to reduce the dead-weight War Debt. No effective reform of the National Finances can be attempted until the steady drain of a million pounds a day in interest is stopped. Treasury experts, in evidence before a Select Committee of the House of Commons, expressed their view that a Tax on War Fortunes could be levied, and have therefore admitted both the principle and its practicability. A labour Chancellor of the Exchequer, in consultation with Treasury experts, would at once work out a scheme to impose a non-recurring, graduated War Debt Redemption levy on all individual fortunes in excess of £5,000, to be devoted solely to the reduction of the Debt.
+The saving thus effected, with reduction of expenditure on armaments, other sane economies, and the increased revenue derived from Taxation of Land Values, would make it possible to reduce the burden of Income Tax, abolish not only the Food Duties, but also the Entertainments Tax and the Corporation Profits Tax, as well as provide money for necessary Social Services.
+The Labour Party is working for the creation of a Commonwealth Co-operative Service. It believes that so far only a beginning has been made in the scientific organisation of industry. It will apply in a practical spirit the principle of Public Ownership and Control to the Mines, the Railway Service and the Electrical Power Stations, and the development of Municipal Services. It will make work safe for the worker by stricter Inspection of Workplaces, and more effective measures against Accidents and Industrial Diseases. It will provide fuller Compensation for the Workers and improve the Standard of Hours.
+Labour Policy is directed to the creation of a humane and civilised society. When Labour rules it will take care that little children shall not needlessly die; it will give to every child equality of opportunity in Education; it will make generous provision for the aged people, the widowed mothers, the sick and disabled citizens.
+It will abolish the slums, promptly build an adequate suppy of decent homes and resist decontrol till the shortage is satisfied. It will place the Drink Traffic under popular control.
+In accordance with its past actions inside and outside Parliament, the Labour Party will do its utmost to see that the Ex-Service men and their dependants have fair play.
+Labour stands for equality between men and women: equal political and legal rights, equal rights and privileges in parenthood, equal pay for equal work.
+The Labour Party submits to the men and women of the country its full programme. It urges them to refuse to make this General Election a wretched partisan squablle about mean and huckstering policies. It appeals to all citizens to take a generous and courageous stand for right and justice, to believe in the possibility of building up a sane and ordered society, to oppose the squalid materialism that dominates the world today, and to hold out their hands in friendship and good-will to the struggling people everywhere who want only freedom, security and a happier life.</t>
+  </si>
+  <si>
+    <t>The Labour Government, defeated in the House of Commons by a partisan combination of Liberals and Tories, appeals to the People.
+The supreme need of this country, as of the whole world, is peace among the nations, and the restoration of industry and commerce. For this the Labour Government has continuously worked; and it has already achieved much. It has insisted on maintaining, in the spirit as in the letter, the honourable binding Treaty with the Irish Free State, no less than the agreement with the Northern Province. It has maintained, and even strengthened the ties of sentiment with the Dominions upon which, rather than upon either force or any Imperialism, the very existence of the British Commonwealth of Nations depends. The embittered relations between France and Germany left by the disastrous tangles of preceding Governments have been improved, and cordial relations established between this country and France. Important steps have been taken at Geneva towards arbitration, security and general disarmament.
+The Labour Government has refused to exclude from this general pacification the Russian people, with whom it is essential to resume our trade in the interests of our unemployed and the country as a whole.
+The Treaties with Russia, now awaiting ratification, open up for our fishing industry thousands of square miles of additional fishing ground, and provide for new outlets for our manufactures and our coal. When compensation has been secured to British subjects for their losses in Russia, a third Treaty will be negotiated providing for the raising (from private financiers) by Russia of a loan the interest and sinking fund charges on which shall be guaranteed by Great Britain. It is laid down in Article 12 of the General Treaty that 'the amount, terms and conditions of the said loan and the purposes to which it shall be applied,' shall be defined in the future Treaty referred to; and this Treaty 'will not come into force until the necessary Parliamentary authority for the guarantee of the said loan has been given.' Will you allow this work for peace and prosperity to be stopped?
+In the face of much opposition, the Labour Government has passed into law the Great Housing Charter, the statute that enabled the Local Authorities and the Building Industry to engage in a fifteen years' uninterrupted building programme, with such generous financial assistance as will provide:
+Houses to let at low rents;
+A separated dwelling for every family in the land;
+A continuous policy of slum clearance and an ending of overcrowding.
+Meanwhile, the Rent Restriction Acts (which practically expire next year) have to be continued and amended; and the Bill to prevent profiteering in building materials has still to be passed. It depends on the result of the Election whether this great Housing Policy will be carried out.
+In Finance, the Labour Government has achieved a marked success. Whilst subjecting to the most competent examination its own and all other schemes for dealing with the War Debt, and the terrible burden upon industry of a tribute of £1,000,000 per day, the Labour Government has swept away no less than £30,000,000 a year of taxes on the people's food (just six times as much in eight months as the Liberal Government did in eight years). The Labour Government has abolished the irritating Inhabited House Duty, which no other Government had dared to do, and has taken the first step towards the Abolition of the Entertainment Tax. It has found means to change the whole spirit of the administration of the War Pensions Ministry, to increase in many thousands of cases the pittance that the preceding Governments had allotted to those Ex-Service Men who had suffered in the War, and to the parents and dependants of those who have fallen. Above all, the Labour Government has found means to stop the contemptible deduction from the weekly ten shillings of many thousands of Old-Age Pensioners, which the Liberal Government instituted, and the Unionist Government persisted in maintaining; whilst nearly 200,000 more old people, to whom the pension has been hitherto denied, have been admitted to the pension fold. Is it not because the Liberals and Unionists fear the Second Labour Budget that an excuse has been found for giving the Labour Government no further chance?
+Labour's intention to 'give every child equality of opportunity in education' has begun to be fulfilled in the drastic change of the policy of the preceding Government. The Labour Government has been insisting on smaller classes, an increase in the number of full-qualified teachers, new schools, maintenance for the poorer children, more free places in Secondary Schools and Scholarships to the University: all practical steps towards the ideal of securing to all children the same chance of advanced education as the children of the rich. The Labour Government has been steadily working towards progressively higher qualifications for teachers; and, consequently, of no niggardly treatment of teachers' salaries. Shall this policy now be reversed?
+The Labour Government has consistently acted on the conviction that Agricultural Prosperity is vital to the nation. It has helped the farmers by laons to their Co-operative enterprises, by assistance to their Credit Societies, by increasing grants for the development of the Sugar Beet Industry in this country. It has included exceptional provision, on a generous scale, for a vast increase of cottages in the rural areas at low rents, which will lessen the evil of the tied-cottage system. It has, after great difficulty and opposition from both the other Parties, got District Wages Committees and an Agricultural Wages Board once more set up by law, in the hope of obtaining and maintaining a decent Standard of Life for the labourers.
+Apart from the necessary transformation of the whole industrial system, the only practicable way of dealing satisfactorily with Unemployment is the working out of a constructive policy of National Development, along with the restoration, through pacification, of the production and trade of other nations. It is along these lines that the Labour Government has made progress. Meanwhile the Government has stimulated useful enterprises and helped works of further relief in all directions. During the building and other industries, the number of unemployed has been reduced by considerably over 100,000, and, indeed, by many more when allowance is made for the increased number of workers brought on to the live register as a result of the extension of the Insurance Act, and who had not previously been recorded as unemployed. The great works, notably in the way of building, involving furnishing, etc., and in the way of iron and steel and engineering for the electrical and mining developments, should provide work for a much larger proportion of the unemployed. For the others, Labour's slogan still remains 'Work or Maintenance'. By the drastic revision of the Unemployment Insurance Acts last Auguest, (1) the 'gap' has been abolished and the Benefits made continuous: (2) the arbitrary refusals of Benefit by the preceding Governments to something like one-fifth of the claimants have been stopped; (3) the weekly amount has been increased by about 25 per cent.
+The increased financial assistance provided by the Labour Government in aid of approved schemes of work and the improvements in the Unemployment Insurance Acts have together substantially relieved the heavy burdens previously borne by Local Authorities.
+All the Labour Government's other Bills before Parliament, great or small, are now summarily brought to an end. The great Factory Acts Amendment Bill, the Bill to prevent Profiteering in Building Materials, the Forty-Eight Hours (Washington Convention) Bill, the Bill to secure Wages for Shipwrecked Seamen, the Bill to prevent Frauds in the Sale of Bread, and various others, are stopped. But besides these Bills actually introduced, the work for the next Session has been going on steadily. The measures still in one or other stage of preparation for the next twelve months include proposals for:
+The reorganisation of the whole Mining Industry (in conjunction with By-Products and Power Stations), on the lines of National Ownership, equitable treatment for all interests concerned, security both for the taxpayer and the consumer, wages under properly-arrived at National Agreements, and participation in administration, both national and local, by the various grades and sections of those engaged in the industry.
+The continuance and amendment of the Rent Restriction Acts with a view to providing adequate protection for tenants.
+A drastic dealing with the whole Poor Law System, so as to secure the economy and efficiency of unified administration in each locality, and complete and honourable provision for the sick and infirm, the aged, the children and the able-bodied unemployed apart from the workhouse and pauperism.
+The Taxation of Land Values and such a dealing with Agricultural Land as will secure its maximum productivity, and with urban land and building sites as would protect the occupying tenants and secure its best use.
+The development of the present chaotic Electrical Generating Stations on the lines of a National System, uniformly standardised with transmission lines linking up town and country, with the primary object of providing cheap power for industry - instead of profit for shareholders - and cheap and convenient light for house-holders everywhere.
+With regard to the measures to be taken in the national interest against the evils and burdens connected with the administration of the Licensing Laws, the first step, it is clear, in the present state of the controversy, is a full and impartial inquiry by a Royal Commission. This is the Labour Government had arranged to begin next Spring.
+In addition to these measures the following proposals are being considered and prepared for:
+A systematic reorganisation, in the national interest and on terms fair to all concerned, of the whole system of Transport, including the more rapid development of an entirely Unified Railway and Canal System in National Ownership and under exclusively Public Control, with fuller use of electric power and in more intimate connection not only with the ports, but also with the increasing road motor service. Without greater and cheaper transport facilities, the British producers of every kind will find it ever harder to compete with their rivals.
+The Prevention of Profiteering and Exploitation by Rings, Trusts and Monopolies, not merely in building materials, but also in foodstuffs and household necessities, in conjunction with concerted arrangements with the Dominions and other Governments for bulk importing and systematically organised distribution from port to consumer, as a means towards establishing reasonable and stable prices.
+A substantial improvement of the Workmen's Compensation Acts, which the Tory Government denied to injured workers.
+The Prevention of Excessive Hours of Labour in the distributive trade, in the mercantile marine, and in other occupations (including those of women) omitted from the Washington Forty-Eight-Hours Convention: together with proposals for such a further development of the system of Trade Boards as will prevent the still existing evils of Sweating.
+Whether any of these projects can be proceeded with, and which of them, and to what extent, depends on the electors' response to the present appeal.
+Is it nothing to you that the Labour Government's successful work for Peace, its great programme of Housebuilding, its sweeping reduction in the Food Taxes, its forward policy for the Children's Chooling, should be interrupted, and that the Bill giving Votes for Women at 21 on the same terms as men should be killed? But there is more to be said. During the past few months the detailed working out of the Labour Government's measure giving Pensions for Widowed Mothers with Children has reached an advanced stage. In the very next Session it was to have been laid before Parliament. This is what the Liberals and Tories have combined to stop. It depends on this Election whether the Labour Government can secure this great reform.
+It is along such lines as those marked out in this Appeal, and in the spirit of public service herein indicated, that the Labour Party, in conformity with its consistent public declarations, would work in Parliament towards the transformation, gradual as it must be, of the existing economic and industrial system into a genuine Commonwealth of Labour. We know the facts. We realise the difficulties. The path to our goal is long and narrow and sometimes so hard to travel that men and women faint by the way. But we have faith in humanity. We refuse to believe that there is nothing to be done but conserve the present order, which is disorder; or that the misery, the demoralisation and the ruin that it causes to innocent men and women and children can be remedied by the perpetual repetition of the abstract principles of Individualism.
+We appeal to the People to support us in our steadfast march - taking each step only after careful examination, making sure of each advance as we go, and using each success as the beginning of further achievements towards a really Socialist Commonwealth, in which there shall at least be opportunity for Good Will to conquer Hate and Strife, and for Brotherhood, if not to supersede Greed, at least to set due bounds to that competition which leads only to loss and death.</t>
+  </si>
+  <si>
+    <t>The long-awaited opportunity has now come for the Nation to give its verdict on the present Government.
+By its inaction during four critical years it has multiplied our difficulties and increased our dangers. Unemployment is more acute than when Labour left office. International relations are worse. Vast areas of the country are derelict. The posters on our hoardings announcing the grim truth that 'a million of our fellow countrymen are needing food and clothing' tell how the Government has failed. In the face of such a state of things this Tory Government has sat supinely with folded arms without a policy, without a vision, waiting for Providence or charity to do its work. For nine months the Government watched the paralysing struggle in the Coal Industry. It aided and abetted the mine owners when they locked out the men, and provoked the industrial unrest that led to the General Strike, for which the Government was mainly responsible. The Government's further record is that it has helped its friends by remissions of taxation, whilst it has robbed the funds of the workers' National Health Insurance Societies, reduced Unemployment Benefits, and thrown thousands of workless men and women on to the Poor law.
+The Tory Government has added £38,000,000 to indirect taxation, which is an increased burden on the wage-earners, shop-keepers and lower middle classes. In its only Budget the Labour Government reduced the Food Taxes by £25,000,000. Now that the Election is in sight the Tory Chancellor has repealed what was left of the Tea Duty but has retained the duties on sugar, coffee and cocoa and other foods. This remission only amounts to one-sixth of the additional indirect taxation he has added in the last four years.
+Whilst every economic influence has been tending to reduce the cost of living the Government's policy has been to put obstacles in the way. It means to continue this policy. The Tory plan for solving Unemployment and improving trade - called 'Safeguarding' was denounced by the Prime Minister in 1923 as 'pottering along'. He was right, as experience shows. 'Safeguarded' countries have unemployment, low wages and sweating, poverty, generally corrupt politics, and high costs of living.
+In order to hide their record of incompetence and reaction, Tory leaders are trying to frighten the electors with horrifying pictures of the disasters which would come upon the country if a Labour Government were returned. It was such scaremongering tactics as this which gave the Tories a majority at the last Election. We do not believe that the voters will be misled a second time by such discreditable deception.
+We warn the electors against the misrepresentations of Socialism and the aims and Policy of the Labour Party, which are already pouring from our opponents.
+The Labour Party is neither Bolshevik nor Communist. It is opposed to force, revolution and confiscation as means of establishing the New Social Order. It believes in ordered progress and in democratic methods.
+The Labour Party gives an unqualified pledge to deal immediately and practically with this question. Its record on Unemployment is a guarantee that this pledge will be kept. Only by the unceasing advocacy of Labour have the claims of the Unemployed been forced to the forefront of political issues in the teeth of the opposition and neglect of the Liberal and Tory Parties.
+When the Labour Government was in office it announced to Parliament schemes of a comprehensive and far-reaching character which it had already begun to put into effect. Immediately afterwards both Parties united and defeated the Government! They could not tolerate its continued success.
+Our schemes for dealing with Unemployment have been before the country for years before the Liberal Party - in the hope of reviving its declining fortunes - appropriated some of them and proclaimed them as original.
+They are three-fold in character.
+1. National Development and Trade Prosperity
+Labour will undertake:
+Housing and Slum Clearance;
+Land Drainage and Reclamation;
+Electrification;
+The Reorganisation of Railways and Transport;
+New Roads and Road and Bridge Improvements;
+Afforestation associated with Small Holdings;
+Training and assistance by agreements with the Dominions for those who wish to try their fortunes in new lands.
+The most important attack upon Unemployment is to restore prosperity to the depressed industries, and develop our country. This programme will not only provide employment for large numbers of those who are now out of work, but its reaction of other industries will be immediate and beneficial.
+There is a great market at home which can be developed by increasing the purchasing power of the working classes. There is a greater market overseas, especially in India and the Crown Colonies, where there are enormous populations with a very low standing of living and vast undeveloped resources.
+A Labour Government will set to work at once by using Export Credits and Trade Facilities Guarantees, to stimulate the depressed export trades of Iron and Steel, Engineering, and Textile Manufactures. Shipbuilding and Shipping will immediately be benefited by an increase of foreign trade, and the improved employment in these industries will be a great addition to the purchasing power in the home market.
+2. Maintenance
+The Labour Party's plan for dealing with Unemployment is to provide work; but pending the absorption of the unemployment in regular occupations it will take steps to relieve the present distress. It will also amend the Unemployment Insurance Act so as to afford more generous maintenance for the unemployed, and will remove those qualifications which deprive them of payments to which they are entitled.
+3. The Young and the Old
+A Labour Government would also relieve the congestion in the labour market. Every year about 400,000 young persons, inadequately educated and inadequately trained, are brought into the labour market; while at the other end there are thousands of aged persons now compelled by poverty to struggle for employment who would be willing to retire if proper provision were made for them.
+The Party would extend the school age of fifteen with the necessary Maintenance Grants and provide Adequate Pensions for Aged Workers.
+The state of the Coal Mining Industry is so tragic that measures would be immediately undertaken to alleviate the distress in the coal fields, organise the industry from top to bottom both on its productive and marketing sides, and shorten the hours of labour. A Labour majority would Nationalise the Mines and Minerals as the only condition for satisfactory working. It would develop the scientific utilisation of coal and its valuable by-products, now largely wasted.
+The Labour Party is the Party of the Workers' Home. In 1924, it revived the policy of building Houses to be let and not sold. It will return to that policy until there are enough Houses let at Working-class Rents. It will deal drastically with the Slum disgrace and will provide the necessary money grants for both purposes. In the meantime it will protect tenants by continuing the Rent Restriction Acts.
+Peace is one of the greatest issues of the Election. The Labour Government found Europe distracted by hostility and left it in a peaceful frame of mind. The Party's record when in office entitles it to the confidence of all lovers of peace. It desires to resume its work and to regain for this country the proud position it held in 1924.
+The Tory Government has hampered Disarmament, and systematically obstructed the work of the League of Nations and of the International Labour Office. Labour's policy is precisely the opposite. It will establish the largest possible measure of political and economic co-operation amongst the nations, and give the fullest and most cordial support to the League and the International Labour Office.
+Labour stands for Arbitration and Disarmament. It will accept the general Act of Arbitration, Conciliation and Judicial Settlement approved by the League. A drastic reduction of armaments is long overdue. Labour welcomes the initiative of the United States. It will press for the speedy completion of the Disarmament Treaty and the convocation of a General Disarmament Conference.
+Labour will re-establish diplomatic and commercial relations with Russia.
+Labour is deeply concerned about Agriclture which, having been a plaything of both the older Parties, is now facing very critical times both for farmers and workers. An Agricltural Policy must be co-ordinated with a Town Policy. Farming must be made to pay.
+Landlordism has ceased to be able to perform its function and it cannot be allowed to go on starving the Land of capital and the countryside of cultivation and people, and generally obstructing national need and development. The Land must therefore pass under Public Control. Meanwhile, Farmers should have Security of Enure; Fair Rents; Capital and Credit Assistance; A system of Organised Marketing; and Stability in the Prices of main crops and products. Workers should have a Minimum Wage; Unemployment Insurance; Easier Access to Holdings; and Better and Untied Cottages. A Labour Government would work with representatives of all the interests concerned to gain these objects.
+The Labour Party has always been committed to securing Equal Educational Opportunities for eveyr child. It will raise the school-leaving age to fifteen with the requisite Maintenance Grants and at once develop facilities for Free Secondary Education. Labour will open the road, to whoever is able to take it, from the Nursery School to the University.
+The Party stands for a system of Taxation which will distribute the burden fairly according to 'ability to pay'. It will abolish Taxes on Food and other necessaries, and provide what revenue is needed by Death Duties on large estates and by graduating the Income Tax and Sur-Tax with a view to relieving the smaller, while increasing the contribution from the larger, incomes. The Labour Party will carry still further the differentiation between 'earned' and 'unearned' incomes.
+The Party will deal drastically with the scandal of the appropriation of Land Values by private landowners. It will take steps to secure for the community the increased value of land which is created by industry and the expenditure of public money.
+The grave injustices of the existing Widows', Orphans' and Old Age Pensioners Acts would be immediately remedied, and as soon as the urgent legislation to deal with Unemployment had been carried through, a comprehensive co-ordination and extension of all the Pensions Schemes would be undertaken so as to give the opportunity to many classes of persons now excluded to come in.
+The limit of seven years which has meant so much injustice to ex-Service Men will be removed, so that cases may still be considered.
+Among the other measures which a Labour Government would enact are the Factories Bill, the Ratification of the Washington Eight Hours' Convention, and the amendment of the Workmen's Compensation Acts and the Trade Union Law. It will also, as promised, appoint Committees of Inquiry into the causes of depression in the Cotton and Iron and Steel Industries with a view to their reorganisation.
+It would take steps to prevent the Profiteering in Food, and in Building Materials, and would watch the operations of Trusts and Combines, so that combinations, which enhance prices unreasonably or refuse to supply or to sell to persons who will not deal exclusively with them, may be made subject to law.
+It would support the creation of separate legislative assemblies in Scotland, Wales and England, with autonomous powers in matters of local concern.
+In order to prepare the way for the Reform of the licensing Laws, the first necessary step is a full and impartial inquiry, which a Labour Government would institute at once by Royal Commission.
+The Labour Party makes its appeal to the Women Voters with the fullest confidence. It was advocating the cause of Equal Citizenship when the Tory and Liberal Parties were either utterly hostile or hopelessly divided on the question. Although Equal Franchise has been secured after a protracted struggle, the fight for women's emancipation is not yet finished. There are other anomalies and injustices - lega, social and economic - especially affecting women and children which must be dealth with.
+The Labour Party recognises that the burden of social injustice and economic exploitation fails with special severity on women, and that women are very seriously affected by Unemployment, Low Wages, Bad Housing, and by any restriction of the necessary public expenditure on Education and on the Health and Welfare of Mothers and Children. The prevention of Maternal Mortality will be an immediate concern of a Labour Government.
+The Labour Party in its legislative and administrative policy would seek to pursue and apply the principle of equal tratment for men and women.
+Moreover, there is the important question of universal peace, vital to all, which requires to be organised on a permanent basis so as to terminate for every the futility of a civilised country squandering human life and wasting its national resources in war.
+We shall not deceive the people by saying that the task of National and Social Reconstruction is easy, or that it can be accomplished in a day or a year. But the Labour Party does pledge itself to undertake this great work with energy and enthusiam, and it confidently believes that, if it has a majority, in the full lifetime of a Parliament great advance in industrial prosperity, in social wellbeing, and in a more just distribution of the fruits of labour, can be made.
+At this Election, voters have to choose not only the representatives of constituencies, but a Government. A Labour Government is the only alternative to the present Tory Government. The Liberal Party, as its leaders admit, can be no more than a small minority in the new Parliament. The electors who desire to save the country from the disaster of continued Tory rule must therefore vote for Labour Candidates.
+Along this path Labour will advance.
+The Labour Programme of peaceful but determined National Development and Reconstruction leading towards the Socialist and Co-operative Commonwealth is the only alternative to Reaction and Revolution. On this Programme Labour asks for the support of men and women of good will of all classes. Labour wants to make its contribution to the removal of poverty and the injustices which today are diseases in society. Both the other Parties have been tried and have failed. The state of the country is the monument of their failure.
+We pledge ourselves to give unsparingly the best we can of our energy, experience and knowledge, to the great of making Britain a happier and more contented land, and establishing peace in the world.</t>
+  </si>
+  <si>
+    <t>A decisive opportunity is given to the nation to reconstruct the foundations of its life.
+The Capitalist system has broken down even in those countries where its authority was thought to be most secure.
+Its fails to give employment to many millions of willing workers.
+Its accumulates vast stocks of commodities which it is unable to distribute.
+To re-establish its position, it now demands from the unemployed and the wage-earner the surrender of their hard-won standard of life; and it seeks to force the Government of this country to restrict or abandon those social services which the Labour Party believes to be an essential condition of a democratic society.
+The Labour Government was sacrificed to the clamour of Bankers and Financiers. Because it placed the needs of the workers before the demands of the rich, a so-called 'National' Government was installed in its place to wrest from Parliament the authority to satisfy them. The policy of that Government has proved a disastrous failure. Formed to maintain that gold standard which it declared in panic-stricken accents to be the indispensable condition of national safety, within less than three weeks it abandoned that standard with the insolent explanation that industry would benefit by the change.
+Having failed completely in its original object, it now seeks from the electorate a mandate for the impossible task of rebuilding Capitalism. Composed of men who differ profoundly on all the main principles of public policy, unable to agree upon any of the essential methods by which to restore prosperity to the nation, this ill-assorted association of life-long antagonists seeks a blank cheque from the people for purposes it is unable to define. Acutely divided within itself; headed by men who are now acting in direct contradiction to their own previous convictions, certain, in the nera future, to split into fragments, it makes the shameless pretence of being the instrument of national unity.
+The Labour Party is confident that the country will not be deceived by claims so arrogant and so dishonest.
+The Labour Party seeks a majority from the electorate upon the basis of a coherent and definite programme. It reaffirms its conviction that Socialism provides the only solution for the evils resulting from unregulated competition and the domination of vested interests. It presses for the extension of public-owned industries and services operated solely in the interests of the people. It works for the substitution of co-ordinated planning for the anarchy of individualistic enterprise.
+Labour insists that we must plan our civilisation or perish.
+The Labour Party reaffirms its faith in the considered principles of its programme of 1929 laid down in Labour and the Nation.
+Despite the unexampled difficulties confronted by the Party when, as a Minority Government, and in the face of a world economic crisis, it took office two years ago, it made a substantial beginning in translating that programme into Acts of Parliament.
+Its policy of national development resulted not only in economic public works of unprecendented magnitude, but also in strenuous attempts, by legislation and otherwise, to imrpove the efficiency of our agricultural, transport, coal and other chief industries. The Labour Government made important improvements in Unemployment Insurance and the consequent transfer of heavy burdens from the Poor Law. There were wide extensions of housing and pensions legislation, and the vigorous promotion of education and the health services. In the international field Labour's record was pre-eminent.
+This record was achieved under the intolerable restrictions of its minority position in the House of Commons. Frustrated by political intrigues and the class-conscious hostility of the House of Lords and undermined by the organised pressue of business interests, it now asks for power to press forward rapidly to the fulfilment of its programme. In that endeavour it will tolerate no opposition from the House of Lords to the considered mandate of the People; and it will seek such emergency powers as are necessary to the full attainment of its objectives.
+The Labour Party recognises that the present situation calls for bold and rapid actions. The decay of capitalist civilisation brooks no delay. Measures of Socialist reconstruction must be vigorously pressed forward. That is the task to which Labour will lay its hand.
+The Labour Party is convinced, in the light particularly of experience since 1925, that the banking and credit system of the country can no longer be left in private hands. It must be brought directly under national ownership and control.
+The Labour Party further is convinced of the need to form a National Investment Board with statutory powers for the control of dmoestic and foreign investment. It would seek powers from the new Parliament to effect this transformation.
+Aiming at a monetary policy which will stabilise prices, the Labour Party condemns either currency inflation or a new and disastrous attempt at deflation to force sterling back to the old gold parity. It will take a vigorous initiative in calling an International Conference to arrive at a concerted monetary policy. It will seek thereby to make the resources of civilisation available for peoples who today in the new world, as in the old, are starving in the midst of plenty.
+The Labour Party has never failed to insist upon the intimate relation between war debts, reparations, and economic depression. It believes that the general acceptance of President Hoover's Moratorium on War Debts permits a reconsideration of the whole question.
+It seeks an immediate reopening of negotiations between the signatories of the Young Plan and the United States with a view to attaining the conditions in which Inter-Allied War Debts and Reparations may be cancelled.
+The Labour Party has no confidence in any attempt to bolster up a bankrupt Capitalism by a system of tariffs. Tariffs would artifically increase the cost of living. They would enrich private interests at the expense of the Nation. They would prejudice the prospect of international co-operation. In the circumstances produced by our departure from the gold standard, they have no relevance to economic need. In the face of the millions unemployed in high-tariff America and Germany, they are clearly no cure for unemployment. They would permanently injure our shipping and export trades and conceal our need for greater efficiency in industrial organisation.
+The Labour Party urges a better way.
+It urges the definite planning of industry and trade so as to produce the highest standard of life for the Nation.
+As a first step, it proposes to reorganise the most important basic industries - Power, Transport, Iron and Steel - as public services owned and controlled in the national interest, with such a regulation of prices as will enable British industry to compete effectively in the markets of the world. Wherever necessary, Import Boards will be created for foodstuffs, raw material, and manufactured goods with all adequate powers of regulation and purchase. For the proper and organised conduct of export, machinery will be set up in connection with the principal industries.
+The Labour Party demands efficiency. Any special assistance of industry must be conditional upon the acceptance of the necessary measure of public ownership or control. Labour will insist upon the adoption of efficient methods of production so as to secure good conditions of employment for the worker. The consumer must be protected by effective regulation of prices.
+Labour in power will remove the unjustified restrictions upon Trade Union activity introduce by the Tory Government in 1927; and it will press forward with legislation upon such matters as Workmen's Compensation, and the Conditions of the Hours of Labour.
+Because it appreciates the vital importantance of the Co-operative Movement, the Labour Party will work in full alliance with co-operators, utilising their long experience and specialised knowledge.
+The tragic position of the Coal Industry reveals the complete inability of private ownership to organise it as a national asset and Labour in power will proceed at the first opportunity to the unification of the industry under public ownership and control.
+The Labour Party has always been in the van of the Movement for International Peace; and it is universally recognised that its record, as a Government, above all in solving disarmament by Arbitration, gave to Great Britain the moral leadership of the World. Labour will seek to make that record even more distinguished.
+It will seek, at the Disarmament Conference next February, to put forward proposals for drastic and far-reaching reductions by international agreement, in the numbers and equipment of all armed forces, and in all expenditure upon them. Labour insists that without this policy of disarmament there cannot be either peace or security.
+Labour will, as in the past, lend its full support to the use of the valuable machinery of the League of Nations in every phase of international activity.
+The Labour Government has already made a real beginning towards the scientific re-organisation of agriculture. The Labour Party will seek to press forward that development. It holds that, for this purpose, the land must be publicly ownered and controlled, and much more fully utilised for food production and the provision of employment under good conditions.
+To achieve this end, full use must be made of the Acts passed under its auspices. The necessary machinery must be set up to make possible that comprehensive plan of development under which alone agriculture can become a prosperous industry.
+The Labour Party emphasises its insistence that the condition of the farm-worker must be improved, especially by provision for Unemployment Insurance, a National Wages Board to control county wage machinery, and the abolition of the tied cottage.
+The Labour Party places on record its conviction that the summoning of the Round Table Conference by the Labour Government in 1930 opened a new epoch in the history of our relations with India. It is convinced that its reassembly offers a unique opportunity to establish a new era of friendly partnership between the two peoples. While recognising the difficulties to be surmounted, the Labour Party will offer stern opposition to those who seek to prevent the Conference from bearing its full result.
+If returned to power, Labour will leave no stone unturned to bring the Conference to a successful issue.
+The Labour Ministers resigned because they refused to abandon Labour's cardinal principle that proper provision for the unemployed is a social duty and a national responsibility. Sound public policy demands the absorption of the unemployed into normal work; while that is being effected, adequate maintenance should be provided.
+The Labour Party protests against the reduction in the rates of unemployment benefit and the increase in contributions. It denounces the introduction of Poor Law Tests and machinery into the administration of Unemployment Insurance.
+It pledges itself to reverse immediately the harsh policy of the present Government.
+Labour accepts a balanced Budget as the first condition of sound national finance, but it condemns the Economy Act as an unjustified means of attaining this end.
+It pledges itself to maintain and develop the social services and to deal with the Rents Problem. It will restore, as rapidly as the claims of the unemployed and other depressed sections of the community permit, the remuneration of teachers and other public servants.
+It is for these ends that the Labour Party asks for power at the forthcoming Election.
+It warns the Nation that the alternative is the continuance in office of a Government harsh in purpose and incompetent in method, whose failure to produce a constructive policy offers no prospect of hope. Dominated as that Government is by the selfish interests of big business and finance, its return would encourage ruinous attacks on wages. Its victory would perpetuate the degradation and misery of unemployment. It would intensify nationalist economic conflict, and imperil all progress towards international co-operation and disarmament without which there can be no hope of peace or prosperity.
+The Labour Party offers to the people of this country planned reconstruction, national and international, instead of the chaos and anarchy which are the parents of disaster. It recognises the gravity of the issue; it is prepared to meet it by bold and drastic remedies.
+Given a majority, the Labour Party pledges itself to unsparing efforts to remove the spectres of want and insecurity from the homes of the people, that this and succeeding generations may be assured of a fuller and richer life.</t>
+  </si>
+  <si>
+    <t>Four years have passed since the 'National' Government obtained a swollen majority in the House of Commons on a campaign of fraud, misrepresentation and panic. The Government has now decided to plunge the nation into an electoral struggle in the midst of an international crisis.
+The Labour Party deplores this attempt to exploit for partisan ends a situation of grave international anxiety.
+It accepts the challenge and enters the Election confident of victory.
+At the end of four years the country faces the grim spectacle of two million workless with an army of well over a million and a half people on the Poor law, and with the deepening tragedy of the distressed areas. Whilst doles of varying kinds have been dispensed on a lavish scale to industry after industry, not a single constructive step has been taken to improve the lot of the people.
+The Government has robbed the unemployed of benefit and subjected them to a harsh and cruel household means test.
+It withdrew, under a storm of public indignation, its new Unemployment Regulations, and after nine months of reconsideration of this burning question it has ignominiously failed to produce any policy for the proper care of the unemployed.
+It has retarded the building of houses to let, curtailed schemes on food and other necessaries of life and by deliberately organising restriction of supplies.
+The international situation
+The Government has a terrible responsibility for the present international situation. It did nothing to check the aggression of Japan in the Far East, and thus seriously discredited the League of Nations and undermined the Collective Peace System.
+It has wrecked the Disarmament Conference by resisting all the constructive proposals made by other States. As regards air armaments, in particular, Lord Londondery has boasted that he succeeded, though with great difficulty, in preventing an agreement for the complete abolition of all national air forces.
+The Government has helped to restart the arms race, and it failed to make Signor Mussolini understand that, if he broke the peace in Africa, Britain would join with other nations in upholding the authority of the League.
+Too late to stop the war, the Government ranged itself at the eleventh hour behind the Covenant at Geneva. Even so, its action has been slow and half-hearted. Whilst paying lip-service to the League it is planning a vast and expensive rearmament programme, which will only stimulate similar programmes elsewhere. This Government is a danger to the peace of the world and to the security of the country.
+The Labour Party calls for a reversal of this suicidal foreign policy. It seeks wholehearted co-operation with the League of nations and with all States outside the League which desire peace. It standard firmly for the Collective Peace System. It demands speedy action, through the League, to bring the war in Africa to an end, to be followed by an immediate resumption of negotiations for all-round disarmament.
+Labour will efficiently maintain such defence forces as are necessary and consistent with our membership of the League; the best defence is not huge competitive national armaments, but the organisation of collective security against any aggressor and the agreed reduction of national armaments everywhere.
+Labour will propose to other nations the complete abolition of all national air forces, the effective international control of civil aviation and the creation of an international air police force; large reductions by international agreement in naval and military forces; and the abolition of the private manufacture of, and trade in, arms.
+A Labour Government would also seek full international co-operation in economic and industrial questions, with a view to increasing trade and raising standards of living throughout the world, and removing the economic causes of war, through equitable arrangements for access to markets, for the international control of sources of supply of raw materials, and for the extension of the mandate system for colonial territories.
+At home, the Labour Party will pursue its policy of Socialist Reconstruction. Labour has already put before the country, boldly and clearly, schemes of public ownership for the efficient conduct, in the national interest, of banking, coal and its products, transport, electricity, iron and steel, and cotton.
+It has also declared for the public ownership of land, in order that the community should profit by its value and proper use, the reorganisation of agriculture, the introduction of unemployment insurance for farm workers, the abolition of the 'tied' cottage, and the provision of cheap cottages in the countryside.
+Labour is pledged to a comprehensive programme of industrial legislation, so as to secure reasonable hours and conditions of employment for all workers and adequate compensation for the accidents of working life. It would restore the freedom of Trade Unions lost through the Trade Disputes and the Trade Unions Act. It would repeal the unjust and penal tax which the Government has imposed upon Co-operative Societies.
+Labour in power will attack the problem of the distressed areas by special steps designed to deal with the root causes of their troubles, as part of a vigorous policy of national planning. Labour will sweep away the humiliating means test imposed by the 'National' Government and will provide adequately for the unemployed, but will seek above all to reabsorb idle workers into productive employment by far-reaching schemes of national development. The Labour Party stands for a big move forward in education, including the raising of the school-leaving age with adequate maintenance allowances. It will vigorously develop the health services, and, in particular, will treat as one of its immediate concerns the terrible and neglected problem of maternal mortality. It favours an increase in the amount of old age pensions and a lowering of the qualifying age. It will go ahead with the provision of healthy homes for the people at reasonable rents, until the needs of the nation are fully met.
+Labour seeks a mandate to carry out this programme by constitutional and democratic means, and with this end in view, it seeks power to abolish the House of Lords and improve the procedure of the House of Commons.
+Labour asks the Nation for a Parliamentary Majority to promote Socialism at home and Peace abroad.</t>
+  </si>
+  <si>
+    <t>Robert Gascoyne-Cecil</t>
+  </si>
+  <si>
+    <t>Arthur Balfour</t>
+  </si>
+  <si>
+    <t>Andrew Bonar Law</t>
+  </si>
+  <si>
+    <t>Stanley Baldwin</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1900/1900-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1906/1906-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1918/1918-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1922/1922-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1923/1923-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1924/1924-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1929/1929-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1931/1931-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1935/1935-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>On the eve of the dissolution I take the liberty of recalling to your minds the considerations which, in my judgement, should weigh with you in the exercise of your rights as voters during the next few weeks.
+The one object you should have in view is to bring about, to the utmost of your power, by the exercise of your vote, the result you desire to attain. This counsel seems a truism; but it is nevertheless tolerably evident that, if the elections fail to produce a Parliament fitted to deal with the emergency of the time, it can only be because the truism is neglected.
+In the forecast of competent prophets we are threatened with many abstentions. These abstentions will be due to one or two causes. Either the candidate whom the voter prefers upon broad issues of policy differs from him as to some subordinate question on which he has set his heart, or the voter is convinced that his friend will succeed without his troubling himself to give a vote.
+It is obvious that if these causes of abstention operate in a sufficient number of instances they will imperil a considerable number of seats; and no man can know how many of his fellow-electors are disposed, by imitating it, to give to his conduct its natural result.
+If they are many the majority of the winning party will be reduced; and it will be so far crippled in carrying out the policy on which the nation has decided. Whose purpose will this result have served?
+It is certainly not the result the abstaining voter desires. He will not be one whit nearer his ideals in respect to various sectional objects in regard to which independent electoral combinations have been proposed. On the fate of these questions the election that is pending will have left no trace; and the abstention of the abstaining elector will have been without effect. But on the broad questions of policy the electors abstaining from whatever cause, whether from resentment on a subordinate question or from indolent over-confidence, will have a formidable influence. They will have contributed within the limits of their ability to weaken the Parlimentary force of the Unionist party, and of the Unionist Government to whom power may be entrusted.
+The gravest questions must be dealt with. The Imperial Power over the territories of the two South African Republics, which, as events have proved, was unwisely relinquished, must be rebuilt upon durable foundations.
+In due time those territories will doubtless enjoy the benignant colonial policy which this country has pursued for half a century, and whose brilliant fruit may be discerned in the affection that so many of our colonies have displayed to the mother country during the recent war.
+How long an interval must elapse before the full position of a British colony can be attained by these South African territories will naturally depend on the disposition and conduct of the inhabitants. But we cannot expect to secure the steady submission of those whom we have overcome in the field, unless they see that the Government of the Queen has so much Parliamentary strength that there is no hope of driving it from its policy of persistent resisteance or agitation. All the recent troubles of South Africa have come from a shift of Parliamentary opinion at a crucial moment.
+The brilliant success of Lord Roberts and his Army must not blind us to the fact that the war has disclosed imperfrections in our own armour of defence which, but for it, might have remained unnoticed. It will be among the most urgent duties of Parliament and the Government, now that peace is apparently restored, to investigate and remove the defects our military system in the light of scientific progress and the experience of other Powers. But for such a task a Government will need strong Parliamentary support. Some may think, though I should not agree with them, that the task might be as effectively performed by our opponents, if any possessed an adequate majority and a party organisation capable of sustaining the burden of government. But it certainly could not be discharged by a nearly divided House of Commons and a Ministry depending upon a broken party.
+To the difficulties which will occupy a future Government China will furnish an abundant contribution. We will fully shared with other Powers that calamities by which the disturbances in that Empire have been commenced; and we are probably more interested than any other nation in the preservation of the treaty rights which protect our commerce. The fact that we are acting with other Powers forbids me from entering without reserve upon questions of Chinese policy. But in maintaining our own rights, and joining in the efforts of our allies to restore and secure tranquillity, we shall be approaching a task of which it is difficult to overrate the complexity.
+I earnestly trust that the electors, in confiding the solution of this and the other problems I have mentioned to the party which is victorious at the polls, will remember that, unless the party is armed with a strong majority in the House of Commons, it will lack the authority at home and abroad which is essential to the performance of its task.</t>
+  </si>
+  <si>
+    <t>The party with which I am connected, and the Government of which I was a member, after being in power for ten years, has been replaced by the late Opposition. The task the constituencies have now to perform is to choose between them. It should not be a difficult one. So far as we are concerned your information is ample; our legislation, our foreign policy, our Colonial policy, are before you, and there are such as need cause neither shame in us nor regret in you. The same principles on which we have based our actions in the past will serve as their foundation in the future, and in the future as in the paast they will promote peace among nations, closer union between different portions of the Empire, and social legislation at home which is not likely to be less beneficient to the community because it is mindful of individual rights.
+Your information about the new Government and its supporters is no doubt more limited. You know them chiefly as critics, and it must be owned that their criticism has been singularly unscrupulous - as in the case of Chinese labour - and sometimes singularly perverse - as in the case of the Prime Minister's famour attack on the humanity of our Army. But, after all, we are not restricted in our survey to the performances of his Majesty's present advisers while they were in Opposition. Some of the most distinguished of them have held office before, and as they boast an unrepentant fidelity to the views which they entertained in 1892, we must anticipate a return to the policy they then attempted, but were fortunately too feeble to accomplish. There are many things still obscure in the long catalogue of revolutionary changes advocated by the new Ministers, but some things are plain enough - Home Rule, disestablishment, the destruction of voluntary schools, and the spoliation of the license-holder have lost none of their ancient charm in the eyes of Radical law-makers, and to the troupe of old acquaintances is now added a procession of shadowy suggestions respecting which we hardly yet know enough to say whether they are dangerous or merely useless.
+On one subject only does change, nay, even to hint of change, seem to them abhorrent. With a light heart the Radical leaders are prepared to destroy the Union, to uproot an ancient Church, to banish denominational religion, or even all religion, from the elementary schools. But one thing is sacred, and that is the fiscal practice of this country. The conditions of international trade may alter, the relation of Britain to other industrial communities may be utterly transformed, her Colonies may press for closer commercial union with the mother country - it matters not at all. The fiscal creed of the new Radical is that what was good 60 years ago must not only be good now, but must for ever be incapable of improvement. I take a more conservative view. I believe in the wisdom of adapting our policy, in fiscal matters as in all matters, to the changing conditions of a changing world, and I hold that the time has come when such adapting is urgently required. Should you return the Unionist party to power, it is to the reform of our fiscal system that its attention ought first to be directed - a task worthy of the efforts of a great party.
+To the foreign policy of the new Government we might seem justified in looking with more satisfaction than to its legislative projects, for apparently it is designed to be a continuation of our own. But, confident as I am of the capacity and patriotism of Sir Edward Grey, I doubt the successor his imitation. A foreign policy which is to be pacific, honourable, and consistent, requires not merely a Foreign Minister of ability, but a Foreign Minister who has two conditions in his favour. The first is a strong defensive naval and military force, without which diplomacy in time of serious stress degenerates either into buff, or into appeals for mercy, or into a haggle over blackmail. Whether this condition will be fulfilled some recent utterances of the Prime Minister leave me in anxious doubt. But there is a second and not less important condition of success whcih the new Foreign Secretary cannot hope to secure, and that is the support of a united Cabinet dependent on a United Party. On their legislation the Ministers may have come to some working agreement - time will show - but no agreement on the unforeseen problems of international statesmanship is possible among men who will look at them when they arise from such different points of view as those of the "Little Englander" and "Liberal Imperialists". But the differences in the Cabinet, serious as in this connexion they cannot fail to be, are nothing compared with the differences which divide the confederation of parties on which the Cabinet depends. In Imperial matters the gulf which divides, say, Mr Perks from Mr Redmond is immeasurable; no formula can conceal it, no compromise can bridge it; and if the new Government survive the general election, and if during their term of office their country becomes involved in international difficulties, the Foreign Secretary may find himself labouring under conditions which are favourable neither to his own fame nor his country's welfare.
+Such, in brief outline, are the public grounds on which I venture to recommend my candidature to your favourable consideration. Other grounds there are - ancient friendship, mutual confidence, long habits of loyal co-operation - to which I might make appearl; but if the personal side of the question is to be touched at all, I have, perhaps no right to do more than ask whether, during the 20 years in which you have extended to me an ungrudging support, I have not done political service which may make me not unworthy of your continued confidence.</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1910/jan/january-1910-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>It is understood that Parliament will be dissolved early in 1910; and I shall then solicit the renewal of the confidence which you bestowed on me in such generous measure nearly four years ago. The immediate occasion of the dissolution is the resolution of the House of Lords that the country should be consulted upon the Budget proposals of 1909. The Budget, therefore, is the subject primarily before the constituencies, and it might have been supposed that the alternative methods of raising money necessary to meet the obligations of the Treasury would have been the topic most deepy interesting to Government. For motives not difficult to conjecture this does not seem to be the case. It is not the merits of the Budget about which they are concerned; it is that those merits should be submitted to the judgement of the people and (bitterest of all) submitted at the instance of the Upper House. There may be good reason for their irritation; but assuredly they are not reasons drawn either from the letter or the spirit of the British Constitution; nor are they based on those more general principles of government common to representative institutions in the best types of modern democracy.
+The claim of the Government, stripped of the bad history and bad law with which it is obscured, is simplicity itself. They hold that the House of Commons, no matter how elected, or when elected, nor matter what its relation to public opinion of the moment, is to be the uncontrolled master of the fortunes of every class in the community; and that to the community itself no appeak, even in the extreme cases, is to be allowed to lie. The question, be it noted, is not whether the Second Chamber may orignate money Bills, for that has never been raised; nor whether they may amend money Bills, for that has not been raised; nor raised are three
+May there not be occastions on which an appeal to the people on matters of finance is necessary?
+Is not this one of them?
+If these questions be answered in the affirmative, does any other machinery exist for securing such an appeal than that which has been set in motion by the House of Lords?
+In the United States of America it is a fundamental principle of the Constitution that no king of property shall be prejudiced by special taxation. That Constitution is not easily changed; and before a measure like the British Budget could be legally attempted the consent must be obtained of a two-thirds majority in both Houses, nor could any such measure become law without a national mandate from a still stronger majority of the country.
+If we suggest the impossible, and imagine these constitutional safeguards withdraw, would the American taxpayer ever then be reduced to the precarious position of his British brother. Far from it. Special taxation might, indeed, by imposed by the House of Representatives, but it could be rejected by the Senate, it could be vetoes by the President.
+I do not ask the British citizen should enjoy the same security for his property as the citizen of the United States. I am not so immoderate. I only ask that if his property be subjected to exceptional taxation, by the caprice of a Minister and his majority, he should not be deprived of the only methods known to our Constitution by which an appeal to his fellow-countrymen may possibly be secured.
+The trust of the matter is that the present attack on the House of Lords is but the culmination of a long-drawn conspiracy. The Government came into office, not to work the Constitution of the country, but to destroy it. They desire what is in effect a single Chamber Legislature. The Second Chamber may be permitted to survive, partly changed so long as names remain the same; partly to correct the legislative slips of the Lower House which, under our existing system, are numerous, and I believe inevitable. But they desire that for all important purposes the Constitution of Britain shall be as definitely a single Chamber Constitution as the Constitution of Guatemala. For this end they have continuously laboured. It is this policy which represents the solitary thread of constitency connecting the wayward legislative projects of the last four years.
+I have watched with interest the progress of this conspiracy. Its results must so far have disappinted the conspirators. On no single occasion when Bills have been rejected by the Upper House or abandoned in the Lower on the alleged grounds that they had been mutilated by the Lords, has the rising tide of the Ministerial unpopularity shown the slightest pause or check. Then came the Budget; and with it the opportunity of manoeuvring the House of Lords into the positino of either abandoning its functions as a Second Chamber or of taking action which might give new life and hope to the contrievers of the single Chamber plot.
+The scheme was ingenious. I do not thinkg it is proving successful. The people of this country are not insulted by having their opinion asked on the Budget, nor do they think that the House of Lords has gone beyond their duty in asking for it. And they are surely right. For the single Chamber system is not consistent with the democratic working of representative Government in complex and developing communities. The representative Assembly is no doubt the primary organ of the popular will, and it possesses powers in this country which it certainly does not possess either in the Republic of America or in the Republic of France. It determines without appeal the political complexion of the Government. It controls all the Estimates. In initiates all the taxes. In legislation it is the dominating partner. The Ministers who direct, and sometimes tyrannize over, its deliberations, are nevertheless its creatures; and while no vote of the House of Lords could reduce the salary of an Under-Secretary by a shilling, the most powerful Cabinet must bow to the House of Commons.
+These are great powers; in some respects they are, I believe, without example. But they do not satisfy the single Chamber conspirators. And why? Because they wish the House of Commons to be independent, not merely of the Peers, but of the people.
+Nor would there be grave objection to this if there was any security that the action of the elected embodied on all great and far-reaching issues the deliberate will of the electors. But there is not and cannot be any such security. It is only by a transparent convention that we can, for example, assume that a House of Commons returned on the cry of Chinese slavery represents the mind of the nation on the question of Socialism. And the convention, which is convenient and in many respects even necessary, because not merely absurd, but perilous, when it is applied to questions of fundamental importance, which have been but imperfectly discussed, which are perhaps but imperfectly understood, which deeply affect individual rights and social well-being.
+In such cases there should be an appeal from the people's representatives to the people themselves; and no machinery, however imperfect, for securing this end should be abandoned until a better has been devised.
+In any case the single Chamber system is impossible. And it is as impossible in the region of finance as in any other. If finace meant in 1909 what it used to mean in earlier days, the question would be unimportant. But directly the need for money is used by a Government as an excuse for adopting the first instalment of a Socialist Budget, for treating property not according to its amount, but according to its origin, and for the vindictive attack on political opponents, then the people have a right to be consulted; and that right could never have been exercised had the Peers not used on behalf of the people the powers entrusted to them by the Constitution.
+If you ask me whether this constitutional machinery could not be improved, either by some change in the composition of the House of Lords, or by the institution of a Referendum, I am certainly not going even to suggest a negative reply. The House of Lords as at present constituted contains, I suppose, more men of first-class eminence in the business of law, of arms, of literature, of science, and of finance, more men who have held great administrative posts overseas, more men in daily touch with local business than the House of Commons. Its debates on great occasions (for reasons in no way derogatory to the Chamber in which I hope to spend all the working days of my political life) are on a more even level of excellence. Nor would it, I think, be wise to turn it into a second and rival House of Commons and make it completely elective. But this does not mean that, even for its comparatively subordiate, though all-important, constitutional functions, it cannot be improved. Nor is any such opinion held by its most distinguished members.
+But schemes of reform, however desirable, are but remotely connected with the present issue. It is not so much the privileges of the Lords which are threatened by the single Chamber plot, as the rights of the people. It is in their interest that the plot must be defeated.
+On the Budget itself I have already said so much elsewhere, that I need say little now. I am interested in it chiefly as it affects security, and through security the prosperity of the country and the employment of its people. For here it touches the problems, or rather groups of problems, which lie at the very heart and centre of social well-being.
+I say groups of problems because unemployment is not a single disease, nor can it be dealt with by a single remedy. It is as complex in its causes as it is tragic in its results. A man may be unemployable through inherited defects of body or mind, through evil training and surroundings, through illness, accident, or age, through the slow deterioration which too often creeps over those who have wasted hope and courage, not in the endeavour to do something, but in the baffled search for something to do.
+Again, a man through employable may be unemployed, either because he and some willing employer do not get into touch, or because there is no demand for the kind of work he is qualified to perform.
+This brief statement is, of course, incomplete; but even as it stands it shows how complicated is the social problem before us. It has long been evident that it cannot be solved through the machinery of the existing Poor Law. Since the Commission appointed by the late Government have reported, it has become plain that the Poor Law machinery cannot even aid in its solution. For every member of that Commission, Unionist and Radical, offical and unofficial, Individualist and Socialist, agreed, after exhaustive inquiries, that the machinery of the Poor Law must be 'scrapped'.
+The task thus imposed upon us must be faced. But it is difficult, and in some respects perilous. The sentimentalist and the doctrinaire, the man who thinkgs that other people's misfortunes are part of an appointed order requiring on his part the exercise of no virtue but resignation; the enthusiast who is prepared to tax two men out of employment in order to compensate one man for being unemployed - all these represent types of criticism which in an unfavourable hour, may prove formidable to the best considered schemes. In truth, this great and pressing reform requires caution as well as courage. If we succeed, the amount of suffering which may be cured or prevented is beyond computation. If we fail (but I think we shall not), we may end by increasing the very ills we desire to remedy.
+It is important, however, to observe that State-organised methods of dealing with destitution, either by way of prevention or cure, can do little directly to promote the market demand for labour. They may add to the labour supply - as by turning the unemployable into the employable. They may render the supply more available - as by the stablishment of labour exchanges. They may increase the number of workmen weeking for employers, but they will not increase the number of employers seeking for workmen. Yet, surely, this is at least as important an object as is the other. If the wise and humane treatment of those who cannot support themselves belong to social pathology, the encouragement of enterprise belongs to social hygiene. And how from this point of view do the fiscal policies compare of Government and Opposition?
+The Budget, now waiting the sentence of the people, seems designed of set purpose to make every man who has invested his money in this country consider how he can remove it, and every man who is hesitating where to invest it, determine to invest it abroad. The super-tax frightens some, the new death duties cripple others, and worse then all, the origin of the proposals and the principles on which they have been defended, show clearly how thin is the dividing line which separates the policy of the Government from that of the avowed Socialists.
+Such is, and must be, the effect of the Budget and Budget speeches on the mind of the investor. Very different are the results I anticipate from Tariff Reform.
+There are those who regard it as a paradox to say that Tariff Reform will stimulate home industry. It seems to me a truism. Only by Tariff Reform can you hope to retain colonial preference; only by Tariff Reform can you hope to modify commercial treaties in your favour. Only by Tariff Reform can you secure from unfair competition the home producer in the home market. It will do him no injury in neutral markets, it may give him valuable aid in protected markets. Is it credible, then, that it will not keep capital here that would otherwise go abroad? Is it credible that, if it does, the demand for labour will not increase?
+On other aspects of Tariff Reform I will here say nothing. The very fact that it is the first 'plank' in the Unionist programme has prevented it every receiving less than its due need of attention, whether from friends or foe.
+But some observation on land I must make; for on the subject of land no absurdity in argument, and no folly in legislation, seems wholly ruled out of court.
+The Government began their career by loudly proclaiming the doctrine known as 'Back to the land'. It might have been supposed, in these circumstances, that they would have done their best to make the position of the small cultivator as attractive as possible. Not at all. The life on the small cultivator living solely on his holding is often a hard one - harder often than that of the agricultural labourer. He is not within easy reach of the urban amusements which attract so many, and in our climate the risks of weather can neither be forgotten nor escaped. These are disadvantages. But there is one great advantage of ownership. The hope of this may bring him to the land. The enjoyment of it may keep him there. But it is just this that the Government in their wisdom refuse to give him. They have some vague idea that private ownership in land is a thing to be discouraged. They do not, I gather, think it criminal, like Henry George. They do not argue, like the land nationalists, that since 'the earth is the Lord's' therefore its rents should go to the Chancellor of the Exchequer. But they do apparently think ownership a little discreditable except in the case of the Irish farmer. To make him a proprietor, British credit may, indded, be lavishly employed. But a different policy is good enough for Britain. Here the possession of land is treated almost as an abuse. Those who indulge in it shall be made to pay: and nothing shall be done to increase their number.
+This being, so far as I can make out, their view, they insist that the small holders should be tenants and (in England at least) tenants of a public body. now there is not a farmer of sense in the whole of Great Britain who would not reather be a tentant of Mr Lloyd George's favourite duke than of any public authority from Caithness to Cornwall. Their whole way of looking at the problem is illogical and absurd. If it be desirable that money should be spent on the land with slight hopes of profit, property in land should not be talked of as an abuse. If it be desirable that small cultivators should give long hours of toil to the development of their holdings, the reward of possession should be within their reach.
+In this address I am compelled to restrict myself to broad constitutional issues and certain great social and financial problems. I am thus perforce constrained to be silent about the navy, but this is of the less importance, as I have spoken more than once in the City upon this great theme since the perilous position of the country first became evident earlier in the year. The situation remains grave and the future is anxious. I do not think the public will readily forget or forgive the lamentable negligence which so dangerously encouraged the very rivalry in shipbuilding which they have so often and, I doubt not, so sincerely deplored.
+Here, then, I close what is not and cannot be more than an indication of certain important portions of the policy which I trust our party will pursue. To maintain the Empire, the Union and the Constitution, these are among the traditional obligations of the party which gain rather than lose in force as time goes on. But we have more to do than merely to preserve what we have received. The world moves, new conditions arise, problems of Empire, problems of trade, problems of national finance, problems of national defence, problems of social amelioration meet us in forms not dreams of a few years since. They must be solved each in its own appropriate way. But, diverse as they are, it will, I think, be found that no substantial advance can be made towards the solution of any one of them, till a change of Government takes place, and a party is returned to office prepared to press through to the utmost of its powers they policy of Tariff Reform.</t>
+  </si>
+  <si>
+    <t>http://www.conservativemanifesto.com/1910/dec/december-1910-conservative-manifesto.shtml</t>
+  </si>
+  <si>
+    <t>In less than a year since the last General Election the Government has resolved again to appeal to the country. They have selected the season at which the register least accurately represents the constinuencies, and which is most inconvenient to trade; and have done so without the excuse of a Parliamentary defeat in either House, and with no visible breach in the strange coalition of parties which keeps them in office.
+It is in these circumstances that I ask you for the third time to honour me with your suffrages. I have little to add to the detailed statment of my views, which I sent to every elector for the City of London last December. Now, as then, Tariff Reform, National Defence, and wider extension of freehold ownership, Poor Law and other social reforms, are vital parts of the programme, to which the party with which I am connected stands pledged. Now, as then, we are resolved that the party of revolution shall not, under the thin disguise of an attack on the Upper House, impair the liberties of the people. Our principles on this last subject are plain, and we share them with all the great men who have helped to develop our Constitution, or have been concerned in framing free institutions for self-governing communities beyond the limits of these islands. Nor would the Ministry, even in the Parliament now drawing to a close, have obtained serious support for their destructive policy were it not forced upon them by their Socialist and Nationalist allies. It is because both Nationalists and Socialists are aware that their darling projects are not in harmony with the considered will of the people that they press for the abolition of the only Constitutional safeguard which at critical moments will enable that will to prevail.
+Behind the Single Chamber conspiracy lurk Socialism and Home Rule. The alternative scheme of Reform which we desire to see adopted has, in spite of the Government, now been brought to the notice of the country. It is true that a full Parliamentary discussion of it has been made impossible by the date selected for the Dissolution. It is also true that in consequence the constituencies have not enjoyed that assistance in judging of its merits which they had a right to demand. Yet I cannot doubt that if they fairly survey the constructive programme which the Unionist Party offers them - fiscal, social, Imperial, and Constitutional - they will feel that on these lines, and on these lines only, is ordered progress possible.</t>
+  </si>
+  <si>
+    <t>The Coalition Government, supported by the strenuous and united labours of the whole nation, has now accomplished the gravest portion of its task. Our enemies have been defeated in the field, their armies are broke, and their Governments are over-turned. Thanks to the patient valour of the hosts of freedom, the knell of military autocracy has sounded forever in the Continent of Europe. Other tasks directly arising out of the war now await our nation, and can only be surmounted by the good sense, the patriotism, and the forbearance of our people. The unity of the nation which has the patriotism, and the forbearance of our people. The unity of the nation which has been the great secret of our strength in war must not be relaxed if the many anxious problems which the war has bequeathed to us are to be handled with the insight, courage, and prompritude which the times demand.
+As a preliminary to the soltuion of these problems it is essential that a fresh Parliament should be summoned, possessed of the authority with a General Election alone can give it, to make the peace of Europe and to deal with the difficult transitional period which will follow the cessation of hostilities. Indeed, the present Parliament has long outstayed its appointed term, and meanwhile millions of new voters, including for the first time representatives of the womanhood of the country, have been added to the electorate. It is right that the Government, upon whom it devolves in conjunction with our Dominions and our allies to settle the political future of Europe, should be supported by the confidence of the vast body of newly enfranchised citizens.
+We appeal, then, to every section of the electorate, without distinction of party, to support the Coalition Government in the execution of a policy devised in the interests of no particular class or section, but, so far as our light serves us, for the furtherance of the general good. Our first task must be to conclude a just and lasting peace, and so to establish the foundations of a new Europe that occasion for further wars may be for ever averted. The brilliant and conclusive triumph of the Allied Armies will, we hope, render it possible to reduce the burden of our armaments and to release by successive and progressive stages the labour and capital of the Empire for the arts of peace. To avert a repetition of the horrors of war, which are aggravated by the onward march of science, it will be the earnest endeavour of the Coalition Government to promote the formatino of a League of Nations, which may serve not only to ensure society against the calamitous results of militarism but to further a fruitful mutual understanding between the associated peoples. Never have the men and women of our race played so great and commanding a part in the affairs of the whole world as during the tempests and trials of this great war, and ever has the British name been so widely honoured.
+The care of the soldiers and sailors, officers and men, whose heroism has won for us this great deliverance, and who return to civil life, is a primary obligation of patriotism, and the Government will endeavour to assist such members of the armed forces of the Crown as may desire to avail themselves of facilities for special industrial training and to return to civil life under conditions worthy of their services to the country. Plans have been prepared, and will be put into execution as soon as the new Parliament assembles, whereby it will be the duty of public authorities and, if necessary, of the State itself to acquire land on simple and economical basis for men who have served in the war, either for cottages with gardens, allotments, or small holdings as the applicants may desire and be suited for, with frants provided to assist in training and initial equipment. In addition to this, we intend to secure and to promote the further development and cultivation of allotments and small holdings generally so far as may be required in the public interest.
+Increased production must necessarily be the basis of all schemes for the improvement the conditions of the people. The war has revealed the extent to which the resources of the country have been dissipated and depressed by lack of organisation or by wasteful organisation. It has been demonstrated that the land of the country, if properly cultivated and used, could have yielded food and other products of the soil to a much larger extent. It must be among the first tasks of the new Government to repair this error, which added so much to our difficulties in our struggles against the submarines of the enemy.
+The war has given fresh impetus to agriculture. This must not be allowed to expire. Scientific farming must be promoted, and the Government regard the maintenance of a satisfactory agricultural wage, the improvement of village life, and the development of rural industries as essential parts of an agricultural policy. Arrangements have been made whereby extensive afforestation and reclamation schemes may be entered upon without delay. A systematic improvement in the transport facilities of the resources of the soil, and the Government are preparing plans with a view to increasing these facilities on a large scale.
+The principal concern of every Government is the must be the condition of the great mass of the people who live by manual toil. The steadfast spirit of our workers, displayed on all the wide field of action opened out by the war - in the trenches, on the ocean, in the air, in field, mine, and factory - has left an imperishable mark on the heart and conscience of the nation. One of the first tasks of the Government will be to deal on broad and comprehensive lines with the housing of the people, which during the war has fallen so sadly into arrears, and upon which the well-being of the nation so largely depends. Larger opportunities for education, improved material conditions, and the prevention of degrading stndards of employment; a proper adaption to peace conditions of the experience which during the war we have gained in regard to the traffic in drink - these are among the conditions of social harmony which we shall earnestly endeavour to promote. It will be the fundamental object of the Coalition to promote the unity and development of our Empire and of the nations of which it is composed, to preserve for them the position and influence and authority which they have gained by their sacrifices and efforts in the cause of human liberty and progress, and to bring into being such conditions of living for the inhabitants of the British Isles as will secure plenty and opportunity to all.
+Until the country has returned to normal industrial conditions it would be premature to prescribe a fiscal policy intended for permanence. We must endeavour to reduce the war debt in such a manner as may inflict the least injury to industry and credit. The country will need all the food, all the raw material, and all the creidt which it can obtain, and fresh taxes ought not to be imposed on food or upon the raw materials of our industry. At the same time a preference will be given to our Colonies upon existing duties and upon any duties which, for our own purpose, may be subsequently imposed. One of the lessons which has been most clearly taught us by the war is the danger to the nation of being dependent upon other countries for vital supplies on which the life of the nation may depend. It is the intention therefore of the Government to preserve and maintain where necessary these key industries in the way which experience and examinatino may prove to be best adapted for the purpose. If production is to be maintained at the highest limit at home, security must be given against the unfair competitino to which our industries may be subjected by the dumping of goods produced abroad and sold on our market below the actual cost of production. The military institutions of the country must necessarily be dependent upon the needs of the Empire and the prospective requirements of any League for the preservation of peace to which this country may hereafter be a party. Meanwhile it will be the aim of the Government to carry through the inevitable reductions in our military and naval establishments with the least possible suffering to individuals and to the best advantage of industry and trade.
+Active measures will be needed to secure employment for the workers of the country. Industry will rightly claim to be liberated at the earliest possible moment from Government control. By the development and control in the best interest of the State of the economical production of power and light, of the railways and the means of communication, by the improvement of the Consular Service, and by the establishment of regular machinery for consultation with representative trade and industrial organisations on matters affecting their interest and prosperity, output will be increased, new markets opened out, and great economies effected in industrial production.
+It will be the duty of the new Government to remove all existing inequalities of the law as between men and women.
+It has been recognised by all parties that reform is urgently required in the constitution of the House of Lords, and it will be one of the objects of the Government to create a Second Chamber which will be based upon direct contract with the people, and will therefore be representative enough adequately to perform its functions.
+The people of this country are not unmindful of the conspicuous services rendered by the Princes and people of India to the common cause of civilisation during the war. The Cabinet has already defined in unmistakeable language the goal of British policy in India to the development of responsible government by gradual stages. To the general terms of that declaration we adhere and propose to give effect.
+Ireland is unhappily rent by contending forces, and the main body of Irish opinion has seldom been more inflamed or less disposed to compromise than it is at the present moment. So long as the Irish question remains unsettled there can be no political peace either in the United Kingdom or in the Empire, and we regard it as one of the first obligations of British statesmanship to explore all practical paths towards the settlement of this grave and difficult question on the basis of self-government. But there are two paths which are closed - the one leading to a complete severance of Ireland from the British Empire, and the other to the forcible submission of the six counties of Ulster to a Home Rule Parliament against their will. In imposing these two limitations we are only acting in accordance with the declared views of all English political leaders.
+It is a source of pride to be of this age, and to be members of this nation. In the whole course of the world's history no generation has been compelled to face sacrifices such as we have steadfastly endured, or perils such as we have victoriously confronted. Well and truly have rich and poor, castle and cottage, stood the ordeal of fire. Right earnestly do we trust that the united temper, the quiet fortitude, the high and resolute patriotism of our nation may be long preserved into the golden times of peace.</t>
+  </si>
+  <si>
+    <t>His Majesty has been graciously pleased to appoint me First Minister of the Crown. I appeal to you to renew your confidence in myself as your representative, and to give your support to the new Government of which I am the head. The crisis which has arisen so suddenly has made it absolutely necessary that an immediate appeal should be made to the people, and in consequence it has been impossible to have an examination with my colleagues into the many questions with which we have to deal. Of necessity, therefore, the outlines of policy which I now submit to you cannot be as definite and precide as in other circumstances would have been possible.
+The crying need of the nation at this moment - a need which in my judgement far exceeds any other - is that we should have tranquility and stability both at home and abroad so that free scope should be given to the initative and enterprise of our citizens, for it is in that way far more than by any action of the Government that we can hope to recover from the economic and social results of the war.
+With this in view I think it is of the utmost importance that we should return as quickly as possible, to the normal procedure which existed before the war. In pursuance of this aim I am satisfied that the time has now come when a change should be made in the machinery of the central Government. Some of the work which has hitherto been done by the Cabinet Secretariat is essential and must be continued, but we intend to bring that body in its present form to an end, and I am certain that the necessary work can be continued, and the invaluable services of the present Secretary retained, in connection with the Treasury, which in the past has always been the central department of Government. As an illustration of the changes which we contemplate, instructions have been already given to transfer to the Foreign Office the machinery of the League of Nations, and in the same way to arrange, as regards any future International Conferences, that even where it is necessary that I as Prime Minister should be present, the machinery of the Conferences and the preliminary work in connection with them will be performed not by the Cabinet Secretariat but by the Foreign Office itself.
+At the present moment the first foreign interest not alone of Great Britain and of the British Empire, but of the world, is the re-establishment of peace. In all our foreign relations we intend to pursue an even course, loyally fulfilling the obligations we have undertaken, but resolutely determined not to extend our commitments, and should reasonable occasion arise to curtail them. It was by wholehearted co-operation, often under great difficulty, and with great differences of opinion, that we won the war. It is only by the same frank and full co-operation, conducted in the same spirit, with France and our other great Allies, that we can hope to solve the difficult problems with which we are not confronted. It is my confident hope that under the well-tried guidance of the Secretary of State for Foreign Affairs the negotiations for the settlement of the Near Eastern crisis will result in a true and lasting peace, conducing both to the political tranquillity of the Near and Middle East, with which so many of our Imperial interests are bound up, and to the personal security and happiness of the inhabitants of all races and creeds in the regions which have been the scene of so much disturbance and suffering.
+During the war the feeling supreme in the minds of men and women throughout the world was that a similar calamity should never again be allowed to fall upon mankind. It was to meet this feeling that the League of Nations was instituted, and it will be our earnest aim to give it wholehearted and practical support. The maintenance of our friendship and good understanding with the United States, based not on any formal friendship and good understanding with the United States, beased not on any formal friendship and good understanding with the United States, beased not on any formal alliance but on community of inherited ideals as well as on recent comradeship in arms, must always be a princial aim of British policy. Above all, we mean, in all matters affecting the external policy or security of the Empire, to act in close and continuous consultation with the Governments of the Dominions and of India in order to ensure that our policy shall keep fully in view both the interests and sentiments of our fellow subjects overseas, and at all times have behind it the moral support of the whole British Commonwealth.
+Our first task, if returned to power, will be the ratification of the Irish Treaty. We are prepared to take our part in making good that Treaty, both in the letter and in the spirit, and to co-operate with the Irish Government in the new relationship within the Empire which the Treaty will have created. We are equally pledged to safeguard the freedom of choice and the security of the Parliament and Government of Northern Ireland. We earnestly hope that further progress will be made in dealing with the anarchy in the South, and that both in the North and in the South it will be realised that the prosperity of Ireland as a whole can only be achieved by good will between the Governments and peoples of the two portions of that country. The position of the innocent victims of recent disturbances is a matter of the gravest concern to the people of this country, and it will be the duty of the Government to keep in the closest touch with the Government of the Irish Free State on this matter, so that just claims for compensation may have sympathetic consideration.
+We desire to promote the quiet and orderly development of India under the constitution which was conferred on her by the Act of 1919. The co-operation of all classes and sections is essential to the progress and prosperity of India, and, if that be secured, we can look forward with confidence to an industrial development which will add to her resources and give increased stability to her economic structure.
+At home our chief preoccupation at this time is the state of trade and employment. The immediate problem of unemployment this winter will call for emergency measures. Plans for dealing with the situation have already been considered by the late Government. They will be examined afresh by us with a view of seeing whether any improvements are possible, and the necessary steps will then be taken with the least avoidable delay. Such remedies, however, can only be palliatives, and the real recovery will not come except from the revival of trade and industry. To secure this result, the first eessential is to reduce expenditure to the lowest attainable level in the hope that the taxpayer may find some relief from the burden fo taxation which not only presses so heavily upon individuals, but is the greatest clog upon the wheels of national industry.
+Every Candidate, in every constituency, will, as I do, make retrenchment an essential part of his programme. All that I can possibly say, knowing how great are the difficulties, is that we should do our best to secure it. It will also be our endeavour in any way in our power to help trade, and the method of doing this, which seems to me most helpful, is the development of trade within the Empire itself. The markets, which for the time at least, as a consequence of the war, we have lost in Europe, can best be replaced by further development of trade with overseas countries, and especially of trade within the British Empire. We propose, therefore, immediately to consult the Governments of the self-governing Dominions and, if they approve, to summon, as early as possible, an Economic Conference with the view of finding in what way by mutual co-operation we can best develop the vast trade of which, in my opinion, the resources of the Empire admit.
+There is one branch of industry to which I must specially refer. As a consequence of the war, agriculture, the greatest of our national industries, is in a most serious condition, and demands the practical sympathy of the Government. It is not easy to specify the exact method by which that sympathy can be shown, but we shall immediately examine the whole problem afresh in the hope of making proposals which will assist the agricultural community to overcome the difficulties that now confront them.
+There are many measures of legislative and administrative importance which, in themselves, would be desirable, and which, in other electorate. But I do not feel that they can, at this moment, claim precedence over the nation's first need, which is, in every walk of life, to get on with its work with the minimum of interference at home and of disturbance abroad.</t>
+  </si>
+  <si>
+    <t>In submitting myself to you for re-election, I propose frankly to put before you the present situation as I see it, and the measures which in the opinion of myself and my colleagues are necessary adequately to deal with it.
+The unemployment and under-employment which our working people and our great national industries are now facing for the fourth winter in succession, on a scale unparalleled in our history, having created a problem which calls urgently for a solution. Their indefinite continuance threatens to impair permanently the trained skill and the independent spirit of our workers, to disorganise the whole fabric of industry and credit, and, by eating away the sources of revenue, to undermine the very foundations of our national and municipal life.
+In large measure this state of affairs is due to the political and economic disorganisation of Europe consequent on the Great War. In accordance with the policy affirmed by the Imperial Conference we shall continue to devote every effort through the League of Nations and by every other practical means, to the restoration of a true peace in Europe. But that at the best must take time. A year ago Mr Bonar Law could still hope that a more settled condition of affairs was in prospect, absence of any modification of fiscal policy, of the ultimate necessity of which he himself was always convinced. Since the occupation of the Ruhr it has become evident that we are confronted by a situation which, even if it does not become worse, is not likely to be normal for years to come.
+The disorganisation and poverty of Europe, accompanied by broken exchanges and by higher tariffs all the world over, have directly and indirectly narrowed the whole field of our foreign trade. In our own home market the bounty given to the importation of foreign goods by depreciated currencies, and by the reduced standard of living in many European countries, has exposed us to a competition which is essentially unfair and is paralysing enterprise and initiative. It is under such conditions that we have to find work for a population which, largely owing to the cessation during the war period of the normal flow of migration to the Dominions, has in the last census period increased by over a million and three quarter souls.
+No Government with any sense of responsibility could continue to sit with tied hands watching the unequal struggle of our industries or content itself with palliatives which, valuable as they are to mitigate the hardship to individuals, must inevitably add to the burden of rates and taxes and thereby still further weaken our whole economic structure. Drastic measures have become necessary for dealing with present conditions as long as they continue.
+The present Government hold themselves pledged by Mr Bonar Law not to make any fundamental change in the fiscal system of the country without consulting the electorate. Convinced, as I am, that only by such a change can a remedy be found, and that no partial measures such as the extension of the Safeguarding of Industries Act, can meet the situation, I am in honour bound to ask the people to release us from this pledge without further prejudicing the situation by any delay. That is the reason, and the only reason, which has made this election necessary.
+What we propose to do for the assistance of employment in industry, if the nation approves, is to impose duties on imported manufactured goods, with the following objects:-
+to raise revenue by methods less unfair to our own home production which at present bears the whole burden of local and national taxation, including the cost of relieving unemployment.
+to give special assistance to industries which are suffering under unfair foreign competition;
+to utilise these duties in order to negotiate for a reduction of foreign tariffs in those directions which would most benefit our export trade;
+to give substantial preference to the Empire on the whole range of our duties with a view to promoting the continued extension of the principle of mutual preference which has already done so much for the expansion of our trade, and the development, in co-operation with the other Governments of the Empire, of the boundless resources of our common heritage.
+Such a policy will defend our industries during the present emergency and will enable us, as more normal conditions return, to work effectively to secure a greater measure of real Free Trade both within the Empire and with foreign countries. Trade which is subject to the arbitrary interference of every foreign tariff, and at the mercy of every disturbance arising from the distractions of Europe, is in no sense free, and is certainly not fair to our own people.
+It is not our intention, in any circumstances, to impose any duties on wheat, flour, oats, meat (including bacon and ham), cheese, butter or eggs.
+While assisting the manufacturing industries of the country we propose also to give a direct measure of support to agriculture. Agriculture is not only, in itself, the greatest and most important of our national industries, but is of especial value as supplying the most stable and essentially complementary home market for our manufacturers.
+We propose to afford this assistance by a bounty of £1 an acre on all holdings of arable land exceeding one acre. The main object of that bounty is to maintain employment on the land and so keep up the wages of agricultural labour. In order to make sure of this we shall decline to pay the bounty to any employer who pays less than 30/- a week to an able-bodied labourer.
+The exclusion from any import duties of the essential foodstuffs which I have mentioned, as well as of raw materials, undoubtedly imposes a certain limitation upon the fullest extension of Imperial Preference. But even the preferences agreed to at the recent Economic Conference within our existing fiscal system, have been acknowledged as of the greatest value by the Dominion representatives, and our present proposals will offer a much wider field, the value of which will be progressively enhanced by the increasing range and variety of Empire production.
+Moreover in the field of Empire development, as well as in that of home agriculture, we are not confined to the assistance furnished by duties. We have already given an earnest of our desire to promote a better distribution of the population of the Empire through the Empire Settlement Act, and at the Economic Conference we have undertaken to co-operate effectively with the Government of any part of the Empire in schemes of economic development. More especially do we intend to devote our attention to the development of cottom growing within the Empire, in order to keep down the cost of a raw material essential to our greatest exporting industry.
+These measures constitute a single comprehensive and inter-dependent policy. Without additional revenue we cannot assist agriculture at home, but the income derived from the tariff will provide for this and leave us with means which can be devoted to cotton growing and other development in the Empire, and to the reduction of the duties on tea and sugar which fall so directly upon the working class household.
+For the present emergency, and pending the introduction of our more extended proposals, we are making, and shall continue to make, every effort to increase the volume of work for our people. The Government are spending very large sums on every measure of emergency relief that can help in this direction. Further, the local Authorities of all kinds throughout the country, and great individual enterprises, such as the railways, with the assistance of the Government, or on its invitation, are co-operating wholeheartedly in the national endeavour to increase the volume of employment. This great combined effort of the Government, of the Local Authorities, and of individual enterprises, represents an expenditure of no less than £100 millions sterling.
+The position of shipbuilding, one of the hardest hit of all our industries, is peculiar. It can only recover as shipping revives with the development of Empire and foreign trade which we believe will follow from our measures. We propose in the meantime to give it special assistance by accelerating the programme of light cruiser construction which will in any case become necessary in the near future. We are informed by our Naval advisers that some light cruisers will be required during the next few years in replacement of the County class, as well as a variety of smaller and auxiliary craft, and we intend that a substantial proportion of these shall be laid down as soon as the designs are ready and Parliamentary sanction secured.
+The solution of the unemployment problem is the key to every necessary social reform. But I should like to repeat my convictino that we should aim aim at the reorganisatino of our various schemes of insurance against old age, ill-health and unemployment. More particularly should we devote our attention to investigating the possibilities of getting rid of the inconsistencies and the discouragement of thrift at present associated with the working of the Old Age Pensions Act. The encouragement of thrift and independence must be the underlying principle of all our social reforms.</t>
+  </si>
+  <si>
+    <t>The Socialist minority Government have forced a rush election upon the country not upon any great issue of principle, such as was submitted to you a year ago, but on the plea that it was incompatible with their dignity to tolerate any inquiry into their conduct in connection with the withdrawal of the Campbell prosecution.
+The admissions already extorted from Ministers in Parliament are sufficient to convince any reasonable person that it was as a result of undue political pressue that the Attorney-General withdrew a prosecution instituted on the grave charge of inciting the troops to sedition and mutiny. The refusal to allow any inquiry inevitably suggests that the result of such investigation would only have been to emphasise the conclusions that the course of justice had been deflected by partisan considerations and to increase the public anxiety.
+There are, however, other considerations which may well have influenced the Government in their decision to precipitate an election. Under pressure from the same extremist section which reversed the considered action of the Attorney-General in the Campbell case - and, indeed, at the same moment - the Government, going back upon its own better judgement and upon the assurances given by the Prime Minister in Parliament, hurriedly patched up a makeshift Treaty with the Soviets which they now realise to be no less indefensible and no less incapable of standing close scrutiny. Under that Treaty the rightful claims of British subjects are whittled down to an undefined extent, and Parliament is to be asked to commit itself in the eyes of Russia and of the world, to the principle of guaranteeing that the British taxpayer shall repay a Bolshevik loan, if the Bolsheviks, in accordance with their principles and their practice, should fail to repay that loan.
+By dissolving Parliament the Government are, no doubt, also hoping to obscure their utter failure to deal with unemployment, or to make good the boast that they possessed the only positive remedy for that most serious of all problems of the day. The unemployment situation is as grave, if not graver, than it was a year ago, and more economic policy of the present Government, as distinguished from the measures initiated by ourselves and carried on by our successors, has had time to take effect, unemployment has steadily increased. At the end of September the unemployment figure was 180,000 higher than at the end of June, and is, I fear, still rising. In this disquieting situation the Government have no remedy whatsoever to propose, beyond mere palliatives or an increase of doles.
+The folly committed by the Government of choosing such a time in order to abolish the McKenna duties and Part 2 of the Safeguarding of Industries Act, under which certain industries were rapidly expanding and giving increasing employment, and the even greater folloy of wrecking the hopes of the rapid expansion of Imperial trade which would have followed on the adoption of the proposals of the Imperial Economic Conference, are now only too clearly evident.
+The Unionist Party would be unfaithful to its principles and to its duty if it did not treat the task of grappling with the unemployment of our people and with the serious condition of industry as a primary obligation. While a general tariff is no part of our programme, we are determined to safeguard the employment and standard of living of our people in any efficient industry in which they are imperilled by unfair foreign compeition, by applying the principle of the Safeguarding of Industries Act or by analogous measures. Without such provision the carrying out of the policy embodied in the Dawes Report, in itself desirable as calculated to secure German reparations and to restore stable economic conditions in Europe, might only prove disastrous to ourselves.
+The burden of taxation weighs heavily upon industry and trade, diminishes real wages, and in a variety of ways adds to the cost of living. To assist in relieving the community of this burden, the most rigid economy in administration is essential.
+Pending the restoration of trade, our duty will be to continue to take all the special relief measures in our power to ease the situation. More particularly do I feel that the grave problem of juvenile unemployement requires fuller and more careful consideration than it has received from the present Government.
+The best hope of industrial revival lies, however, in my opinion, in the development of the resources and trade of the British Empire. The policy of encouraging mutual trade in the Empire by measures of Imperial Preference, and of using our finance to promote Empire Development and Empire Settlement, is one of which we adhere, and which we shall steadily keep the front.
+To strengthen and develop the Empire by every possible means is, indeed, the first and dominant item in our policy, believing, as we do, that only through the fullest co-operation of the partner states of the British Commonwealth can the common peace, security and prosperity of each and all of us be assured.
+We favour the progressive grant of constitutional liberties in every part of the Empire where the capacity and loyalty of the people will make such measures a benefit to themselves and a strngth to the Empire. But we are no less determined to maintain the authority and the unity of the Empire against factious and misguided agitation wherever it may asset itself.
+The same principles must underly our policy in relation to the outside world. The foreign policy of this country must be such as will comment itself to the Dominions and must be carried on in closest consultation with their Governments. We stand for the maintenance of the most friendly relations with our Allies, for the re-establishment of a settled state of affairs in Europe and for co-operation in all matters admitting common action with the United States of America. The support and strngthening of the League of Nations on practical fines should, in our opinion, continue to be a cardinal principle of British foreign policy, subject always to the overriding consideration that we cannot enter into any commitments involving issues of peace and war without the concurrence of the Dominions which would inevitably be affected by them.
+The maintenance of our security at sea, on land and in the air is one of the first duties of any Government, and the Unionist Party, if returned to power, will have to examine afresh the position in which the defences of the Empire have been left by the present Administration. While in favour of any practical proposals for a general limitation of armaments, we shall have to scrutinise carefully in conjunction with the Dominions, the far-reaching commitments and implications of the scheme recently put forward at Geneva.
+I regard it as vital that the great basic industry of agriculture should be not merely preserved, but restored to a more prosperous condition as an essential balancing element in the economic and social life of the country. For a permanent solution of the agricultural problem, a common agreement between all parties is desirable; and the Unionist Party, if returned to power, will summon a representative Conference in the hope of arriving at an agreed policy by which the arable acreage may be maintained and regular employment and adequate wages secured to the agricultural worker. The Act for the regulation of wages, passed in the last session of Parliament, will be maintained. Unionists can justly claim to have been instrumental in passing this Act in a form more generally acceptable to all agriculturists.
+We shall continue to agricultural ratepayers the relief already given during our previous tenure of office.
+We shall support the provision of agricultural credit for all forms of efficient, co-operative enterprise.
+The interests of the Fishing Industry will not be neglected, and with that object in view the provisino of further and extended credit facilities in this direction will be the subject of enquiry.
+The interests of the Fishing Industry will not be neglected, and with that object in view the provision of further and extended credit facilities in this direction will be the subject of enquiry.
+We shall promote the provision of small and cottage holdings by affording facilities for occupation and ownership, and will encourage the allotment movement with reasonable security for holders.
+We shall seek to make available on easy terms to all cultivators the results of the latest agricultural scientific research.
+We shall take all practical steps to ensure that imported foreign foodstuffs should be sold as such.
+The further development of the sugar beet industry and rural industries generally will receive particular consideration.
+Afforestation and land drainage will be developed and improved rural transport promoted.
+We are opposed to land nationalisation, the taxation of land values, and all schemes of spoliation.
+In short, the purpose of our Party is to protect agriculturists from Socialistic and bureaucratic tyranny, and to secure for them the just reward due to all investment in the soil, whether it be of money, muscle, or brains.
+The problem of the cost of foodstuffs is one which demands careful investigation by a Royal Commission. The importance of any feasible reduction in those costs in its effects, both directly upon the cost of living, and indirectly upon our industrial position, is obvious.
+Next to the problem of unemployment, the gravest of our domestic problems still is the housing problem. The Unionist Act of 1923, under which no less than 161,441 houses have been authorised by the Ministry of Health, has demonstrated that it will produce all the houses for which labour and materials are available with present methods of construction, and the best tribute to its success is that the present Government by the first section of their own Housing Act have prolonged its operation unchanged until the year 1939.
+Something more, however, is required if the rate of building is to be materially increased, and houses are to be produced capable of being let at a rent approaching that which can be afforded by the poorer classes. This end can only be achieved by the employment of new materials and new methods of construction. The Unionist Party, which was the first to recognise the importance of this aspect of the problem, will, if returned to power, do everything possible to foster and develop the various experiments which are not being carried out in these directions, and will not hesitate, if it be necessary, to lend financial aid to bring them to early fruition, recognising that, in this way, and in this way alone, can the provision of the housing accommodation so sorely needed be secured in a reasonable time.
+The Unionist Party is, moreover, determined that side by side with the provision of new houses, the improvement of the slums shall be taken in hand. The conditions in large cities are such that new houses can only be built at a considerable distance from the factories and other places of business at which the occupants work. For many of them, migration into the suburbs would be difficult, if not impossible, on account of the expense and time that would be taken up in travelling to and from their work. It is, therefore, urgently necessary that without waiting until the whole population is rehoused, the standard of existing houses should be made to approximate more nearly to modern ideas, and as soon as the present shortage of accommodation has been sufficiently eased, steps will be taken to carry out this reform.
+Soon after the resignation of the late Government in the early part of the year, I appointed a Committee to investigate a comprehensive scheme of Insurance to cover both Old Age and Widows' Pensions. The three principal defects in the present Old Age Pension scheme are:
+First:	That it involves an investigation into the means of the applicant.
+Second:	That the pensino is reduced where the means exceed a certain annual sum, even though those means result from his own thrift; and
+Third:	That the pension itself is inadequate in amount.
+Most of the proposals for Widow's Pensions also include investigation and supervision of a kind that would be a constant source of irritation and annoyance to the widow. The Committee have come to the conclusion that the only way of avoiding such investigation is, whilst conserving the present rights of old age pensioners, to supplement them by a contributory scheme which would enable the contributor to receive his old age pension at an earlier age and a substantially larger amount. In the same system, provision should be made for the widow with dependent children to receive her pension as a right, for which payment has been made, instead of a dole or a charity. Accordingly, they have caused exhaustive actuarial investigation to be made, and although their labours are not yet completed, they are satisfied that it will be possible to frame a workable scheme. It will be the task of a Unionist Government, returned with an adequate majority, to complete the details of the scheme, and to carry it into operation as soon as practicable.
+Believing that the object of any Education Policy should be the welfare of the child rather than the forwarding of some plan of educational progress, based on social theories, and keeping in mind that our immediate aim should be to develop our existing national system on practical lines, and to link up elementary education more closely with the various forms of advanced study, so taht no child which can profit thereby shall be debarred from doing so by reason of the inability of the parents to pay fees, we are in favour of the carrying out of agreed schemes as between local Education Authorities and the Board of Education which shall ensure, among other matters:
+A progressive Reduction in the size of classes.
+The improvement, or when necessary, the replacement of insanitary schools.
+The development of Central Schools and other forms of education above the Elementary School stage, with an adequate supply in the number of Secondary School places, and a corresponding increase in the number of scholarships and free places, applicable to all advanced courses.
+The maintenance, by agreement between Local Education Authroties and the Teachers, of such scales of salaries as will secure efficient teachers and attract the best men and women to the profession. Such scales, when they have been accepted by Local Education Authorities, to be obligatory.
+The systematic promotion of schemes of adult education under the Local Education Authorities and the further development of all kinds of technical education.
+The maintenance of the rights of parents to have their children brought up in the religion to which they are attached.
+In addition to such questions as Housing and Widows' Pensions, there are certain other reforms affecting women and children that I desire to see carried out. The Probationary system for dealing with offenders should be developed; a Bill to amend the consolidate the Factory and Workshop Acts should be passed; children born out of wedlock whose parents have subsequently married should be legitimised, the law relating to separation and maintenance orders should be amended; equal rights should be ensured to women in the guardianship of children; adoption should be legalised, the number of women police should be increased, and the penalties for criminal assaults against women and children made adequate to the offence.
+The Unionist Party, will not cease to safeguard and further the interest of those who sacriced so much for their country in the Great War, or that of their dependants. The proposals of the present Government for carrying out the recommendatino of the Southborough Committee with regard to the position of Temporary ex-Service Civil Servants will be carefully examined, if we are returned to power, and our conclusions will be presented to Parliament before any action is taken to put them into effect.
+In conclusion, I would appeal to you to help to secure for the country, in this difficult and anxious time, a strong and stable Government, based on an independent majority in Parliament, resolved to maintain the existing constitutional and economic liberties under which Britian has grown great and prosperious, and empowered to solve on practical and commonsense lines the urgent industrial and social problems of the day. The experiment of a minority Government has proved a short-lived failure. But it has afforded sufficient indication of what would be the character of a Socialist Government dependent, not upon other Parties, but upon the extremist section of its own majority, to make it imperative upon all who wish to see the restoration of prosperity and social peace, to unite their efforts in averting such a possibility. The only way in which that can be achieved lies in the return of a solid Unionist majority. I appeal, therefore, to all men and women who desire stable Government to support the broad and national policy that I have outlined and to ensure the return of a House of Commons that will have the will and power to carry it into effect.</t>
+  </si>
+  <si>
+    <t>Four and a half years ago, you returned me to Parliament and to Office as the leader of a great majority. Today it is my duty to lay before you the record of the Conservative and Unionist Government and its policy for the future; and to ask at your hands a renewal of your confidence. The Conservative Government has had to face difficulties and dangers at home and abroad which could not have been foreseen at the last Election. In spite of all obstacles, we have fulfilled the pledges given in 1924, to an extent which no Government has equalled, and as a result of our administration the Empire is more firmly united, the prestige of the country stands higher, the prosperity the welfare of our people is greater than ever before in our history. In submitting myself to the electorate, I make no spectacular promises for a sudden transformation of our social or industrial conditions, but I am resolved to maintain and consolidate the advance already made, to bring to fruition the schemes on which we are engaged, and to carry still further the solid work of reconstruction on which depend the unity of the Empire and the peace and well-being of its people.
+The Imperial Conference of 1926 will remain a memorable landmark in the constitutional development of the British Empire. The policy of any British Government of the future must be based on the principle then laid down: that the unity of the British Commonwealth is to be maintained by unfettered co-operation between its partner members, who enjoy an equal freedom under the Crown. This principle has consistently inspired and shapred our policy. In foreign affairs, in defence, in trade and in migration, we have worked and shall work to promote unity of aim and every form of helpful co-operation with the Dominions.
+Among these forms of co-operation none is of greater importance than the policy of Imperial Preference. That policy we have consistently and successfully pursued from the first moment of our entry into office. Reversing the unwise action of our predecessors, we at once honoured all the undertakings given at the Imperial Economic Conference of 1923, partly by the preferential remission of existing duties, and partly by the establishment of the Empire Marketing Board. The preferences to which we then gave effect have since been stabilised and extended with excellent results. In sugar, tobacco, silk, coffee, cocoa, dried fruits, and wine, there has been a great expansion of Empire products. The Empire Marketing Board has proved its value as a new agency of Imperial co-operation in many ways, and not least by its encouragement of scientific research both in Britain and in the Dominions and Colonies. Throughout the Empire, our policy has met with an appreciative response. The Empire today is by far our best market, buying nearly as much of our manufactures as all foreign countries together. Our opponents both liberal and Socialist, have, by their action in 1924, and by their declarations since, shown their determined hostility to the whole idea of Imperial Preference. We, on the contrary, have demonstrated its great possibilities, and subject to my pledge not to impose any protective taxation on food, we shall continue to promote it as an essential part of our policy of Imperial development
+In working out a policy of Imperial development, we have a special duty towards the vast colonial territories for which the British nation is responsible. That duty was defined at the end of last century by Joseph Chamberlain, when he declared that these territories should be treated as the undeveloped estates of the British Empire to be developed by British capital and British enterprise. Such a task is frequently beyond the unaided resources of the Colony concerned, for trade and population will follow rather than precede the opening up of the country. For this purpose transport must be improved and production must be stimulated by scientific research, but capital expended upon these subjects may often bring in no return for several years.
+We propose, therefore, to extend the expedite the policy already pursued in Africa and elsewhere, which in the past 4.5 years has resulted in so great an expansion in the Colonial market for British produce. A Colonial Development Fund will be created which will assist Colonial Governments in financing approved projects of development.
+While thus fulfilling our responsibilities towards the native populations and towards those of our own race who have linked their fortunes with them, we regard the employment of British capital to finance British enterprise as likely to prove a more fruitful investment for this country than speculative loans or guarantees to a foreign Government which has squandered its own resources in a futile war against capitalism, and which has hitherto shown neither a friendly disposition to us nor any readiness to recognise past obligations.
+This policy of Empire development forms part of a comprehensive programme directed to stimulate trade and to create permanent employment. The following are the main features in that programme.
+First, we are pressing steadily on with our policy of helping special industries. The country has watched with keen interest the progress and effect of safeguarding. Few people are interested in catchwords; they want to judge by practical results. The results of the duties which have been imposed are already apparent. Not only has employment been improved in every one of the safeguarded industries, but coal, steel, engineering, building, transport and other industries have profited by orders received and work created. The employment thus given directly and indirectly has put thousands of men in work, has increased their purchasing power, and has thus benefited the distributive trades. In many cases prices have been reduced because costs of production have fallen with increased output. Exports over the whole range of dutiable articles have materially increased; efficiency has been encouraged; new capital has been introduced; new factories have been built and existing factories have been extended. This expereince has convinced many people of the wisdom of our policy. Our opponents have consistently obstructed it and are committed to its reversal, a step which must throw thousands out of work. We, on the other hand, are determined to continue it. We pledged ourselves at the last Election that there should be no protective taxation of food and that there should be no general tariff. We have kept that pledge and we renew it. Bu, subject to that pledge, we intend that no manufacturing industry, large or small, shall be debarred from presenting its case for a safeguarding duty to an impartial tribunal, which will judge each case on its merits and make recommendations accordingly.
+One of the main purposes of safeguarding duties, as of Empire development is to stimulate the export trade.
+No greater stimulus could, however, be given in this direction than the great scheme of Rating Relief which we have carried through in the face of persistent opposition from our political opponents, and which we are not putting into force. By relieving the whole of productive industry from three-fourths of the burden of rates we have not only swept away an unjust form of taxation but have greatly increased the competitive power of our national industries. This is no temporary or sporadic encouragement. It is on the contrary a continuing benefit, which will add about £27 millions every year to the resources of industry. This unprecedented measure of relief operates universally. The assistance is greatest where the need is greatest; but it is no mere subsidy to the depressed industries. It is an essential feature of the scheme that it should also encourage the prosperous industries on which we rely to create new employment, and the distrbutive industries on which we rely to create new employment, and the distributive trades will benefit by the increased purchasing power of the wage earners.
+One important part of the Rating Reform Scheme has already been brought into operation - the reduction of railway freights. By this means the heavy basic industries have been granted reductions of freights amounting in all to more than £3 millions a year, while agriculture is benefited by similar relief amounting to over £750,000. Already this reduction is having marked effect on the recovery of these industries.
+Here we approach the central problem of our national trade. The heavy basic industries of Britain - the coal, iron and stell group - depend upon the railways. Their traffics can only be carried along the steel track. They employ a fifth of our insured wage earners, contain more than a quarter of the whole number of the unemployed and constitute with cotton and wollens two-thirds of our export trade. It is to this point especially that help must be directed if unemployment is to be swiftly and effectually reduced to normal. The rating relief scheme and particularly the reduction of railway freights and dock dues is designed to afford a special measure of assistance to these industries and to agriculture. The remission of the railway passenger duty in the Budget has enabled the railways to undertake a programme of capital expenditure amounting to £6.5 millions, which will assist to modernise and develop the means of transport, and will facilitate the use of heavier rolling stock. In our view the basic trades of Britain which have to depend on the railways as their principal means of transport ought to have at their disposal facilities at least equal to any transportation system in any part of the world. The Government will take such steps as may seem to them necessary to assist the railways, and the industries concerned, to achieve this end.
+While we attach special importance to railway development we realise the part which our great highways must play in a national transportation system.
+The last five years have seen the building and improvement of roads upon the greatest scale yet known, although our roads are already the best in the world, and we are spending more upon them than any European nation.
+At the present time we are making provisino for an annual expenditure from the Road Fund of £23 millions as compared with £15 millions in the year in which we took office, while the total expenditure on roads out of rates and taxes amounts to approximately £60 millions a year. The percentages of State contribution to the various classes of roads have been increased, and the problem of rural roads have been met by substantial increases in the grants towards them.
+Throughout its tenure of office the policy of the Government has been to encourage and assist highway authorities to pursue a comprehensive and orderly programme of road development, improvement and maintenance.
+We intend to pursue this policy, paying special attention to the improvements which will give immediate assistance to our trade and thus bring in a full return for the money expended, rather than to put in hand hasty and ill-considered schemes which could only lead to wasteful and unfruitment expenditure, and could be of no permanent benefit to the unemployed.
+If modern industry needs an efficient transportation system, it needs no less a fully adequate supply of electrical power. There has been no more remarkable achievement in recent times than the re-organisation of the generation and transmission of electricity in Great Britain which was effected by the Electricity (Supply) Act. Progress under that Act has been rapid. It was passed at the end of 1926; in March, 1927, the Central Electricity Board was established, and by the coming Autumn detailed schemes will have been prepared covering about 97 per cent. of the population of 98 per cent. of the present sales of current. The placing of contracts in respect of the constructional work on the transmission system has been pressed on, and the total value of orders already placed amounts to £8.5 millions, all of which have been placed with British firms. Further substantial orders will be placed during the year and unemployment in the skilled electrical trades is practically non-existent.
+While we are thus directing our policy primarily to the permanent restoration of industrial prosperity, on which the solution of the unemployment problem depends, we have also undertaken a wide range of subsidiary measures designed to enable the unemployed, especially in the depressed areas, to find permanent work.
+Training Centres have been established which have already enabled thousands of men and women to fit themselves for new employment. The system of juvenile unemployment centres has been greatly developed, and more than 250,000 boys and girls have passed through these centres. As a result of these and other measures, the problem of juvenile unemployment has been largely overcome. There is now little unemployment among boys and girls, except in the depressed mining areas, and as a result of the arrangements made while we have been in office, practically every boy in these areas can now attend an unemployment centre when he is unemployed, and there be fitted for a carefully chosen job elsewhere.
+We shall steadily expand our training system, as need requires, and we shall continue to provide money for public works with due regard to the requirements of industry for which the maintenance of public credit is so necessary.
+The policy outlined above has already justified itself. Employment improved under our administration until the Spring of 1926 when, for the first time since the great depression of 1920, the number of unemployed fell below a million. Trade then suffered a severe set-back owing to the General Strike, and the industrial troubles of 1926. In the last two years it has made a remarkable recovery.
+In the insured industries, other than the coal mining industry, there are now 800,000 more people employed and 125,000 fewer unemployed than when we assumed office. The coal industry itself is now reviving; many thousands of miners displaced by the re-organisation of the industry have been absorbed into other industries and there are 150,000 fewer miners unemployed than nine months ago.
+This recovery has been achieved by the combined efforts of our people assisted by the Government's policy of helping industry to help itself. The establishment of stable conditions has given industry confidence and opportunity.
+A new spirit of co-operation is abroad. Fewer days have been lost through trade disputes in 1927 and 1928 than in any year since records were established forty years ago. Negotiations on a friendly basis are proceeding between the partners in industry.
+If such co-operation continues with peace at home and abroad, and if full effect is given to the Government's proposals for helping trade, there is every reason to believe that trade and industry will be placed on a sound basis and that men and women will find permanent employment at their proper trades in steadily increasing numbers.
+This peace and revival in industry opens the way to a revision and improvement of the Factory laws.
+This is the one pledge we gave at the last Election which we have been unable to fulfil. It was impossible to legislate wisely for industry still torn by dissensions and harassed by the uncertainties following the troubles of 1926. In our view the time has now arrived for the enactment of a single and clearly drafted statute which shall protect the health, safety and general welfare of the workers without imposing on industry burdens which might retard its recovery.
+Factory legislation of this kind will complete the work we have already done to give greater security to the partners in trade and industry. By the legislation we have passed during our term of office we have given both to the business tenant and to shop assistants a measure of security which they have long demands. By the Trade Disputes Act the Trade Unions were protected against the misuse of the strike weapon for political and revolutionary ends, and the Trade Unionist has been secured against intimidation and coercion in the free exercise of his industrial and political rights. The threat of the Socialist Party to repeal this Act is in itself a ground for asking the support of the workers for the present Government.
+Our policy for agriculture have been consitently directed, and will continue to be directed, to the relief of burdens, the finding of markets, the provision of credit facilities, and the development of education and research.
+We have crowned the Conservative policy of relieving the essential equipment of agriculture from unfair burdens by the entire remission in England and Wales of local rates on farm land and buildings and in Scotland by an equivalent relief from rates. We have found it possible to advance our programme by bringing this relief into immediate operation. We have thus conferred upon the agricultual industry a benefit of not less than £2.5 millions for the year ending October 1, 1929, and nearly £5 millions in a full year. The substantial rebates railway freight charges for certain agricultural traffics which we have also secured by our de-rating scheme, and the special grants made from the Road Fund towards the maintenance and improvement of roads in rural areas, with consequent relief to local rates, are further instances of the same policy of easing the burdens of agriculture.
+We have endeavoured to improve the farmer's position by helping him to reform the methods of marketing agricultural produce. We are surveying the whole marketing system of the country. New methods of standardised grading and packaging have been introduced and under the Agricultural Produce (Grading and Marking) Act, 1928, agricultural products can now be sold in standard grades under a National Mark. A most successful beginning has been made in the application of the Mark to eggs and certain kinds of fruit and vegetables. Provision has also been made for the marking of imported foodstuffs in suitable cases.
+The policy of preference to the home producer has been steadily pressed by the Empire Marketing Board, and is already showing results. In order to give a lead in this matter by direct Government example, we have decided that in future only homefed beef shall be supplied to the Army, Air Force and Navy in Home Ports during the six months October to March, and that during six months after harvest 25 per cent. of the flour used for those services shall be milled from home-grown wheat.
+We have initiated a long called-for reform in the finance of British agriculture by the Agricultural Credits Acts under which both long term and short term credits are being provided; considerable advantage is already being taken by the farming community of these provisions.
+Large sums have been provided for improving the drainage of agricultural land, and we propose to introduce legislation, based on the Report of the recent Royal Commission, which should give a fresh stimulus to this work.
+Recognising that arable farming has been specially affected by the depression in agriculture, we have vigorously supported and developed the infant sugar beet industry, with results which have already exercised a marked influence on the prosperity of agriculture, particularly in the eastern part of England.
+We have ensured throughout England and Wales that the minimum and overtime rates of wages of agricultural workers prescribed under the Agricultural Wages Act of 1924 are being paid, and where necessary we have secured the enforcement of the Act through the medium of the Courts.
+We have extended the facilities for Small Holdings both for renting and purchase by easy instalments, including a new type of cottage holding, and legislation has also been passed facilitating the provisino of allotments. We also propose to afford the poublic in rural areas improved telephone facilities. The radius from the nearest exchange within which a telephone is provided without extra mileage charge will be extended from 1.5 to 2 miles. Call offices will be provided at some 5,000 rural post offices which have at present neither telegraph nor telephone facilities and at more than 1,000 rural railway stations. The electrification of rural areas will be greatly facilitated by the transmission system provided under the Electricity Act.
+Taken together these measures constitute a practical policy. They have proved, and will increasingly prove, their value as a contribution to the re-establishment of British agriculture. It is a policy which enables the costs of production to be reduced and the marketing of agricultural produce to be improved.
+But such a policy must be assisted by all the resources of modern science and skill. To this end we have greatly extended the provision for agricultural education and research, and have directed the attention of teachers in the elementary and secondary schools to the need for closer co-operation between those schools and the industry of agriculture. The further extension of this work will be one of our main cares.
+We are utterly opposed both to nationalisation of the land and to bureaucratic control, the policies of our Socialist and liberal opponents. We do not believe that these expedients can ever overcome the difficulties confronting the agricultural industry, or bring prosperity to those who live by the land.
+We recognise the great importance of the fishing industry. We have given and shall continue to give financial assistance towards all forms of research beneficial to the industry, including the search for new fishing grounds and the investigations now being conducted into the preservation of fish, its transport and the use of by-products. A start has been made to develop the fisk canning industry.
+We are taking steps to help the herring and inshore fishermen by improving harbour facilities, by lightening the burden of existing loans and by the reduction of harbour dues.
+Share-fishermen have been included in the National Health Insurance scheme and can now qualify for the Contributory Old Age Pensions.
+The Conservative Party regards the prosperity of trade and industry, not as an end in itself, but as a means to improve the condition of the people. During our tenure of office we have carried through a great programme of social welfare and have thus prepared the ground for the further programme which we now lay before the country.
+At the last election a promise was given that a Conservative Government, if returned with an adequate majority, would complete the details of a Contributory Scheme of pensions for widows, orphans and old people at an earlier age, without the irritating enquiries and restrictions that had accompanied the earlier scheme of pensions at 70, and would put this scheme into operation as soon as practicable. That promise was fulfilled in the first nine months of our career and already one and three-quarter million persons have been awarded pensions and allowances under our Act.
+We also promised special attention to the vigorous promotion of housing schemes, and the 930,000 houses which have been built during our term of office, providing accommodation for nearly four millions of people, constitute a record in this respect in the the history of the world.
+Realising that the most pressing need is for houses which can be let at lower rents, we have reduced the subsidy which was keeping up prices, and this measure has been so successful that since it was announced the average cost of a non-parlour house has been reduced by no less than £1.12 shillings. With this encouragement Local Authorities are now placing fresh contracts, and we shall continue to urge them to build houses for the lower paid workers until the shortage, which for this class still remains acute, is completely overcome. Meanwhile, the success already achieved has made it possible to attack with a new prospect of success the formidable problem of the slums which has hitherto baffled all attempts to find a solution.
+Plans for the improvement of the present procedure in slum clearance are far advanced. The present basis of compensation to owners, the unfairness of which has had a delaying effect, will be amended after consulation with the various interests concerned. New powers will be given to local Authorities in England and Wales, enabling them to undertake the re-conditioning of old houses after acquisition and providing for an enlightened system of careful and sympathetic management. Where improvement schemes of this kind are carried out it will be possible so to control the tenancies as to put an end to the exploitation of sub-tenants who occupy furnished or unfurnished rooms and who are often in no position to protect themselves against undue charges. The corresponding problem in Scotland will be dealt with by measures adapted to the special conditions of that country.
+The continuance of these Acts in their present form has created hardship for certain owners of small houses. But, whatever modifications may be made to mitigate their difficulties, the protection afforded to tenants by these Acts will not be removed until the shortage of houses has been overcome sufficiently to warrant such a course.
+By the adjustment of financial relations between Local Authorities and the Exchequer an increased national contribution will be directed to the places mostly in need of it. Under the provisions of the scheme the vast majority of ratepayers will gain materially.
+Under the present administration special attention has been given to mothers and children. The network of ante-natal clinics and infant welfare centres has been greatly extended, and largely owing to these measures infant mortality has been reduced from 75 to 65 per 1,000 of the population. The provisions of the local Government Act may be expected to facilitate further expansion in those places where it is most needed by directing to them an increased proportion of the Exchequer contributions to local expenditure.
+We desire, however, that this expansion should be carried beyond the infant welfare centres, whose work is chiefly concerned with children up to one year old. The school medical service is now providing treatment every year for half a million more school children than in 1924, but there is still a gap between the work of this service and that of the infant welfare centres. Existing agencies, such as nursery schools, have done much, and can do more, to solve this problem, but the gap cannot be bridged by these means alone. While encouraging these agencies, therefore, we shall also immediately undertake a comprehensive enquiry into the best methods of providing for the health and welfare of children between one and five years of age.
+Another enquiry is already being carried out into the causes of maternal mortality, and it is expected that when completed it will throw fresh light upon this grave and urgent problem. In the meanwhile, the Government have come to the conclusion that the maternity benefit under the National Health scheme might be more effectively utilised in the preservation of the health and life of mothers, and they purpose to reorganise this provision so as to ensure that proper and adequate midwifery and medical services shall be available to them.
+Finally, the national provision for child welfare needs to be completed by measures designed to protect the interest of older children. Several Committees appointed during our term of office have examined this question and have recommended important reforms. One of our first measures in the next Parliament will be a Bill to consolidate and improve the Acts relating to children and young people, and to bring them into conformity with enlightened opinion.
+Among the social services which affect only a limited number of the population are the provisions made for the welfare of the Blind. Much has been done to ease the lot of those who are thus afflicted, and many are now enabled by special training to make at least a considerable contribution towards their own support. Pensions are provided at the age of 50 for such as have not sufficient means of their own to be independent, but since at that age it is difficult, if not impossible, for a blind person to take advantage of the training facilities provided, the Government have come to the conclusion that pensions should be made available earlier in life, and if they should be returned to power they will introduce legislation to make the pensionable age 40 instead of 50.
+As at the last election, we are issuing a separate statement of our education policy. In that statement we show the progress we have made in carrying out the pledges we gave four years ago, and we renew those pledges. Further, we place before the electors for the first time a complete and balanced scheme of education which has behind it the support both of education reformers and of the trades and industries of the country. This scheme, for which we shall pass the necessary legislation, will offer to all our people the opportunity to pursue a connected course of study from childhood to manhood, and will give to each phase of education - primary, secondary, technical and university - its proper place in one coherent structure. In this task we need the co-operation of all types of schools and every kind of educational effort, and we therefore pledge ourselves actively to seek an agreed settlement which will enable provided and non-provided schools to work together for the accomplishment of these reforms upon just terms of parnership. We need, too, the speedy completion of the reconditioning of all defective school premises in the interests of the children who attend them, and we propose to bring forward a special measure for this purpose. We need, finally, the services of a teaching profession enjoying security of remuneration and professional prospects and we shall endeavour to complete the work in this direction which has already been carried so far during the past four years.
+The efficiency of our public administration is an essential factor in our national well-being. The changes that have taken place during recent years and the increase in the numbers of women employed have given rise to many difficult problems affecting the Civil Service. We have decided that the time has come when it should be make the subject of a comprehensive enquiry by a Royal Commission.
+By the end of this year the country will have spent on Great War Pensions £913 millions, a sum greater in amount than the combined expenditure of France and Germany on the same object.
+War pensioners have been relieved by the Government's action from any anxiety that the rates of their pensions might be reduced owing to the fall in the cost of living.
+Four hundred thousand officers and men have been given security of pensions for life by the policy of final award which is being, and will be, steadily pursued. Altogether over 800,000 men and women have been made secure in the possession of their war pensions.
+Arrangements have been made whereby exceptional cases of all kinds can and do receive pension beyond the seven years' time limit.
+Great as are the benefits conferred upon the community by the public social services, the happiness of the individual depends primarily upon the conditions of his home life. During the past four years there has been a substantial improvement in those conditions. Over the working population as a whole wage rates have risen slightly while there has been a marked fall in the cost of living.
+The reduction of 6d. in the standard rate of Income Tax, together with the increase in the earned income allowance and in the rates of children's allowances for income tax purposes, has effected a striking diminution in the burden of direct taxation, especially in the case of the family man who is dependent for his livelihood upon his own labours. In the sphere of indirect taxation we have abolished altogether the Tea Duty which has been in existence for 300 years, and by our rearrangement of the Sugar Duties, we have effected a reduction of 1/4d. a lb. in the price of sugar to the consumer, and this reduction has been doubled in consequence of world market conditions. But these contributions to a reduction in the cost of living are far transcended by the general reduction which has taken place as a result of the Government's policy in returning to the Gold Standard. During our term of office wage rates over the working population as a whole have risen slightly while the cost of living has fallen by 10 per cent.</t>
+  </si>
+  <si>
+    <t>are far transcended by the general reduction which has taken place as a result of the Government's policy in returning to the Gold Standard. During our term of office wage rates over the working population as a whole have risen slightly while the cost of living has fallen by 10 per cent. This fall is equivalent to a reduction of £160 millions a year on the household budgets of the insured wage earners of the national alone, and if it is applied to all wages, salaried, old age pensions and war pensions, the increased purchasing power would be the equivalent of £240 millions a year. It is not surprising that there has been a remarkable growth in the savings and investments of the workers.
+This growth in the material prosperity of the home has been accompanied by a series of reforms in our legislation affecting family life. By these reforms, such as the Acts relating to the Adoption of Children, the Guardianship of Infants, Legitimacy and the Age of Marriage, we have sought especially to improve the position of women and children.
+It is the steady improvement in the resources and spending power of the individual home which should form the main object of our national financial policy. Our opponents in all their schemes to gain votes never count the cost in cash or credit. Yet money is the measure of all that can be done. We are told that immense new burdens are to be placed upon the direct taxpayer by the Socialist Party, and formidable drains upon our credit will be made by the Liberals. All this will simply be taken from the common stock, and the saving power and economic energy of the country will be reduced accordingly. We do not think that this is a time for imposing new and heavy taxes and it is certainly most necessary to nourish by every means the financial credit upon which the whole activity of industry and enterprise depends. Instead of placing heavy new burdens upon the taxpayer, the process of strict and steady economies in every branch of the public service must continue to be pursued with the aim of lightening the public burdens and leaving larger sums of money to fructify in the pockets of the people. The large savings which we have made on armaments are already apparent, and it is to be hoped that international agreements and further departmental economies will continue this process in the new Parliament, provided always that national safety is not jeopardised.
+The promotion of peace and disarmament has been the prime object of our foreign policy, and that policy has proved successful over the whole field of foreign affiars. Under the guarantees given by the Treaty of Locarno, security, on which peace depends, has been assured in Europe, and Germany has entered the League of Nations. This security has been extended from Europe to the whole world by the signature of the Kellogg Pact, under which all nations have solemnly undertaken to renounce war as an instrument of policy and so have assumed the obligation to settle international disputes by peaceful means.
+The improvement in the international situation wrought by these important treaties leads us to look with confidence for an early advance towards disarmament. We stand for the reduction and not merely the limitation of armaments and in this field we have set a notable example.
+Despite the emergence of the Royal Air Force as a third fighting service and the additional defence responsibilities we have assumed for the Mandated Territories, the combined strength of the three Services is today substantially lower than the corresponding figure for the Navy and Army before the War.
+Along with this reduction in fighting strength, we have progressively reduced the cost of Imperial Defence, despite the considerable programmes of replacement and rearmament in all three Services necessitated by modern conditions. In 1929-30 the total estimated expenditure on Defence Services shows a reduction of approximately £7.5 millions as compared with the corresponding cost in 1924-25.
+The development of the League of Nations is a cardinal principle of our foreign policy. The importance attached by the present Government to the work of the League is illustrated by the fact that Great Britain has been continuously represented by the Secretary of State for Foreign Affairs on the Council and in the Assembly of the League.
+We welcome, as the fruit of this consistent policy, the advance recently made at Geneva towards an international agreement for the reduction of armaments and we greatly hope for a further advance in this direction on the lines of the proposals fore-shadowed by the representatives of the United States of America.
+As in European and world politics, so also in the special affairs of the Middle and Far East, we have shown our desire and our ability to settle differences and promote friendly relations. In the case of both Turkey and China, where we were confronted with special difficulties, our policy has fully justified itself; it has re-established old friendships and afforded new opportunities for British export trade.
+We shall continue, in every sphere of foreign policy, to act in the closest consultation and co-operation with the Governments of the Dominions. We believe this to be essential if the unity of the Empire and its influence in the councils of the world is to be maintained.
+Finally, we stand for the scrupulous execution of all international engagements, in accordance with the traditions of this country.
+It is for the electors to judge, in the light of our past record, whether we have not faithfully redeemed the promises which we made four and a half years ago. We have striven consistently to build up industrial prosperity on sound and permanent foundations, and to improve the social conditions of our people. The results can be seen in the steady revival of trade, especially in the great basic industries, and in the reduction in the cost of living. The future destinies of the country rest in the hands of the electorate. I am confident that, with the growth of the new spirit of co-operation in industry, the present trade revival will make steady and even rapid progress, provided that British industry is guaranteed a period of stable government and can thus enjoy that confidence in the future without which trade recovery is impossible. If, as I hope, the Conservative and Unionist Party is returned to power with an independent majority, those conditions can be secured. The alternatives are a Socialist Government with, or without, liberal support, or a state of political chaos and uncertainty through the existence of three parties, none of which has a clear majority over the other two. Either of these contingencies would be disastrous to the welfare of industry and to the welfare of the nation as a whole, and I ask the electorate once again to place their confidence in our Party as the only one which can secure stable conditions and ordered progress along sound and practical lines.</t>
+  </si>
+  <si>
+    <t>The decision of the Nation four years ago to put its trust in a National Government formed from various Parties in the State, was a turning point in the history of Britain and has exercised a profound influence upon the course of international events. Under this leadership we have emerged from the depths of depression to a condition of steadily returning prosperity, and the name of Britain stands high in the councils of the world. There now falls upon the people of this country the grave responsibility of exercising a choice which may well prove equally momentous for the future.
+The broad issue is whether the stability and confidence with the National Government have built up are to be preserved in a period of special difficulty and anxiety. But we have considered it right, for the information of the Electors, to set forth on behalf of a united Government their general aims and policy on various aspects of home and foreign affairs.
+The League of Nations will remain, as heretofore, the keystone of British foreign policy. The prevention of war and the establishment of settled peace in the world must always be the most vital interest of the British people, and the League is the instrument which has been framed and to which we look for the attainment of these objects. We shall therefore continue to do all in our power to uphold the Covenant and to maintain and increase the efficiency of the League. In the present unhappy dispute between Italy and Abyssinia where will be no wavering in the policy we have hitherto pursued. We shall take no action in isolation, but we shall be prepared faithfully to take our part in any collective action decided upon by the League and shared in by its Members. We shall endeavour to further any discussion which may offer the hope of a just and fair settlement, provided that it be within the framework of the League and acceptable to the three parties to the dispute - Italy, Abyssinia and the League itself.
+Peace is not only the first interest of the British people; it is the object to which all their hopes and efforts are diverted. Our attitude to the League is dictated by the conviction that collective security by collective action can alone save us from a return to the old system which resulted in the Great War. The Covenant itself requires that national armaments should be measured both by the needs of national defence and by the duty of fulfilling international obligations. A Commonwealth which holds the positino in the world occupied by the United Kingdom and its partners in the British Empire must always take an influential part in League discussions. But our influence can be fully exerted only if we are recognised to be strong enough to fulfil any obligations which, jointly with others, we may undertake. The fact is that the actual condition of our defence forces is not satisfactory. We have made it clear that we must in the course of the next few years do what is necessary to repair the gaps in our defences, which have accumulated over the past decade, and we shall in due course present to Parliament our proposals, which will include provisions to ensure that the programme, is carried out without either waste or unreasonable profit to contractors.
+The defence programme will be strictly confined to what is required to make the country and the Empire safe, and to fulfil our obligations towards the League. All the world knows that Britain will never use her forces for any aggressive purpose. And we shall not for one moment relax our efforts to attain, by international agreement, a general limitation of armaments by every possible means, whether by restriction of numbers or by prohibition of weapons and methods of warfare. Already we have summoned a new Naval Conference to meet in London this year, at which we earnestly hope it may be possible to continue the good work done in this direction at the previous Naval Conferences of Washington and London.
+The Agreements entered into at Ottawa in 1932 marked the beginning of a new epoch in inter-imperial trading relations. The results of those Agreements have increased employment both in the Dominions and in this country, without injuring the rest of the world, and it is our intention further to promote the exchange of goods between ourselves and our partners in the Empire, believing that any increase in their prosperity will always be reflected in an increase in the volume of British trade and employment.
+The Colonial Empire also benefited greatly by the arrangements made at Ottwa. The greatest need of the British Colonies today is an extension of their markets. Special and sympathetic consideration will be given to the possibilities of providing further facilities to enable them to sell their products to the best advantage in the markets of the world and thereby increase their purchase of British goods.
+While the growing volume of British exports to the Dominions and Colonies has done something to fill the gap left by the shrinkage of international trade since 1929, it still remains true that if our foreign trade could be restored to its former dimensions an immense fillip would be given to employment in this country. It is probable that the reduction of excessive tariffs and the abolition of quotas and of other barriers to international trade will only come about by degress as general confidence is restored. There are, however, hopeful indications that opinion is moving in the right direction. In the meantime it will be our endeavour to continue the policy of reducing these barriers by means of bilateral commercial treaties, which has already had so beneficial an effect in increasing our exports to the countries with whom we have been able to make trade agreements.
+A properous countryside is an essential foundatino of national well-being. The National Government have from the first recognised that agriculture is not one but many industries, each working under different conditions and requiring different treatments for its improvement . Accordingly, they have had to make use of import duties, levies, or combinations of these devices according to the circumstances of each case. The producers have played their part by organisation and co-operation, and this we have encouraged and helped. So bold a treatment was bound to raise some problems not yet solved, but we can claim that, broadly speaking, our efforts have met with success. The prices received by farmers have recovered by 15 per cent from the low point of two years ago. The agricultural worker in England and Wales has today an average wage which is the highest recorded for ten years. At the same time the customer in the shops has been able this year to buy more food for 19s. than could be bought for £1 when the Government took office. Yet it is important for our townspeople to recognise that it is not wise to rely entirely upon foodstuffs brought from overseas. The prudent housewife wants some at least of her supplies from near at hand, where they would be readily available in any circumstances.
+It has already been announced that the Government have accepted the principle of unemployment insurance for agricultural workers, and it is our intention, if returned, to introduce legislation to that end.
+In all branches of agriculture our policy has been and will remain one of expansion of the home market. As the market expands home production can expand with it, and in this way only can a real opportunity be afforded for new men to make a career on the land.
+The Government have recognised the great importance of the fishing industry and have taken vigorous and far-reaching measures to assist the fishermen round our coasts. Here, again, our policy is to extend the market both at home and abroad. We shall not slacken in our efforts to carry this policy into effect.
+The remarkable fact that more persons are now employed in this country than ever before in its whole history has not sprung from accident or the unfettered operation of natural las. It has been the result of the deliberate policy of the Government in protecting the home market and in creating a regime of cheap money, which has facilitated enterprise and stimulated industrial expansion. In particular, cheap money, resulting from the increased confidence in Great Britain, has been the most powerful factor in bringing about the phenomenal growth of the building industry, which is the most far-reaching of all home industries in the wide field of employment which it creates. It is porbable that the improvement in the home trade, which has been so marked a feature of the past four years, has by no means reached its limit. Nevertheless, the Government are constantly working on all kinds of plans by which they make use of the present favourable circumstances to inititate new enterprises, thereby creating additional employment by use of credit or other resources of the State. The building of the Queen Mary, the subsidy to tramp shipping, the production of oil from coal by the hydrogenation process, and the great scheme of London transport improvements, at a cost of between £30 and £40 millions, are instances in point. Further schemes of a similar character are under consideration, and will, if the National Government are returned to power, be announced from time to time as they mature.
+The arrangments under the Unemployment Assistance scheme have received prolonged and anxious consideration by the Government, and, as already stated in Parliament, no alteration will be made in the existing "standstill" arrangements before next spring at the earliest. The Government regard it as important to maintain the existing powers of the Unemployment Assistance Board and the general framework of the Unemployment Assistance Act. They will, however, give effect to any recommendations by the Board for improved arrangements, where these may be shown by experience to be desirable. The "standstill" arrangements are, as they were always intended to be, temporary. They must be replaced by permanent arrangments, which must remedy certain abuses and at the same time avoid hardship to applicants. Any action must be gradual, and must be carried out in full association with local opinion, so as to give effect to reasonable differences in the localities. As regards the Means Test, the Government believe that no responsible person would seriously suggest that Unemployment Assisteance, which is not insurance benefit, ought to be paid without regard to the resources properly available to the applicant. The question is not whether there should be a Means Test, but what that test should be. This is a matter which is now under close examination, but in any scheme great importance will be attached to maintaining the unity of family life and, in addition, provision will be made to meet any cases of proved hardship.
+No branch of the Government's activities has been more constantly misrepresented that their work in the Special Areas. From the first they have recognised that in these areas - the unfortunate victimes of a contraction in the limited number of great industries on which they were formerly chiefly dependent - the problems of unemployment present features of exceptional difficulty. The removal of these difficulties and the restoration of the areas to their proper position in the normal life of the country must necessarily take time. The Government have shown their determination to grapple with the situation by the appointment of the Special Commissioners, and the granting to them of special powers to facilitate their work. As a commencement, a sum of two million pounds was placed at the Commissioners' disposal, with an intimation that more would be forthcoming as it was required. Already the commitments have considerably exceeded the initial sum, and financial considerations will not be allowed to stand in the way of any practical and reasonable scheme.
+It is generally recognised that the depression of the Special Areas has been brought about by the contraction in certain large industries, prominent among which is coal mining. Any improvement in this industry, therefore, while it would affect much larger districts than are comprised in the Special Areas, would bring particular benefits to them. The market for coal has been gradually curtailed by economy in its use, by the growth of competitive fuels and by the introduction of restrictive measures in foreign markets. There are, however, certain directions in which the industry can be made more efficient, and we hope more profitable, for the miner will always rightly command the sympathy of the public in his dangerous calling, and there is no part of the community that would not wish to see employment in the industry improved to the level of wages raised. The Government are convinced that improved selling arrangements, without which there is not the money in the industry to provide a higher rate of wages, should be put into operation and, if given the opportunity, we shall devote our energy to ensuring that measures to attain this object are adopted at an early date. We have further decided to effect the unification of coal-mining royalties, a step which will enable greater progress to be made with the organisation of production and thus improve the efficiency of the industry. Nor shall we neglect the problems of safety in coal mining. A Royal Commission will be set up to examine these subjects afresh, and to consider, not only how the present rules and regulations can best be brought up to date in the light of modern methods, but also how the latest discoveries of scientific research can help to secure the safety of those working in the pits.
+The introduction of new industries into the Special Areas is extremely desirable. As a result of the efforts which have already been made by the Special Commissioners, and of other plans which are under consideration, it is hoped to enter upon new industrial developments, including the preparation of a trading estate in which industrialists can find ready-made factories provided with all the necessary services. While every effort will be made to find the maximum amount of employment in the Special Areas, increased attention will be given to the training and transfer of such labour as cannot be provided for locally to other places where greater opportunities will be open to them. It may be observed that the new orders required for defence purposes will undoubtedly bring a considerable volume of work and employment into some parts of the country which hitherto have been most hard hit by the heavy depression, and most backward in feeling the general improvement which has been manifest elsewhere.
+On the foundations which sound financial policy has laid, new and rapid progress in Social Reform has again become possible. We have already referred to the immense development in housing. In the four years during which the Government have been in office more than 1,000,000 houses have been built. A very considerable proportion are small houses, and a substantial number which are being erected today are houses "to let". The Slum Clearance campaign is actively proceeding. Already 420,000 occupiers have been actually rehoused, and transfer to new and well-built homes is now proceeding at the unprecedented rate of over 200,000 persons a year. The first steps have already been taken to deal with the evil of overcrowding in accordance with the provisions of the Acts which have just been placed upon the Statute Book. We shall proceed vigorously with all these efforts.
+There are a number of other Social Reforms long dealyed by the necessity of first restoring the national finances, which are now ripe for action. The Contributory Pensions scheme has been a boon of inestimable value to large numbers of the people. But it has always been recognised that it was not complete so long as persons with small incomes, but not themselves insurably employed, were unable to share in its benefits. Accordingly the Government will, if returned, supplement the present scheme by arrangements which will permit other men - and women, too - whether working on their own account or not, such as shopkeepers, clerks and other black-coated workers, whose income does not exceed a certain limit, to enjoy the benefits of widows', orphans' and old age contributory pensions on a voluntary basis.
+Education must always take a foremost place in social progess, and for some time past the Government have been engaged in drawing up a comprehensive scheme of reform. Full details are being published elsewhere; here it suffices to say that it includes the raising of the school-leaving age to fifteen, with exemptions for those children who can obtain satisfactory employment. Considerable preparations, which include reorganisation of schools as well as the provision of further accommodation, will be necessary before this can be made effective. Financial adjustments will include provisions, by which building grants can be made to non-provided schools towards meeting these obligations, and also increased grants can be made to non-provided schools towards meeting these obligations, and also increased grants to Local Authorities for school buildings and conveyance of children.
+Finally, a great combined effort should now be made to raise still further the general standard of health of the Nation, especially that of the younger generation. It will require a simultaneous attack on many fronts. We must further improve our maternity services and make provision of Nursery Schools. We must meet the increasing demand, especially from our young people, for further physical exercise and training, both in the schools and after school days are over.
+We have prepared plans covering all these apects of this important subject, and when carried into effect they will go far to ensure that future generations shall bave full opportunities for the enjoyment of life that comes from the possession of a healthy mind in a healthy body.
+Scottish problems will continue to receive sympathetic attention. The programme outlined will be generally applicable to the United Kingdom, but in many spheres separate treatment is necessary to meet the special circumstances of Scotland. In particular, the further improvement of housing in the rural as well as urban areas; the needs of Scottish agriculture; the settling of families, and the finding of work for the unemployed, on the land; the provision of water supply and drainage, especially in the sparsely populated areas; and the further betterment of the fishing industry and of the Highlands and Islands will be the subject of special care and attention.
+The advent of power of the Labour Opposition, pledged to a number of revolutionary measures of which the ultimate results could not be clearly foreseen, would inevitably be followed by a collapse of confidence. The measures we have outlined above can only be carried through if the resources of the country are such as to enable it to support the necessary cost. Those resources must be derived from the income of the country, and that income can only increase if the country can rely on a period in which stability will be assured and confidence remain undisturbed.
+The international situation reinforces the same lesson. The influence of Britain among other mations, now so conspicuous, could never be maintained under an Administration drawn from a Party whose leaders of experience in foreign affairs no longer co-operate with it, and which is hopelessly divided on the most important points in foreign policy.
+In present circumstances it is more than ever necessary that the British Government should not only be united among themselves, but that they should represent that spirit of national co-operation which will best secure the confidence and respect of the world.</t>
   </si>
 </sst>
 </file>
@@ -1968,21 +2812,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D6C4B3-4694-4D7C-8241-D0EA9A7209FC}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E28" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="62.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="62.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1999,1378 +2843,1918 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B9" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B10" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" t="s">
+        <v>282</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B11" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B12" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B13" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" t="s">
+        <v>283</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>132</v>
-      </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>229</v>
       </c>
       <c r="C14" t="s">
-        <v>153</v>
+        <v>225</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>129</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>283</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>192</v>
+        <v>288</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>225</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>132</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>172</v>
+        <v>271</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>129</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>284</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>193</v>
+        <v>289</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>131</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>225</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>132</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>149</v>
+        <v>232</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>173</v>
+        <v>272</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>129</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>149</v>
+        <v>232</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>284</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>149</v>
+        <v>232</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>225</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>132</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>124</v>
+        <v>233</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>181</v>
+        <v>273</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>124</v>
+        <v>233</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>284</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>202</v>
+        <v>291</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>124</v>
+        <v>233</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>236</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>144</v>
+        <v>243</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>260</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>35</v>
+        <v>274</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>129</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>284</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>205</v>
+        <v>292</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>131</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
+        <v>237</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>146</v>
+        <v>244</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>132</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>126</v>
+        <v>235</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>156</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>184</v>
+        <v>275</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>129</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>126</v>
+        <v>235</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>284</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>131</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>126</v>
+        <v>235</v>
       </c>
       <c r="C31" t="s">
-        <v>142</v>
+        <v>237</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>132</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>129</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>131</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>119</v>
+        <v>210</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>132</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>156</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>129</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>37</v>
+        <v>189</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>131</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>132</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>38</v>
+        <v>169</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>39</v>
+        <v>190</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>131</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>120</v>
+        <v>212</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>132</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>129</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>131</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>121</v>
+        <v>213</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B47" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="B48" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C48" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B49" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>132</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B50" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="B51" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>12</v>
-      </c>
       <c r="B52" s="3" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>48</v>
+        <v>216</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>132</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C53" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>129</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>52</v>
+        <v>202</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>131</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>132</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C58" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="B59" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>129</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" t="s">
-        <v>57</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="B60" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>131</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C60" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>12</v>
-      </c>
       <c r="B61" s="3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C61" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>150</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>88</v>
+        <v>182</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C64" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B66" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" t="s">
-        <v>55</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>15</v>
-      </c>
       <c r="B67" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>132</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>129</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C69" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>131</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" t="s">
+        <v>115</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>131</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>132</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C82" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>132</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s">
+        <v>51</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" t="s">
+        <v>83</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>132</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>131</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C90" t="s">
+        <v>55</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C92" t="s">
+        <v>87</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>132</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C94" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>131</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C95" t="s">
+        <v>55</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C96" t="s">
+        <v>63</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>15</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C97" t="s">
+        <v>65</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>132</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C98" t="s">
+        <v>67</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C99" t="s">
+        <v>71</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>131</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C100" t="s">
         <v>69</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C101" t="s">
         <v>63</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C102" t="s">
         <v>74</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>132</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C103" t="s">
         <v>67</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>129</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C104" t="s">
         <v>77</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>131</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C105" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>12</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C106" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>130</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C107" t="s">
         <v>65</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D26" r:id="rId1" xr:uid="{D7371718-58B6-44A1-B12B-1BCAA4964B42}"/>
-    <hyperlink ref="D35" r:id="rId2" xr:uid="{29613CAF-2038-4D33-999A-49CC0C5EBEA1}"/>
-    <hyperlink ref="D36" r:id="rId3" xr:uid="{82003BC9-261C-498E-A7A0-5A316A101FA0}"/>
-    <hyperlink ref="D38" r:id="rId4" xr:uid="{86BA4AB3-91DE-4965-8A52-5C7915BF2288}"/>
-    <hyperlink ref="D39" r:id="rId5" xr:uid="{5BF064B8-4788-444B-852E-B0F85BF9F61F}"/>
-    <hyperlink ref="D41" r:id="rId6" xr:uid="{CAD11900-4F62-49AA-897C-CBDADF5AE6BB}"/>
-    <hyperlink ref="D42" r:id="rId7" xr:uid="{7815F4BA-E0C6-4D59-93A4-6C3C546AE73B}"/>
-    <hyperlink ref="D44" r:id="rId8" xr:uid="{6A8BFAE7-F4C3-4962-BACD-18EC0517CE75}"/>
-    <hyperlink ref="D45" r:id="rId9" xr:uid="{E62BFF6B-2EA8-4D63-92E4-9C439375677F}"/>
-    <hyperlink ref="D47" r:id="rId10" xr:uid="{D68A4F37-6F6F-49A2-9DB1-7F9CFEB0E36E}"/>
-    <hyperlink ref="D48" r:id="rId11" xr:uid="{F80DFD9A-574E-4CB4-A487-9B96169AD3DD}"/>
-    <hyperlink ref="D49" r:id="rId12" xr:uid="{DBB52C04-7E52-4463-94BC-455822B92727}"/>
-    <hyperlink ref="D50" r:id="rId13" xr:uid="{9C390DB6-3210-49EC-B23E-0539EB002217}"/>
-    <hyperlink ref="D51" r:id="rId14" xr:uid="{D4F6D3AD-651D-4864-B3AF-EDABDDF98652}"/>
-    <hyperlink ref="D52" r:id="rId15" xr:uid="{501D7B83-5D4B-4647-A5A7-6FC823F7EE00}"/>
-    <hyperlink ref="D53" r:id="rId16" xr:uid="{2C05A670-2A5A-469B-BF8E-E5667A1D24DF}"/>
-    <hyperlink ref="D55" r:id="rId17" xr:uid="{9A4FB7A9-6B5E-4D25-BEE5-D6B1DCBE8646}"/>
-    <hyperlink ref="D54" r:id="rId18" xr:uid="{DA8B88A4-3CA8-44D2-A01A-C085094FD401}"/>
-    <hyperlink ref="D58" r:id="rId19" xr:uid="{8C7F8365-5BCF-47D2-BA54-012A4111D58F}"/>
-    <hyperlink ref="D60" r:id="rId20" xr:uid="{66A90D95-889E-4EEC-A486-278CE83ABCD1}"/>
-    <hyperlink ref="D59" r:id="rId21" xr:uid="{B7DBD44E-CB6B-42EE-96BC-D4676A8C8D5F}"/>
-    <hyperlink ref="D63" r:id="rId22" xr:uid="{75B1BB56-2757-415D-94A2-816A8DFBBBD6}"/>
-    <hyperlink ref="D65" r:id="rId23" xr:uid="{79AA7B72-6791-4FA5-AAB8-0EFFAD1FA2CA}"/>
-    <hyperlink ref="D64" r:id="rId24" xr:uid="{A03EDA82-3A2E-4B03-89D3-C3D5CE2D7582}"/>
-    <hyperlink ref="D66" r:id="rId25" xr:uid="{4BC1A719-F7FF-426D-8C51-6F4708899C76}"/>
-    <hyperlink ref="D67" r:id="rId26" xr:uid="{9E76004A-CC93-42C9-B93A-CFB844B12859}"/>
-    <hyperlink ref="D68" r:id="rId27" xr:uid="{D7F16FB4-1888-4303-B2D3-BFD3FF131743}"/>
-    <hyperlink ref="D70" r:id="rId28" xr:uid="{B38BCD6E-D43B-407E-BDA6-8082CD44215B}"/>
-    <hyperlink ref="D69" r:id="rId29" xr:uid="{C9A71007-38B7-4B17-88DC-CFBD806BFB6E}"/>
-    <hyperlink ref="D71" r:id="rId30" xr:uid="{592C30BE-BA5D-493F-BFC0-118C3EAA15A6}"/>
-    <hyperlink ref="D72" r:id="rId31" xr:uid="{AE34F1D4-1906-479F-A55B-827199F1ADDA}"/>
-    <hyperlink ref="D73" r:id="rId32" xr:uid="{49CE0AD2-5EB2-44CE-A43F-26E05E7CE28A}"/>
-    <hyperlink ref="D74" r:id="rId33" xr:uid="{75640ADC-21AA-4D0C-8639-AA4E5B345998}"/>
-    <hyperlink ref="D75" r:id="rId34" xr:uid="{137F227D-7821-4183-B122-92EF8BAC7DFE}"/>
-    <hyperlink ref="D76" r:id="rId35" xr:uid="{05E1DA35-0899-474D-8533-6CF1F1556381}"/>
-    <hyperlink ref="D46" r:id="rId36" xr:uid="{36843EB4-D203-4905-9CBA-08E0CF7E7DFB}"/>
-    <hyperlink ref="D57" r:id="rId37" xr:uid="{E54BFA64-F35A-402E-AE35-D2D6E81485EA}"/>
-    <hyperlink ref="D56" r:id="rId38" xr:uid="{A2E9EFAD-FEB5-4964-97B5-A05A27DAD294}"/>
-    <hyperlink ref="D61" r:id="rId39" xr:uid="{2076C4C5-164A-43EA-8EDC-FBE2AE2287A1}"/>
-    <hyperlink ref="D62" r:id="rId40" xr:uid="{BADCAE52-CBAA-4307-B7B2-7C3961A92C9D}"/>
-    <hyperlink ref="D77" r:id="rId41" xr:uid="{5448D857-AD73-4762-9F4B-B55411AAD96F}"/>
-    <hyperlink ref="D37" r:id="rId42" xr:uid="{858B6E84-29F7-429E-AE95-25B7AD93E5C0}"/>
-    <hyperlink ref="D34" r:id="rId43" xr:uid="{FD3E3B4C-29F6-4D8B-A1AF-D186679148B8}"/>
-    <hyperlink ref="D40" r:id="rId44" xr:uid="{089089D2-B642-4566-B78E-B4DD9735D31B}"/>
-    <hyperlink ref="D43" r:id="rId45" xr:uid="{024C1334-D7CE-4286-AA92-8288553A807E}"/>
-    <hyperlink ref="D25" r:id="rId46" xr:uid="{ED613AAC-A737-402A-A7AE-86BC0DF101E0}"/>
-    <hyperlink ref="D28" r:id="rId47" xr:uid="{B3DC5D65-F951-4D80-AFA7-F84B7CB7EB7D}"/>
-    <hyperlink ref="D31" r:id="rId48" xr:uid="{DB9CBA10-86A7-4664-9FBA-51B23AA846DD}"/>
-    <hyperlink ref="D2" r:id="rId49" xr:uid="{9FDBF89D-D0E0-435A-843C-9E4F8088BEDE}"/>
-    <hyperlink ref="D5" r:id="rId50" xr:uid="{1B825FEC-378E-4719-BB83-5C5EC859A9F0}"/>
-    <hyperlink ref="D8" r:id="rId51" xr:uid="{E96C1A10-B9D2-4BE2-BB30-AFED637D77A5}"/>
-    <hyperlink ref="D11" r:id="rId52" xr:uid="{CAFB0F4A-C9D9-4887-9328-D8B7AA42086F}"/>
-    <hyperlink ref="D14" r:id="rId53" xr:uid="{59264C40-5848-4257-861C-5EB690848749}"/>
-    <hyperlink ref="D17" r:id="rId54" xr:uid="{DE13670C-FACA-4694-AA2A-3FB3FA7EC2BD}"/>
-    <hyperlink ref="D20" r:id="rId55" xr:uid="{22D87374-DFA4-4CC3-B4CB-A37089FACC43}"/>
-    <hyperlink ref="D23" r:id="rId56" xr:uid="{44EF5743-9AF1-447B-A028-563DA71EB2EE}"/>
-    <hyperlink ref="D29" r:id="rId57" xr:uid="{4E6365BD-CB9F-4764-A3A4-4C077B22D98A}"/>
-    <hyperlink ref="D32" r:id="rId58" xr:uid="{B6BC084B-93B7-4D62-97C2-2A7302161267}"/>
-    <hyperlink ref="D3" r:id="rId59" xr:uid="{735A807E-A069-47B2-ACBD-88A8382DC7C0}"/>
-    <hyperlink ref="D6" r:id="rId60" xr:uid="{2F8727A1-BB8A-4818-9903-593953DAC4D7}"/>
-    <hyperlink ref="D9" r:id="rId61" xr:uid="{F83C40E1-D412-443D-8F1E-8B2E58973B42}"/>
-    <hyperlink ref="D12" r:id="rId62" xr:uid="{32D171CB-2A22-4AF6-9304-2BE62606820C}"/>
-    <hyperlink ref="D15" r:id="rId63" xr:uid="{EC562266-9033-4350-912C-2964574CC1AD}"/>
-    <hyperlink ref="D18" r:id="rId64" xr:uid="{709542EC-4CE9-4A7C-AF90-735102CFAC68}"/>
-    <hyperlink ref="D21" r:id="rId65" xr:uid="{10F4B09A-7449-4289-B264-B7F399EAA683}"/>
-    <hyperlink ref="D24" r:id="rId66" xr:uid="{B9D519DC-A441-4DC3-BE20-95799F858DAC}"/>
-    <hyperlink ref="D27" r:id="rId67" xr:uid="{FB5B66B5-8CE2-4A1A-9EFA-090190206CE6}"/>
-    <hyperlink ref="D30" r:id="rId68" xr:uid="{990C6BDB-84F6-4ED5-91E0-C6BDCE50EC19}"/>
-    <hyperlink ref="D33" r:id="rId69" xr:uid="{EB13DC78-CD4E-40D9-AF42-F03708587C2C}"/>
-    <hyperlink ref="D4" r:id="rId70" xr:uid="{B78B4CF4-2838-4592-A00A-884D53D76D35}"/>
-    <hyperlink ref="D7" r:id="rId71" xr:uid="{08355141-B1B5-43F1-8BE2-411A86D96BEF}"/>
-    <hyperlink ref="D10" r:id="rId72" xr:uid="{8FCF0E72-4E67-425E-8DB0-B65A50895DC8}"/>
-    <hyperlink ref="D13" r:id="rId73" xr:uid="{72F650FC-8EB0-48AB-A40F-C03F4A5B8A8D}"/>
-    <hyperlink ref="D16" r:id="rId74" xr:uid="{4A3F7F64-64BD-4AEF-9A5D-385A80847A7F}"/>
-    <hyperlink ref="D19" r:id="rId75" xr:uid="{76D08BD9-6ACB-465C-95C8-AC7BC74FA433}"/>
-    <hyperlink ref="D22" r:id="rId76" xr:uid="{B2F277A7-CC8B-42DE-9BAB-B973904EB620}"/>
+    <hyperlink ref="D56" r:id="rId1" xr:uid="{D7371718-58B6-44A1-B12B-1BCAA4964B42}"/>
+    <hyperlink ref="D65" r:id="rId2" xr:uid="{29613CAF-2038-4D33-999A-49CC0C5EBEA1}"/>
+    <hyperlink ref="D66" r:id="rId3" xr:uid="{82003BC9-261C-498E-A7A0-5A316A101FA0}"/>
+    <hyperlink ref="D68" r:id="rId4" xr:uid="{86BA4AB3-91DE-4965-8A52-5C7915BF2288}"/>
+    <hyperlink ref="D69" r:id="rId5" xr:uid="{5BF064B8-4788-444B-852E-B0F85BF9F61F}"/>
+    <hyperlink ref="D71" r:id="rId6" xr:uid="{CAD11900-4F62-49AA-897C-CBDADF5AE6BB}"/>
+    <hyperlink ref="D72" r:id="rId7" xr:uid="{7815F4BA-E0C6-4D59-93A4-6C3C546AE73B}"/>
+    <hyperlink ref="D74" r:id="rId8" xr:uid="{6A8BFAE7-F4C3-4962-BACD-18EC0517CE75}"/>
+    <hyperlink ref="D75" r:id="rId9" xr:uid="{E62BFF6B-2EA8-4D63-92E4-9C439375677F}"/>
+    <hyperlink ref="D77" r:id="rId10" xr:uid="{D68A4F37-6F6F-49A2-9DB1-7F9CFEB0E36E}"/>
+    <hyperlink ref="D78" r:id="rId11" xr:uid="{F80DFD9A-574E-4CB4-A487-9B96169AD3DD}"/>
+    <hyperlink ref="D79" r:id="rId12" xr:uid="{DBB52C04-7E52-4463-94BC-455822B92727}"/>
+    <hyperlink ref="D80" r:id="rId13" xr:uid="{9C390DB6-3210-49EC-B23E-0539EB002217}"/>
+    <hyperlink ref="D81" r:id="rId14" xr:uid="{D4F6D3AD-651D-4864-B3AF-EDABDDF98652}"/>
+    <hyperlink ref="D82" r:id="rId15" xr:uid="{501D7B83-5D4B-4647-A5A7-6FC823F7EE00}"/>
+    <hyperlink ref="D83" r:id="rId16" xr:uid="{2C05A670-2A5A-469B-BF8E-E5667A1D24DF}"/>
+    <hyperlink ref="D85" r:id="rId17" xr:uid="{9A4FB7A9-6B5E-4D25-BEE5-D6B1DCBE8646}"/>
+    <hyperlink ref="D84" r:id="rId18" xr:uid="{DA8B88A4-3CA8-44D2-A01A-C085094FD401}"/>
+    <hyperlink ref="D88" r:id="rId19" xr:uid="{8C7F8365-5BCF-47D2-BA54-012A4111D58F}"/>
+    <hyperlink ref="D90" r:id="rId20" xr:uid="{66A90D95-889E-4EEC-A486-278CE83ABCD1}"/>
+    <hyperlink ref="D89" r:id="rId21" xr:uid="{B7DBD44E-CB6B-42EE-96BC-D4676A8C8D5F}"/>
+    <hyperlink ref="D93" r:id="rId22" xr:uid="{75B1BB56-2757-415D-94A2-816A8DFBBBD6}"/>
+    <hyperlink ref="D95" r:id="rId23" xr:uid="{79AA7B72-6791-4FA5-AAB8-0EFFAD1FA2CA}"/>
+    <hyperlink ref="D94" r:id="rId24" xr:uid="{A03EDA82-3A2E-4B03-89D3-C3D5CE2D7582}"/>
+    <hyperlink ref="D96" r:id="rId25" xr:uid="{4BC1A719-F7FF-426D-8C51-6F4708899C76}"/>
+    <hyperlink ref="D97" r:id="rId26" xr:uid="{9E76004A-CC93-42C9-B93A-CFB844B12859}"/>
+    <hyperlink ref="D98" r:id="rId27" xr:uid="{D7F16FB4-1888-4303-B2D3-BFD3FF131743}"/>
+    <hyperlink ref="D100" r:id="rId28" xr:uid="{B38BCD6E-D43B-407E-BDA6-8082CD44215B}"/>
+    <hyperlink ref="D99" r:id="rId29" xr:uid="{C9A71007-38B7-4B17-88DC-CFBD806BFB6E}"/>
+    <hyperlink ref="D101" r:id="rId30" xr:uid="{592C30BE-BA5D-493F-BFC0-118C3EAA15A6}"/>
+    <hyperlink ref="D102" r:id="rId31" xr:uid="{AE34F1D4-1906-479F-A55B-827199F1ADDA}"/>
+    <hyperlink ref="D103" r:id="rId32" xr:uid="{49CE0AD2-5EB2-44CE-A43F-26E05E7CE28A}"/>
+    <hyperlink ref="D104" r:id="rId33" xr:uid="{75640ADC-21AA-4D0C-8639-AA4E5B345998}"/>
+    <hyperlink ref="D105" r:id="rId34" xr:uid="{137F227D-7821-4183-B122-92EF8BAC7DFE}"/>
+    <hyperlink ref="D106" r:id="rId35" xr:uid="{05E1DA35-0899-474D-8533-6CF1F1556381}"/>
+    <hyperlink ref="D76" r:id="rId36" xr:uid="{36843EB4-D203-4905-9CBA-08E0CF7E7DFB}"/>
+    <hyperlink ref="D87" r:id="rId37" xr:uid="{E54BFA64-F35A-402E-AE35-D2D6E81485EA}"/>
+    <hyperlink ref="D86" r:id="rId38" xr:uid="{A2E9EFAD-FEB5-4964-97B5-A05A27DAD294}"/>
+    <hyperlink ref="D91" r:id="rId39" xr:uid="{2076C4C5-164A-43EA-8EDC-FBE2AE2287A1}"/>
+    <hyperlink ref="D92" r:id="rId40" xr:uid="{BADCAE52-CBAA-4307-B7B2-7C3961A92C9D}"/>
+    <hyperlink ref="D107" r:id="rId41" xr:uid="{5448D857-AD73-4762-9F4B-B55411AAD96F}"/>
+    <hyperlink ref="D67" r:id="rId42" xr:uid="{858B6E84-29F7-429E-AE95-25B7AD93E5C0}"/>
+    <hyperlink ref="D64" r:id="rId43" xr:uid="{FD3E3B4C-29F6-4D8B-A1AF-D186679148B8}"/>
+    <hyperlink ref="D70" r:id="rId44" xr:uid="{089089D2-B642-4566-B78E-B4DD9735D31B}"/>
+    <hyperlink ref="D73" r:id="rId45" xr:uid="{024C1334-D7CE-4286-AA92-8288553A807E}"/>
+    <hyperlink ref="D55" r:id="rId46" xr:uid="{ED613AAC-A737-402A-A7AE-86BC0DF101E0}"/>
+    <hyperlink ref="D58" r:id="rId47" xr:uid="{B3DC5D65-F951-4D80-AFA7-F84B7CB7EB7D}"/>
+    <hyperlink ref="D61" r:id="rId48" xr:uid="{DB9CBA10-86A7-4664-9FBA-51B23AA846DD}"/>
+    <hyperlink ref="D32" r:id="rId49" xr:uid="{9FDBF89D-D0E0-435A-843C-9E4F8088BEDE}"/>
+    <hyperlink ref="D35" r:id="rId50" xr:uid="{1B825FEC-378E-4719-BB83-5C5EC859A9F0}"/>
+    <hyperlink ref="D38" r:id="rId51" xr:uid="{E96C1A10-B9D2-4BE2-BB30-AFED637D77A5}"/>
+    <hyperlink ref="D41" r:id="rId52" xr:uid="{CAFB0F4A-C9D9-4887-9328-D8B7AA42086F}"/>
+    <hyperlink ref="D44" r:id="rId53" xr:uid="{59264C40-5848-4257-861C-5EB690848749}"/>
+    <hyperlink ref="D47" r:id="rId54" xr:uid="{DE13670C-FACA-4694-AA2A-3FB3FA7EC2BD}"/>
+    <hyperlink ref="D50" r:id="rId55" xr:uid="{22D87374-DFA4-4CC3-B4CB-A37089FACC43}"/>
+    <hyperlink ref="D53" r:id="rId56" xr:uid="{44EF5743-9AF1-447B-A028-563DA71EB2EE}"/>
+    <hyperlink ref="D59" r:id="rId57" xr:uid="{4E6365BD-CB9F-4764-A3A4-4C077B22D98A}"/>
+    <hyperlink ref="D62" r:id="rId58" xr:uid="{B6BC084B-93B7-4D62-97C2-2A7302161267}"/>
+    <hyperlink ref="D33" r:id="rId59" xr:uid="{735A807E-A069-47B2-ACBD-88A8382DC7C0}"/>
+    <hyperlink ref="D36" r:id="rId60" xr:uid="{2F8727A1-BB8A-4818-9903-593953DAC4D7}"/>
+    <hyperlink ref="D39" r:id="rId61" xr:uid="{F83C40E1-D412-443D-8F1E-8B2E58973B42}"/>
+    <hyperlink ref="D42" r:id="rId62" xr:uid="{32D171CB-2A22-4AF6-9304-2BE62606820C}"/>
+    <hyperlink ref="D45" r:id="rId63" xr:uid="{EC562266-9033-4350-912C-2964574CC1AD}"/>
+    <hyperlink ref="D48" r:id="rId64" xr:uid="{709542EC-4CE9-4A7C-AF90-735102CFAC68}"/>
+    <hyperlink ref="D51" r:id="rId65" xr:uid="{10F4B09A-7449-4289-B264-B7F399EAA683}"/>
+    <hyperlink ref="D54" r:id="rId66" xr:uid="{B9D519DC-A441-4DC3-BE20-95799F858DAC}"/>
+    <hyperlink ref="D57" r:id="rId67" xr:uid="{FB5B66B5-8CE2-4A1A-9EFA-090190206CE6}"/>
+    <hyperlink ref="D60" r:id="rId68" xr:uid="{990C6BDB-84F6-4ED5-91E0-C6BDCE50EC19}"/>
+    <hyperlink ref="D63" r:id="rId69" xr:uid="{EB13DC78-CD4E-40D9-AF42-F03708587C2C}"/>
+    <hyperlink ref="D34" r:id="rId70" xr:uid="{B78B4CF4-2838-4592-A00A-884D53D76D35}"/>
+    <hyperlink ref="D37" r:id="rId71" xr:uid="{08355141-B1B5-43F1-8BE2-411A86D96BEF}"/>
+    <hyperlink ref="D40" r:id="rId72" xr:uid="{8FCF0E72-4E67-425E-8DB0-B65A50895DC8}"/>
+    <hyperlink ref="D43" r:id="rId73" xr:uid="{72F650FC-8EB0-48AB-A40F-C03F4A5B8A8D}"/>
+    <hyperlink ref="D46" r:id="rId74" xr:uid="{4A3F7F64-64BD-4AEF-9A5D-385A80847A7F}"/>
+    <hyperlink ref="D49" r:id="rId75" xr:uid="{76D08BD9-6ACB-465C-95C8-AC7BC74FA433}"/>
+    <hyperlink ref="D52" r:id="rId76" xr:uid="{B2F277A7-CC8B-42DE-9BAB-B973904EB620}"/>
+    <hyperlink ref="D3" r:id="rId77" xr:uid="{118747A5-A443-4111-B6FB-1E02912590F3}"/>
+    <hyperlink ref="D8" r:id="rId78" xr:uid="{D51726A3-DFAF-4388-B9CF-78823DCB320C}"/>
+    <hyperlink ref="D11" r:id="rId79" xr:uid="{BA63D756-9C0B-40EA-B0DB-3115FE6CA807}"/>
+    <hyperlink ref="D14" r:id="rId80" xr:uid="{24F57854-9CA9-4AA5-A36B-3D733F0A4B4C}"/>
+    <hyperlink ref="D16" r:id="rId81" xr:uid="{C8A0338F-93A3-49F4-B1F7-105E66778EDD}"/>
+    <hyperlink ref="D19" r:id="rId82" xr:uid="{F08669FC-046D-4FC9-92DB-54E2ECB1ABCD}"/>
+    <hyperlink ref="D22" r:id="rId83" xr:uid="{1A73DBA9-7E25-4D7B-87F9-737FCD46AF74}"/>
+    <hyperlink ref="D25" r:id="rId84" xr:uid="{F427ECAB-5CF9-4DA9-B414-BB853626D0AF}"/>
+    <hyperlink ref="D28" r:id="rId85" xr:uid="{24C049FB-DD7C-4F0D-B240-6816F9FD4BAC}"/>
+    <hyperlink ref="D31" r:id="rId86" xr:uid="{6662865C-380B-4AB1-9260-A1336D490881}"/>
+    <hyperlink ref="D4" r:id="rId87" xr:uid="{285FC0F6-0A30-4CD0-8501-7ACCFC133CA7}"/>
+    <hyperlink ref="D12" r:id="rId88" xr:uid="{5074C14C-2076-4A21-A5C9-88F484A31D46}"/>
+    <hyperlink ref="D6" r:id="rId89" xr:uid="{77926429-C823-4AED-9CE7-32AC7D24EFE8}"/>
+    <hyperlink ref="D9" r:id="rId90" xr:uid="{C349B6D5-CBDF-4ADB-B223-859C06729B17}"/>
+    <hyperlink ref="D17" r:id="rId91" xr:uid="{937CE1BD-43D5-4228-A4B8-4B460B32B0F2}"/>
+    <hyperlink ref="D20" r:id="rId92" xr:uid="{81EB0156-2FA3-4EA2-8272-0D954A226FE8}"/>
+    <hyperlink ref="D23" r:id="rId93" xr:uid="{3714C995-03DC-4EC6-8C61-48E1882270E9}"/>
+    <hyperlink ref="D26" r:id="rId94" xr:uid="{C9E05E41-F76E-44DA-8BD5-4ABEB99B6D26}"/>
+    <hyperlink ref="D29" r:id="rId95" xr:uid="{A5D2D02F-429E-49D0-9394-7A98392DFA68}"/>
+    <hyperlink ref="D2" r:id="rId96" xr:uid="{4B10B1BC-A542-4880-BF03-CC7B968AB975}"/>
+    <hyperlink ref="D5" r:id="rId97" xr:uid="{9829FC15-377B-4351-8D1E-3645A8099953}"/>
+    <hyperlink ref="D7" r:id="rId98" xr:uid="{384D41CD-49DD-453A-B709-E271AA25277C}"/>
+    <hyperlink ref="D10" r:id="rId99" xr:uid="{CCA2D330-77BD-4006-8C22-31284BBDD542}"/>
+    <hyperlink ref="D13" r:id="rId100" xr:uid="{A3B55F07-891B-4F55-B64F-CD8E9001AB86}"/>
+    <hyperlink ref="D15" r:id="rId101" xr:uid="{7239FF59-7F67-4CA3-A4A5-8BE03F9DAD72}"/>
+    <hyperlink ref="D18" r:id="rId102" xr:uid="{9E3E56AB-302B-4C7A-B922-601E25E87BAB}"/>
+    <hyperlink ref="D21" r:id="rId103" xr:uid="{F77ECE8C-309C-4857-94D8-99C09EB0B27A}"/>
+    <hyperlink ref="D24" r:id="rId104" xr:uid="{920AB4B7-DCE5-40DA-A550-8EA65DCC58B0}"/>
+    <hyperlink ref="D27" r:id="rId105" xr:uid="{03E96B5B-0E95-44D4-A254-70F0471E8E83}"/>
+    <hyperlink ref="D30" r:id="rId106" xr:uid="{7BB5ECE2-8196-4CB3-B982-81DECB47898C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId107"/>
 </worksheet>
 </file>
</xml_diff>